<commit_message>
Korrektur Lukas, 2xM Hose weiblich
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -1519,48 +1519,6 @@
   </cellStyleXfs>
   <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2011,10 +1969,52 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="74" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2608,32 +2608,32 @@
   <dimension ref="A1:IW69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="15"/>
-    <col min="2" max="2" width="10.42578125" style="15"/>
-    <col min="3" max="3" width="13.140625" style="15"/>
-    <col min="4" max="4" width="7.42578125" style="16"/>
-    <col min="5" max="5" width="11" style="17"/>
-    <col min="6" max="11" width="6.5703125" style="15"/>
-    <col min="12" max="13" width="10.42578125" style="15"/>
-    <col min="14" max="14" width="10.5703125" style="18"/>
-    <col min="15" max="257" width="10.42578125" style="15"/>
+    <col min="1" max="1" width="12.28515625" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1"/>
+    <col min="3" max="3" width="13.140625" style="1"/>
+    <col min="4" max="4" width="7.42578125" style="2"/>
+    <col min="5" max="5" width="11" style="3"/>
+    <col min="6" max="11" width="6.5703125" style="1"/>
+    <col min="12" max="13" width="10.42578125" style="1"/>
+    <col min="14" max="14" width="10.5703125" style="4"/>
+    <col min="15" max="257" width="10.42578125" style="1"/>
     <col min="258" max="1025" width="8.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
@@ -2651,10 +2651,10 @@
       <c r="R2"/>
     </row>
     <row r="3" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C3"/>
@@ -2674,10 +2674,10 @@
       <c r="R3"/>
     </row>
     <row r="4" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="10">
         <f ca="1">TODAY()</f>
         <v>42682</v>
       </c>
@@ -2736,1571 +2736,1569 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="13" t="s">
+      <c r="B7" s="164"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
+      <c r="F7" s="165" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13" t="s">
+      <c r="G7" s="165"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="165"/>
+      <c r="K7" s="165"/>
+      <c r="L7" s="165" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="N7" s="165"/>
+      <c r="O7" s="165"/>
       <c r="Q7"/>
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="31" t="s">
+      <c r="O8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="Q8"/>
       <c r="R8"/>
     </row>
     <row r="9" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="167" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="168" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="20">
         <v>14</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="21">
         <f t="shared" ref="F9:F40" si="0">E9-G9-H9-I9-J9-K9</f>
         <v>11</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33">
+      <c r="G9" s="19"/>
+      <c r="H9" s="19">
         <v>2</v>
       </c>
-      <c r="I9" s="33">
-        <v>1</v>
-      </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="38">
+      <c r="I9" s="19">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="24">
         <f>49.18-(49.18*10/100)</f>
         <v>44.262</v>
       </c>
-      <c r="O9" s="39"/>
-      <c r="Q9" s="40"/>
+      <c r="O9" s="25"/>
+      <c r="Q9" s="26"/>
       <c r="R9"/>
     </row>
     <row r="10" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="41" t="s">
+      <c r="A10" s="166"/>
+      <c r="B10" s="167"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="28">
         <v>18</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41">
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27">
         <v>3</v>
       </c>
-      <c r="K10" s="44"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="47"/>
-      <c r="Q10" s="40"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="33"/>
+      <c r="Q10" s="26"/>
       <c r="R10"/>
     </row>
     <row r="11" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="33" t="s">
+      <c r="A11" s="166"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="20">
         <v>20</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="29">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="39"/>
-      <c r="Q11" s="40"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="25"/>
+      <c r="Q11" s="26"/>
       <c r="R11"/>
     </row>
     <row r="12" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="48" t="s">
+      <c r="A12" s="166"/>
+      <c r="B12" s="167"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E12" s="35">
         <v>7</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="36">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="51">
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="37">
         <v>2</v>
       </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
-      <c r="Q12" s="40"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="40"/>
+      <c r="Q12" s="26"/>
       <c r="R12"/>
     </row>
     <row r="13" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="9" t="s">
+      <c r="A13" s="166"/>
+      <c r="B13" s="167"/>
+      <c r="C13" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="42">
         <v>4</v>
       </c>
-      <c r="F13" s="57">
+      <c r="F13" s="43">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55">
-        <v>1</v>
-      </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="60">
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41">
+        <v>1</v>
+      </c>
+      <c r="J13" s="41"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="46">
         <f>56.01-(56.01*10/100)</f>
         <v>50.408999999999999</v>
       </c>
-      <c r="O13" s="61"/>
-      <c r="Q13" s="40"/>
+      <c r="O13" s="47"/>
+      <c r="Q13" s="26"/>
       <c r="R13"/>
     </row>
     <row r="14" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="62" t="s">
+      <c r="A14" s="166"/>
+      <c r="B14" s="167"/>
+      <c r="C14" s="159"/>
+      <c r="D14" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="63">
+      <c r="E14" s="49">
         <v>4</v>
       </c>
-      <c r="F14" s="64">
+      <c r="F14" s="50">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62">
-        <v>1</v>
-      </c>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62">
-        <v>1</v>
-      </c>
-      <c r="K14" s="65"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="68"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48">
+        <v>1</v>
+      </c>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48">
+        <v>1</v>
+      </c>
+      <c r="K14" s="51"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="54"/>
       <c r="R14"/>
     </row>
     <row r="15" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="69" t="s">
+      <c r="A15" s="166"/>
+      <c r="B15" s="167"/>
+      <c r="C15" s="159"/>
+      <c r="D15" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="70">
+      <c r="E15" s="56">
         <v>0</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="75"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="61"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="76" t="s">
+      <c r="A16" s="166"/>
+      <c r="B16" s="167"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="77">
+      <c r="E16" s="63">
         <v>2</v>
       </c>
-      <c r="F16" s="78">
+      <c r="F16" s="64">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="79">
-        <v>1</v>
-      </c>
-      <c r="L16" s="80"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="82"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="65">
+        <v>1</v>
+      </c>
+      <c r="L16" s="66"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="68"/>
       <c r="R16"/>
     </row>
     <row r="17" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="8" t="s">
+      <c r="A17" s="166"/>
+      <c r="B17" s="167"/>
+      <c r="C17" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="83">
+      <c r="E17" s="69">
         <v>7</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33">
-        <v>1</v>
-      </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="38">
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19">
+        <v>1</v>
+      </c>
+      <c r="J17" s="19"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="24">
         <f>50.08-(50.08*10/100)</f>
         <v>45.072000000000003</v>
       </c>
-      <c r="O17" s="39"/>
+      <c r="O17" s="25"/>
       <c r="R17"/>
     </row>
     <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="84" t="s">
+      <c r="A18" s="166"/>
+      <c r="B18" s="167"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="85">
+      <c r="E18" s="71">
         <v>13</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84">
+      <c r="G18" s="70"/>
+      <c r="H18" s="70">
         <v>2</v>
       </c>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="84"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="89"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="70"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="75"/>
       <c r="R18"/>
     </row>
     <row r="19" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="90" t="s">
+      <c r="A19" s="166"/>
+      <c r="B19" s="167"/>
+      <c r="C19" s="160"/>
+      <c r="D19" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="91">
+      <c r="E19" s="77">
         <v>10</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="90">
-        <v>1</v>
-      </c>
-      <c r="K19" s="92"/>
-      <c r="L19" s="93"/>
-      <c r="M19" s="90"/>
-      <c r="N19" s="94"/>
-      <c r="O19" s="95"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76">
+        <v>1</v>
+      </c>
+      <c r="K19" s="78"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="81"/>
       <c r="R19"/>
     </row>
     <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="96" t="s">
+      <c r="A20" s="166"/>
+      <c r="B20" s="167"/>
+      <c r="C20" s="160"/>
+      <c r="D20" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="97">
+      <c r="E20" s="83">
         <v>9</v>
       </c>
-      <c r="F20" s="98">
+      <c r="F20" s="84">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G20" s="96"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="96">
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82">
         <v>2</v>
       </c>
-      <c r="K20" s="99">
+      <c r="K20" s="85">
         <v>2</v>
       </c>
-      <c r="L20" s="100"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="101"/>
-      <c r="O20" s="102"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="88"/>
       <c r="R20"/>
     </row>
     <row r="21" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="166"/>
+      <c r="B21" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="162" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="103" t="s">
+      <c r="D21" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="104">
+      <c r="E21" s="90">
         <v>5</v>
       </c>
-      <c r="F21" s="105">
+      <c r="F21" s="91">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G21" s="103">
+      <c r="G21" s="89">
         <v>2</v>
       </c>
-      <c r="H21" s="103"/>
-      <c r="I21" s="103"/>
-      <c r="J21" s="103"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="103"/>
-      <c r="N21" s="108">
+      <c r="H21" s="89"/>
+      <c r="I21" s="89"/>
+      <c r="J21" s="89"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="89"/>
+      <c r="N21" s="94">
         <f>48.02-(48.02*10/100)</f>
         <v>43.218000000000004</v>
       </c>
-      <c r="O21" s="109"/>
+      <c r="O21" s="95"/>
       <c r="R21"/>
     </row>
     <row r="22" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="110" t="s">
+      <c r="A22" s="166"/>
+      <c r="B22" s="161"/>
+      <c r="C22" s="162"/>
+      <c r="D22" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="111">
+      <c r="E22" s="97">
         <v>5</v>
       </c>
-      <c r="F22" s="112">
+      <c r="F22" s="98">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110">
-        <v>1</v>
-      </c>
-      <c r="J22" s="110"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="114"/>
-      <c r="M22" s="110"/>
-      <c r="N22" s="115"/>
-      <c r="O22" s="116"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96">
+        <v>1</v>
+      </c>
+      <c r="J22" s="96"/>
+      <c r="K22" s="99"/>
+      <c r="L22" s="100"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="101"/>
+      <c r="O22" s="102"/>
       <c r="R22"/>
     </row>
     <row r="23" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="117" t="s">
+      <c r="A23" s="166"/>
+      <c r="B23" s="161"/>
+      <c r="C23" s="162"/>
+      <c r="D23" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="118">
+      <c r="E23" s="104">
         <v>5</v>
       </c>
-      <c r="F23" s="119">
+      <c r="F23" s="105">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G23" s="117">
-        <v>1</v>
-      </c>
-      <c r="H23" s="117"/>
-      <c r="I23" s="117">
-        <v>1</v>
-      </c>
-      <c r="J23" s="117"/>
-      <c r="K23" s="120"/>
-      <c r="L23" s="121"/>
-      <c r="M23" s="117"/>
-      <c r="N23" s="122"/>
-      <c r="O23" s="123"/>
+      <c r="G23" s="103">
+        <v>1</v>
+      </c>
+      <c r="H23" s="103"/>
+      <c r="I23" s="103">
+        <v>1</v>
+      </c>
+      <c r="J23" s="103"/>
+      <c r="K23" s="106"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="103"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="109"/>
       <c r="R23"/>
     </row>
     <row r="24" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="110" t="s">
+      <c r="A24" s="166"/>
+      <c r="B24" s="161"/>
+      <c r="C24" s="162"/>
+      <c r="D24" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="111">
+      <c r="E24" s="97">
         <v>3</v>
       </c>
-      <c r="F24" s="112">
+      <c r="F24" s="98">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G24" s="110"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="110">
-        <v>1</v>
-      </c>
-      <c r="K24" s="113"/>
-      <c r="L24" s="114"/>
-      <c r="M24" s="110"/>
-      <c r="N24" s="115"/>
-      <c r="O24" s="116"/>
+      <c r="G24" s="96"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="96"/>
+      <c r="J24" s="96">
+        <v>1</v>
+      </c>
+      <c r="K24" s="99"/>
+      <c r="L24" s="100"/>
+      <c r="M24" s="96"/>
+      <c r="N24" s="101"/>
+      <c r="O24" s="102"/>
       <c r="R24"/>
     </row>
     <row r="25" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="124" t="s">
+      <c r="A25" s="166"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="162"/>
+      <c r="D25" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="125">
+      <c r="E25" s="111">
         <v>2</v>
       </c>
-      <c r="F25" s="126">
+      <c r="F25" s="112">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G25" s="124"/>
-      <c r="H25" s="124"/>
-      <c r="I25" s="124"/>
-      <c r="J25" s="124">
-        <v>1</v>
-      </c>
-      <c r="K25" s="127"/>
-      <c r="L25" s="128"/>
-      <c r="M25" s="124"/>
-      <c r="N25" s="129"/>
-      <c r="O25" s="130"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="110"/>
+      <c r="J25" s="110">
+        <v>1</v>
+      </c>
+      <c r="K25" s="113"/>
+      <c r="L25" s="114"/>
+      <c r="M25" s="110"/>
+      <c r="N25" s="115"/>
+      <c r="O25" s="116"/>
       <c r="R25"/>
     </row>
     <row r="26" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="5" t="s">
+      <c r="A26" s="166"/>
+      <c r="B26" s="161"/>
+      <c r="C26" s="169" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="103" t="s">
+      <c r="D26" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="104">
+      <c r="E26" s="90">
         <v>3</v>
       </c>
-      <c r="F26" s="105">
+      <c r="F26" s="91">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G26" s="103">
-        <v>1</v>
-      </c>
-      <c r="H26" s="103"/>
-      <c r="I26" s="103"/>
-      <c r="J26" s="103"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="103"/>
-      <c r="N26" s="108">
+      <c r="G26" s="89">
+        <v>1</v>
+      </c>
+      <c r="H26" s="89"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="93"/>
+      <c r="M26" s="89"/>
+      <c r="N26" s="94">
         <f>54.85-(54.85*10/100)</f>
         <v>49.365000000000002</v>
       </c>
-      <c r="O26" s="109"/>
+      <c r="O26" s="95"/>
       <c r="R26"/>
     </row>
     <row r="27" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="110" t="s">
+      <c r="A27" s="166"/>
+      <c r="B27" s="161"/>
+      <c r="C27" s="169"/>
+      <c r="D27" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="111">
+      <c r="E27" s="97">
         <v>3</v>
       </c>
-      <c r="F27" s="112">
+      <c r="F27" s="98">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110">
-        <v>1</v>
-      </c>
-      <c r="J27" s="110"/>
-      <c r="K27" s="113"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="110"/>
-      <c r="N27" s="115"/>
-      <c r="O27" s="116"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="96">
+        <v>1</v>
+      </c>
+      <c r="J27" s="96"/>
+      <c r="K27" s="99"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="101"/>
+      <c r="O27" s="102"/>
       <c r="R27"/>
     </row>
     <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="117" t="s">
+      <c r="A28" s="166"/>
+      <c r="B28" s="161"/>
+      <c r="C28" s="169"/>
+      <c r="D28" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="118">
+      <c r="E28" s="104">
         <v>3</v>
       </c>
-      <c r="F28" s="119">
+      <c r="F28" s="105">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G28" s="117"/>
-      <c r="H28" s="117"/>
-      <c r="I28" s="117">
-        <v>1</v>
-      </c>
-      <c r="J28" s="117"/>
-      <c r="K28" s="120"/>
-      <c r="L28" s="121"/>
-      <c r="M28" s="117"/>
-      <c r="N28" s="122"/>
-      <c r="O28" s="123"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="103">
+        <v>1</v>
+      </c>
+      <c r="J28" s="103"/>
+      <c r="K28" s="106"/>
+      <c r="L28" s="107"/>
+      <c r="M28" s="103"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="109"/>
       <c r="R28"/>
     </row>
     <row r="29" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="110" t="s">
+      <c r="A29" s="166"/>
+      <c r="B29" s="161"/>
+      <c r="C29" s="169"/>
+      <c r="D29" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="111">
-        <v>1</v>
-      </c>
-      <c r="F29" s="112">
+      <c r="E29" s="97">
+        <v>1</v>
+      </c>
+      <c r="F29" s="98">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G29" s="110"/>
-      <c r="H29" s="110"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="113"/>
-      <c r="L29" s="114"/>
-      <c r="M29" s="110"/>
-      <c r="N29" s="115"/>
-      <c r="O29" s="116"/>
+      <c r="G29" s="96"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="96"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="99"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="102"/>
       <c r="R29"/>
     </row>
     <row r="30" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="131" t="s">
+      <c r="A30" s="166"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="169"/>
+      <c r="D30" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="132">
+      <c r="E30" s="118">
         <v>0</v>
       </c>
-      <c r="F30" s="133">
+      <c r="F30" s="119">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="131"/>
-      <c r="H30" s="131"/>
-      <c r="I30" s="131"/>
-      <c r="J30" s="131"/>
-      <c r="K30" s="134"/>
-      <c r="L30" s="135"/>
-      <c r="M30" s="131"/>
-      <c r="N30" s="136"/>
-      <c r="O30" s="137"/>
+      <c r="G30" s="117"/>
+      <c r="H30" s="117"/>
+      <c r="I30" s="117"/>
+      <c r="J30" s="117"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="121"/>
+      <c r="M30" s="117"/>
+      <c r="N30" s="122"/>
+      <c r="O30" s="123"/>
       <c r="R30"/>
     </row>
     <row r="31" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="4" t="s">
+      <c r="A31" s="166"/>
+      <c r="B31" s="161"/>
+      <c r="C31" s="170" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="103" t="s">
+      <c r="D31" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="104">
+      <c r="E31" s="90">
         <v>7</v>
       </c>
-      <c r="F31" s="119">
+      <c r="F31" s="105">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G31" s="117">
+      <c r="G31" s="103">
         <v>2</v>
       </c>
-      <c r="H31" s="117"/>
-      <c r="I31" s="117"/>
-      <c r="J31" s="117"/>
-      <c r="K31" s="120"/>
-      <c r="L31" s="121"/>
-      <c r="M31" s="117"/>
-      <c r="N31" s="122">
+      <c r="H31" s="103"/>
+      <c r="I31" s="103"/>
+      <c r="J31" s="103"/>
+      <c r="K31" s="106"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="108">
         <f>38.88-(38.88*10/100)</f>
         <v>34.992000000000004</v>
       </c>
-      <c r="O31" s="123"/>
+      <c r="O31" s="109"/>
       <c r="R31"/>
     </row>
     <row r="32" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="110" t="s">
+      <c r="A32" s="166"/>
+      <c r="B32" s="161"/>
+      <c r="C32" s="170"/>
+      <c r="D32" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="111">
+      <c r="E32" s="97">
         <v>6</v>
       </c>
-      <c r="F32" s="112">
+      <c r="F32" s="98">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G32" s="96">
+        <v>1</v>
+      </c>
+      <c r="H32" s="96"/>
+      <c r="I32" s="96">
+        <v>2</v>
+      </c>
+      <c r="J32" s="96"/>
+      <c r="K32" s="99"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="101"/>
+      <c r="O32" s="102"/>
+      <c r="R32"/>
+    </row>
+    <row r="33" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="166"/>
+      <c r="B33" s="161"/>
+      <c r="C33" s="170"/>
+      <c r="D33" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="104">
         <v>4</v>
       </c>
-      <c r="G32" s="110">
-        <v>1</v>
-      </c>
-      <c r="H32" s="110"/>
-      <c r="I32" s="110">
-        <v>1</v>
-      </c>
-      <c r="J32" s="110"/>
-      <c r="K32" s="113"/>
-      <c r="L32" s="114"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="115"/>
-      <c r="O32" s="116"/>
-      <c r="R32"/>
-    </row>
-    <row r="33" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="117" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="118">
-        <v>4</v>
-      </c>
-      <c r="F33" s="119">
+      <c r="F33" s="105">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G33" s="103"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="103">
+        <v>1</v>
+      </c>
+      <c r="K33" s="106"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="103"/>
+      <c r="N33" s="108"/>
+      <c r="O33" s="109"/>
+      <c r="R33"/>
+    </row>
+    <row r="34" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="166"/>
+      <c r="B34" s="161"/>
+      <c r="C34" s="170"/>
+      <c r="D34" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="97">
         <v>2</v>
       </c>
-      <c r="G33" s="117"/>
-      <c r="H33" s="117"/>
-      <c r="I33" s="117">
-        <v>1</v>
-      </c>
-      <c r="J33" s="117">
-        <v>1</v>
-      </c>
-      <c r="K33" s="120"/>
-      <c r="L33" s="121"/>
-      <c r="M33" s="117"/>
-      <c r="N33" s="122"/>
-      <c r="O33" s="123"/>
-      <c r="R33"/>
-    </row>
-    <row r="34" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="110" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="111">
-        <v>2</v>
-      </c>
-      <c r="F34" s="112">
+      <c r="F34" s="98">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G34" s="110"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110">
-        <v>1</v>
-      </c>
-      <c r="K34" s="113"/>
-      <c r="L34" s="114"/>
-      <c r="M34" s="110"/>
-      <c r="N34" s="115"/>
-      <c r="O34" s="116"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="96"/>
+      <c r="J34" s="96">
+        <v>1</v>
+      </c>
+      <c r="K34" s="99"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="101"/>
+      <c r="O34" s="102"/>
       <c r="R34"/>
     </row>
     <row r="35" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="138" t="s">
+      <c r="A35" s="166"/>
+      <c r="B35" s="161"/>
+      <c r="C35" s="170"/>
+      <c r="D35" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="139">
-        <v>1</v>
-      </c>
-      <c r="F35" s="140">
+      <c r="E35" s="125">
+        <v>1</v>
+      </c>
+      <c r="F35" s="126">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G35" s="138"/>
-      <c r="H35" s="138"/>
-      <c r="I35" s="138"/>
-      <c r="J35" s="138"/>
-      <c r="K35" s="141"/>
-      <c r="L35" s="142"/>
-      <c r="M35" s="138"/>
-      <c r="N35" s="143"/>
-      <c r="O35" s="144"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="124"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="124"/>
+      <c r="K35" s="127"/>
+      <c r="L35" s="128"/>
+      <c r="M35" s="124"/>
+      <c r="N35" s="129"/>
+      <c r="O35" s="130"/>
       <c r="R35"/>
     </row>
     <row r="36" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="157" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="145" t="s">
+      <c r="D36" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="146">
+      <c r="E36" s="132">
         <v>10</v>
       </c>
-      <c r="F36" s="147">
+      <c r="F36" s="133">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G36" s="145">
-        <v>1</v>
-      </c>
-      <c r="H36" s="145">
+      <c r="G36" s="131">
+        <v>1</v>
+      </c>
+      <c r="H36" s="131">
         <v>2</v>
       </c>
-      <c r="I36" s="145">
-        <v>1</v>
-      </c>
-      <c r="J36" s="145">
-        <v>1</v>
-      </c>
-      <c r="K36" s="148"/>
-      <c r="L36" s="149"/>
-      <c r="M36" s="145"/>
-      <c r="N36" s="150">
+      <c r="I36" s="131">
+        <v>1</v>
+      </c>
+      <c r="J36" s="131">
+        <v>1</v>
+      </c>
+      <c r="K36" s="134"/>
+      <c r="L36" s="135"/>
+      <c r="M36" s="131"/>
+      <c r="N36" s="136">
         <f>49.18-(49.18*10/100)</f>
         <v>44.262</v>
       </c>
-      <c r="O36" s="151"/>
+      <c r="O36" s="137"/>
       <c r="R36"/>
     </row>
     <row r="37" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="41" t="s">
+      <c r="A37" s="156"/>
+      <c r="B37" s="157"/>
+      <c r="C37" s="158"/>
+      <c r="D37" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="42">
+      <c r="E37" s="28">
         <v>13</v>
       </c>
-      <c r="F37" s="35">
+      <c r="F37" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41">
-        <v>1</v>
-      </c>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41">
+      <c r="G37" s="27"/>
+      <c r="H37" s="27">
+        <v>1</v>
+      </c>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27">
         <v>4</v>
       </c>
-      <c r="K37" s="44"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="47"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="33"/>
       <c r="R37"/>
     </row>
     <row r="38" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="33" t="s">
+      <c r="A38" s="156"/>
+      <c r="B38" s="157"/>
+      <c r="C38" s="158"/>
+      <c r="D38" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="34">
+      <c r="E38" s="20">
         <v>6</v>
       </c>
-      <c r="F38" s="43">
+      <c r="F38" s="29">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="38"/>
-      <c r="O38" s="39"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="25"/>
       <c r="R38"/>
     </row>
     <row r="39" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="48" t="s">
+      <c r="A39" s="156"/>
+      <c r="B39" s="157"/>
+      <c r="C39" s="158"/>
+      <c r="D39" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="49">
+      <c r="E39" s="35">
         <v>3</v>
       </c>
-      <c r="F39" s="50">
+      <c r="F39" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="51">
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="37">
         <v>2</v>
       </c>
-      <c r="L39" s="52"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="54"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="40"/>
       <c r="R39"/>
     </row>
     <row r="40" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="9" t="s">
+      <c r="A40" s="156"/>
+      <c r="B40" s="157"/>
+      <c r="C40" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="56">
+      <c r="E40" s="42">
         <v>4</v>
       </c>
-      <c r="F40" s="57">
+      <c r="F40" s="43">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55">
-        <v>1</v>
-      </c>
-      <c r="J40" s="55"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="55"/>
-      <c r="N40" s="60">
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="41">
+        <v>1</v>
+      </c>
+      <c r="J40" s="41"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="46">
         <f>56.01-(56.01*10/100)</f>
         <v>50.408999999999999</v>
       </c>
-      <c r="O40" s="61"/>
+      <c r="O40" s="47"/>
       <c r="R40"/>
     </row>
     <row r="41" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="62" t="s">
+      <c r="A41" s="156"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="159"/>
+      <c r="D41" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="63">
+      <c r="E41" s="49">
         <v>4</v>
       </c>
-      <c r="F41" s="64">
-        <f t="shared" ref="F41:F72" si="1">E41-G41-H41-I41-J41-K41</f>
+      <c r="F41" s="50">
+        <f t="shared" ref="F41:F60" si="1">E41-G41-H41-I41-J41-K41</f>
         <v>2</v>
       </c>
-      <c r="G41" s="62"/>
-      <c r="H41" s="62">
-        <v>1</v>
-      </c>
-      <c r="I41" s="62"/>
-      <c r="J41" s="62">
-        <v>1</v>
-      </c>
-      <c r="K41" s="65"/>
-      <c r="L41" s="66"/>
-      <c r="M41" s="62"/>
-      <c r="N41" s="67"/>
-      <c r="O41" s="68"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48">
+        <v>1</v>
+      </c>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48">
+        <v>1</v>
+      </c>
+      <c r="K41" s="51"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="54"/>
       <c r="R41"/>
     </row>
     <row r="42" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="69" t="s">
+      <c r="A42" s="156"/>
+      <c r="B42" s="157"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="70">
+      <c r="E42" s="56">
         <v>0</v>
       </c>
-      <c r="F42" s="71">
+      <c r="F42" s="57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="73"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="75"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="58"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="60"/>
+      <c r="O42" s="61"/>
       <c r="R42"/>
     </row>
     <row r="43" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="76" t="s">
+      <c r="A43" s="156"/>
+      <c r="B43" s="157"/>
+      <c r="C43" s="159"/>
+      <c r="D43" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="77">
+      <c r="E43" s="63">
         <v>2</v>
       </c>
-      <c r="F43" s="78">
+      <c r="F43" s="64">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="76"/>
-      <c r="K43" s="79">
-        <v>1</v>
-      </c>
-      <c r="L43" s="80"/>
-      <c r="M43" s="76"/>
-      <c r="N43" s="81"/>
-      <c r="O43" s="82"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="65">
+        <v>1</v>
+      </c>
+      <c r="L43" s="66"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="67"/>
+      <c r="O43" s="68"/>
       <c r="R43"/>
     </row>
     <row r="44" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="8" t="s">
+      <c r="A44" s="156"/>
+      <c r="B44" s="157"/>
+      <c r="C44" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="83">
+      <c r="E44" s="69">
         <v>3</v>
       </c>
-      <c r="F44" s="35">
+      <c r="F44" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G44" s="33">
+      <c r="G44" s="19">
         <v>2</v>
       </c>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33">
-        <v>1</v>
-      </c>
-      <c r="K44" s="36"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="38">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19">
+        <v>1</v>
+      </c>
+      <c r="K44" s="22"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="24">
         <f>50.08-(50.08*10/100)</f>
         <v>45.072000000000003</v>
       </c>
-      <c r="O44" s="39"/>
+      <c r="O44" s="25"/>
       <c r="R44"/>
     </row>
     <row r="45" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="84" t="s">
+      <c r="A45" s="156"/>
+      <c r="B45" s="157"/>
+      <c r="C45" s="160"/>
+      <c r="D45" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="85">
+      <c r="E45" s="71">
         <v>8</v>
       </c>
-      <c r="F45" s="43">
+      <c r="F45" s="29">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G45" s="84">
-        <v>1</v>
-      </c>
-      <c r="H45" s="84"/>
-      <c r="I45" s="84"/>
-      <c r="J45" s="84">
-        <v>1</v>
-      </c>
-      <c r="K45" s="86"/>
-      <c r="L45" s="87"/>
-      <c r="M45" s="84"/>
-      <c r="N45" s="88"/>
-      <c r="O45" s="89"/>
+      <c r="G45" s="70">
+        <v>1</v>
+      </c>
+      <c r="H45" s="70"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="70">
+        <v>1</v>
+      </c>
+      <c r="K45" s="72"/>
+      <c r="L45" s="73"/>
+      <c r="M45" s="70"/>
+      <c r="N45" s="74"/>
+      <c r="O45" s="75"/>
       <c r="R45"/>
     </row>
     <row r="46" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="90" t="s">
+      <c r="A46" s="156"/>
+      <c r="B46" s="157"/>
+      <c r="C46" s="160"/>
+      <c r="D46" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="91">
+      <c r="E46" s="77">
         <v>13</v>
       </c>
-      <c r="F46" s="43">
+      <c r="F46" s="29">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G46" s="90"/>
-      <c r="H46" s="90">
+      <c r="G46" s="76"/>
+      <c r="H46" s="76">
         <v>3</v>
       </c>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90">
+      <c r="I46" s="76"/>
+      <c r="J46" s="76">
         <v>2</v>
       </c>
-      <c r="K46" s="92"/>
-      <c r="L46" s="93"/>
-      <c r="M46" s="90"/>
-      <c r="N46" s="94"/>
-      <c r="O46" s="95"/>
+      <c r="K46" s="78"/>
+      <c r="L46" s="79"/>
+      <c r="M46" s="76"/>
+      <c r="N46" s="80"/>
+      <c r="O46" s="81"/>
       <c r="R46"/>
     </row>
     <row r="47" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="84" t="s">
+      <c r="A47" s="156"/>
+      <c r="B47" s="157"/>
+      <c r="C47" s="160"/>
+      <c r="D47" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="85">
+      <c r="E47" s="71">
         <v>7</v>
       </c>
-      <c r="F47" s="43">
+      <c r="F47" s="29">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
-      <c r="I47" s="84"/>
-      <c r="J47" s="84">
-        <v>1</v>
-      </c>
-      <c r="K47" s="86"/>
-      <c r="L47" s="87"/>
-      <c r="M47" s="84"/>
-      <c r="N47" s="88"/>
-      <c r="O47" s="89"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="70"/>
+      <c r="J47" s="70">
+        <v>1</v>
+      </c>
+      <c r="K47" s="72"/>
+      <c r="L47" s="73"/>
+      <c r="M47" s="70"/>
+      <c r="N47" s="74"/>
+      <c r="O47" s="75"/>
       <c r="R47"/>
     </row>
     <row r="48" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="90" t="s">
+      <c r="A48" s="156"/>
+      <c r="B48" s="157"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="91">
+      <c r="E48" s="77">
         <v>7</v>
       </c>
-      <c r="F48" s="43">
+      <c r="F48" s="29">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="90">
+      <c r="G48" s="76"/>
+      <c r="H48" s="76"/>
+      <c r="I48" s="76"/>
+      <c r="J48" s="76">
         <v>2</v>
       </c>
-      <c r="K48" s="92">
+      <c r="K48" s="78">
         <v>2</v>
       </c>
-      <c r="L48" s="93"/>
-      <c r="M48" s="90"/>
-      <c r="N48" s="94"/>
-      <c r="O48" s="95"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="76"/>
+      <c r="N48" s="80"/>
+      <c r="O48" s="81"/>
       <c r="R48"/>
     </row>
     <row r="49" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="156"/>
+      <c r="B49" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="162" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="103" t="s">
+      <c r="D49" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="104">
+      <c r="E49" s="90">
         <v>4</v>
       </c>
-      <c r="F49" s="105">
+      <c r="F49" s="91">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G49" s="103">
+      <c r="G49" s="89">
         <v>2</v>
       </c>
-      <c r="H49" s="103"/>
-      <c r="I49" s="103"/>
-      <c r="J49" s="103">
-        <v>1</v>
-      </c>
-      <c r="K49" s="106"/>
-      <c r="L49" s="107"/>
-      <c r="M49" s="103"/>
-      <c r="N49" s="108">
+      <c r="H49" s="89"/>
+      <c r="I49" s="89"/>
+      <c r="J49" s="89">
+        <v>1</v>
+      </c>
+      <c r="K49" s="92"/>
+      <c r="L49" s="93"/>
+      <c r="M49" s="89"/>
+      <c r="N49" s="94">
         <f>48.02-(48.02*10/100)</f>
         <v>43.218000000000004</v>
       </c>
-      <c r="O49" s="109"/>
+      <c r="O49" s="95"/>
       <c r="R49"/>
     </row>
     <row r="50" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="110" t="s">
+      <c r="A50" s="156"/>
+      <c r="B50" s="161"/>
+      <c r="C50" s="162"/>
+      <c r="D50" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="111">
+      <c r="E50" s="97">
         <v>5</v>
       </c>
-      <c r="F50" s="112">
+      <c r="F50" s="98">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G50" s="110"/>
-      <c r="H50" s="110"/>
-      <c r="I50" s="110"/>
-      <c r="J50" s="110">
-        <v>1</v>
-      </c>
-      <c r="K50" s="113"/>
-      <c r="L50" s="114"/>
-      <c r="M50" s="110"/>
-      <c r="N50" s="115"/>
-      <c r="O50" s="116"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="96">
+        <v>1</v>
+      </c>
+      <c r="K50" s="99"/>
+      <c r="L50" s="100"/>
+      <c r="M50" s="96"/>
+      <c r="N50" s="101"/>
+      <c r="O50" s="102"/>
       <c r="R50"/>
     </row>
     <row r="51" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="117" t="s">
+      <c r="A51" s="156"/>
+      <c r="B51" s="161"/>
+      <c r="C51" s="162"/>
+      <c r="D51" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="118">
-        <v>1</v>
-      </c>
-      <c r="F51" s="119">
+      <c r="E51" s="104">
+        <v>1</v>
+      </c>
+      <c r="F51" s="105">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G51" s="117"/>
-      <c r="H51" s="117"/>
-      <c r="I51" s="117"/>
-      <c r="J51" s="117"/>
-      <c r="K51" s="120"/>
-      <c r="L51" s="121"/>
-      <c r="M51" s="117"/>
-      <c r="N51" s="122"/>
-      <c r="O51" s="123"/>
+      <c r="G51" s="103"/>
+      <c r="H51" s="103"/>
+      <c r="I51" s="103"/>
+      <c r="J51" s="103"/>
+      <c r="K51" s="106"/>
+      <c r="L51" s="107"/>
+      <c r="M51" s="103"/>
+      <c r="N51" s="108"/>
+      <c r="O51" s="109"/>
       <c r="R51"/>
     </row>
     <row r="52" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="110" t="s">
+      <c r="A52" s="156"/>
+      <c r="B52" s="161"/>
+      <c r="C52" s="162"/>
+      <c r="D52" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="111">
+      <c r="E52" s="97">
         <v>0</v>
       </c>
-      <c r="F52" s="112">
+      <c r="F52" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G52" s="110"/>
-      <c r="H52" s="110"/>
-      <c r="I52" s="110"/>
-      <c r="J52" s="110"/>
-      <c r="K52" s="113"/>
-      <c r="L52" s="114"/>
-      <c r="M52" s="110"/>
-      <c r="N52" s="115"/>
-      <c r="O52" s="116"/>
+      <c r="G52" s="96"/>
+      <c r="H52" s="96"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="96"/>
+      <c r="K52" s="99"/>
+      <c r="L52" s="100"/>
+      <c r="M52" s="96"/>
+      <c r="N52" s="101"/>
+      <c r="O52" s="102"/>
       <c r="R52"/>
     </row>
     <row r="53" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="124" t="s">
+      <c r="A53" s="156"/>
+      <c r="B53" s="161"/>
+      <c r="C53" s="162"/>
+      <c r="D53" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="125">
+      <c r="E53" s="111">
         <v>0</v>
       </c>
-      <c r="F53" s="126">
+      <c r="F53" s="112">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G53" s="124"/>
-      <c r="H53" s="124"/>
-      <c r="I53" s="124"/>
-      <c r="J53" s="124"/>
-      <c r="K53" s="127"/>
-      <c r="L53" s="128"/>
-      <c r="M53" s="124"/>
-      <c r="N53" s="129"/>
-      <c r="O53" s="130"/>
+      <c r="G53" s="110"/>
+      <c r="H53" s="110"/>
+      <c r="I53" s="110"/>
+      <c r="J53" s="110"/>
+      <c r="K53" s="113"/>
+      <c r="L53" s="114"/>
+      <c r="M53" s="110"/>
+      <c r="N53" s="115"/>
+      <c r="O53" s="116"/>
       <c r="R53"/>
     </row>
     <row r="54" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="169" t="s">
+      <c r="A54" s="156"/>
+      <c r="B54" s="161"/>
+      <c r="C54" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="103" t="s">
+      <c r="D54" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="E54" s="104">
+      <c r="E54" s="90">
         <v>4</v>
       </c>
-      <c r="F54" s="105">
+      <c r="F54" s="91">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G54" s="103">
-        <v>1</v>
-      </c>
-      <c r="H54" s="103"/>
-      <c r="I54" s="103"/>
-      <c r="J54" s="103"/>
-      <c r="K54" s="106"/>
-      <c r="L54" s="107"/>
-      <c r="M54" s="103"/>
-      <c r="N54" s="108">
+      <c r="G54" s="89">
+        <v>1</v>
+      </c>
+      <c r="H54" s="89"/>
+      <c r="I54" s="89"/>
+      <c r="J54" s="89"/>
+      <c r="K54" s="92"/>
+      <c r="L54" s="93"/>
+      <c r="M54" s="89"/>
+      <c r="N54" s="94">
         <f>54.85-(54.85*10/100)</f>
         <v>49.365000000000002</v>
       </c>
-      <c r="O54" s="109"/>
+      <c r="O54" s="95"/>
       <c r="R54"/>
     </row>
     <row r="55" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="169"/>
-      <c r="D55" s="110" t="s">
+      <c r="A55" s="156"/>
+      <c r="B55" s="161"/>
+      <c r="C55" s="163"/>
+      <c r="D55" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="E55" s="111">
+      <c r="E55" s="97">
         <v>5</v>
       </c>
-      <c r="F55" s="112">
+      <c r="F55" s="98">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G55" s="110"/>
-      <c r="H55" s="110"/>
-      <c r="I55" s="110"/>
-      <c r="J55" s="110">
-        <v>1</v>
-      </c>
-      <c r="K55" s="113"/>
-      <c r="L55" s="114"/>
-      <c r="M55" s="110"/>
-      <c r="N55" s="115"/>
-      <c r="O55" s="116"/>
+      <c r="G55" s="96"/>
+      <c r="H55" s="96"/>
+      <c r="I55" s="96"/>
+      <c r="J55" s="96">
+        <v>1</v>
+      </c>
+      <c r="K55" s="99"/>
+      <c r="L55" s="100"/>
+      <c r="M55" s="96"/>
+      <c r="N55" s="101"/>
+      <c r="O55" s="102"/>
       <c r="R55"/>
     </row>
     <row r="56" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="169"/>
-      <c r="D56" s="117" t="s">
+      <c r="A56" s="156"/>
+      <c r="B56" s="161"/>
+      <c r="C56" s="163"/>
+      <c r="D56" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="118">
-        <v>1</v>
-      </c>
-      <c r="F56" s="119">
+      <c r="E56" s="104">
+        <v>1</v>
+      </c>
+      <c r="F56" s="105">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G56" s="117"/>
-      <c r="H56" s="117"/>
-      <c r="I56" s="117"/>
-      <c r="J56" s="117"/>
-      <c r="K56" s="120"/>
-      <c r="L56" s="121"/>
-      <c r="M56" s="117"/>
-      <c r="N56" s="122"/>
-      <c r="O56" s="123"/>
+      <c r="G56" s="103"/>
+      <c r="H56" s="103"/>
+      <c r="I56" s="103"/>
+      <c r="J56" s="103"/>
+      <c r="K56" s="106"/>
+      <c r="L56" s="107"/>
+      <c r="M56" s="103"/>
+      <c r="N56" s="108"/>
+      <c r="O56" s="109"/>
       <c r="R56"/>
     </row>
     <row r="57" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A57" s="3"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="169"/>
-      <c r="D57" s="110" t="s">
+      <c r="A57" s="156"/>
+      <c r="B57" s="161"/>
+      <c r="C57" s="163"/>
+      <c r="D57" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="E57" s="111">
+      <c r="E57" s="97">
         <v>0</v>
       </c>
-      <c r="F57" s="112">
+      <c r="F57" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G57" s="110"/>
-      <c r="H57" s="110"/>
-      <c r="I57" s="110"/>
-      <c r="J57" s="110"/>
-      <c r="K57" s="113"/>
-      <c r="L57" s="114"/>
-      <c r="M57" s="110"/>
-      <c r="N57" s="115"/>
-      <c r="O57" s="116"/>
+      <c r="G57" s="96"/>
+      <c r="H57" s="96"/>
+      <c r="I57" s="96"/>
+      <c r="J57" s="96"/>
+      <c r="K57" s="99"/>
+      <c r="L57" s="100"/>
+      <c r="M57" s="96"/>
+      <c r="N57" s="101"/>
+      <c r="O57" s="102"/>
       <c r="R57"/>
     </row>
     <row r="58" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="169"/>
-      <c r="D58" s="124" t="s">
+      <c r="A58" s="156"/>
+      <c r="B58" s="161"/>
+      <c r="C58" s="163"/>
+      <c r="D58" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="E58" s="125">
+      <c r="E58" s="111">
         <v>0</v>
       </c>
-      <c r="F58" s="126">
+      <c r="F58" s="112">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G58" s="124"/>
-      <c r="H58" s="124"/>
-      <c r="I58" s="124"/>
-      <c r="J58" s="124"/>
-      <c r="K58" s="127"/>
-      <c r="L58" s="128"/>
-      <c r="M58" s="124"/>
-      <c r="N58" s="129"/>
-      <c r="O58" s="130"/>
+      <c r="G58" s="110"/>
+      <c r="H58" s="110"/>
+      <c r="I58" s="110"/>
+      <c r="J58" s="110"/>
+      <c r="K58" s="113"/>
+      <c r="L58" s="114"/>
+      <c r="M58" s="110"/>
+      <c r="N58" s="115"/>
+      <c r="O58" s="116"/>
       <c r="R58"/>
     </row>
     <row r="59" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59"/>
-      <c r="C59" s="170" t="s">
+      <c r="C59" s="155" t="s">
         <v>36</v>
       </c>
-      <c r="D59" s="152" t="s">
+      <c r="D59" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="153">
+      <c r="E59" s="139">
         <v>36</v>
       </c>
-      <c r="F59" s="154">
+      <c r="F59" s="140">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="G59" s="155">
+      <c r="G59" s="141">
         <v>2</v>
       </c>
-      <c r="H59" s="155"/>
-      <c r="I59" s="155">
+      <c r="H59" s="141"/>
+      <c r="I59" s="141">
         <v>10</v>
       </c>
-      <c r="J59" s="155">
+      <c r="J59" s="141">
         <v>2</v>
       </c>
-      <c r="K59" s="156"/>
-      <c r="L59" s="157"/>
-      <c r="M59" s="155"/>
-      <c r="N59" s="158">
+      <c r="K59" s="142"/>
+      <c r="L59" s="143"/>
+      <c r="M59" s="141"/>
+      <c r="N59" s="144">
         <v>4.6500000000000004</v>
       </c>
-      <c r="O59" s="159"/>
-      <c r="R59" s="40"/>
+      <c r="O59" s="145"/>
+      <c r="R59" s="26"/>
     </row>
     <row r="60" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
-      <c r="C60" s="170"/>
-      <c r="D60" s="160" t="s">
+      <c r="C60" s="155"/>
+      <c r="D60" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="161">
+      <c r="E60" s="147">
         <v>64</v>
       </c>
-      <c r="F60" s="162">
+      <c r="F60" s="148">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="G60" s="163"/>
-      <c r="H60" s="163">
+      <c r="G60" s="149"/>
+      <c r="H60" s="149">
         <v>5</v>
       </c>
-      <c r="I60" s="163"/>
-      <c r="J60" s="163">
+      <c r="I60" s="149"/>
+      <c r="J60" s="149">
         <v>8</v>
       </c>
-      <c r="K60" s="164">
+      <c r="K60" s="150">
         <v>2</v>
       </c>
-      <c r="L60" s="165"/>
-      <c r="M60" s="166"/>
-      <c r="N60" s="167"/>
-      <c r="O60" s="168"/>
+      <c r="L60" s="151"/>
+      <c r="M60" s="152"/>
+      <c r="N60" s="153"/>
+      <c r="O60" s="154"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61"/>
@@ -4309,51 +4307,42 @@
       <c r="A62"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A36:A58"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:O7"/>
@@ -4366,6 +4355,15 @@
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C35"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A36:A58"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Bestand für Lager aktualisiert, devinitver Verkaufsstatus Anfangsbestand/Endbestand
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,6 +15,8 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$36:$P$58</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Tabelle1!$7:$8</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -30,6 +32,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
+    <author>Ruth</author>
   </authors>
   <commentList>
     <comment ref="G23" authorId="0" shapeId="0">
@@ -43,6 +46,30 @@
           </rPr>
           <t>Ruth:
 für Schwester</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H23" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+FÜR ALEX</t>
         </r>
       </text>
     </comment>
@@ -60,6 +87,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="H32" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+FÜR ALEX</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G36" authorId="0" shapeId="0">
       <text>
         <r>
@@ -70,7 +121,31 @@
             <charset val="1"/>
           </rPr>
           <t>Ruth:
-Guide Südtirol</t>
+Guide Südtirol, muss noch übergeben werden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I36" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+für Simon, muss noch übergeben</t>
         </r>
       </text>
     </comment>
@@ -84,7 +159,31 @@
             <charset val="1"/>
           </rPr>
           <t>Ruth:
-Guide Südtirol</t>
+Guide Südtirol, muss noch übergeben werden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I45" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+für simon, muss noch übergeben werden</t>
         </r>
       </text>
     </comment>
@@ -93,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
   <si>
     <t>Inventar</t>
   </si>
@@ -260,16 +359,21 @@
   <si>
     <t>Helga W (Kunden)</t>
   </si>
+  <si>
+    <t>BESTAND FÜR 
+VERKAUF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ _€"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -390,6 +494,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -501,7 +618,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="75">
+  <borders count="87">
     <border>
       <left/>
       <right/>
@@ -513,19 +630,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1110,17 +1214,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -1508,6 +1601,180 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1517,7 +1784,7 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1539,308 +1806,305 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="16" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1849,172 +2113,280 @@
     <xf numFmtId="0" fontId="12" fillId="15" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="69" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="70" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="69" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="72" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="69" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="70" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="72" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="70" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="70" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="74" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="74" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="75" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="77" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="80" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="81" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="10" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="10" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="11" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="13" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="11" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="13" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="8" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="16" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="49" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="52" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="8" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2114,7 +2486,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -2163,7 +2535,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -2212,7 +2584,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -2261,7 +2633,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -2605,10 +2977,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW69"/>
+  <dimension ref="A1:IX69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2619,19 +2992,21 @@
     <col min="4" max="4" width="7.42578125" style="2"/>
     <col min="5" max="5" width="11" style="3"/>
     <col min="6" max="11" width="6.5703125" style="1"/>
-    <col min="12" max="13" width="10.42578125" style="1"/>
-    <col min="14" max="14" width="10.5703125" style="4"/>
-    <col min="15" max="257" width="10.42578125" style="1"/>
-    <col min="258" max="1025" width="8.28515625"/>
+    <col min="12" max="12" width="10.42578125" style="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="10.42578125" style="1"/>
+    <col min="15" max="15" width="10.5703125" style="4"/>
+    <col min="16" max="258" width="10.42578125" style="1"/>
+    <col min="259" max="1026" width="8.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2"/>
@@ -2647,10 +3022,11 @@
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
-      <c r="Q2"/>
+      <c r="P2"/>
       <c r="R2"/>
-    </row>
-    <row r="3" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="S2"/>
+    </row>
+    <row r="3" spans="1:19" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -2670,16 +3046,17 @@
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
-      <c r="Q3"/>
+      <c r="P3"/>
       <c r="R3"/>
-    </row>
-    <row r="4" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="S3"/>
+    </row>
+    <row r="4" spans="1:19" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10">
         <f ca="1">TODAY()</f>
-        <v>42682</v>
+        <v>42699</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2694,10 +3071,11 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
-      <c r="Q4"/>
+      <c r="P4"/>
       <c r="R4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -2713,10 +3091,11 @@
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
-      <c r="Q5"/>
+      <c r="P5"/>
       <c r="R5"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5"/>
+    </row>
+    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -2732,37 +3111,39 @@
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
-      <c r="Q6"/>
+      <c r="P6"/>
       <c r="R6"/>
-    </row>
-    <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="155" t="s">
+      <c r="S6"/>
+    </row>
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="155"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="156" t="s">
+      <c r="B7" s="200"/>
+      <c r="C7" s="200"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="156"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="156"/>
-      <c r="J7" s="156"/>
-      <c r="K7" s="156"/>
-      <c r="L7" s="156" t="s">
+      <c r="G7" s="201"/>
+      <c r="H7" s="201"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="201"/>
+      <c r="L7" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="156" t="s">
+      <c r="M7" s="201"/>
+      <c r="N7" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="156"/>
-      <c r="O7" s="156"/>
-      <c r="Q7"/>
+      <c r="O7" s="201"/>
+      <c r="P7" s="202"/>
       <c r="R7"/>
-    </row>
-    <row r="8" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="1:19" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
@@ -2796,29 +3177,32 @@
       <c r="K8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="179" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="N8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="O8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="17" t="s">
+      <c r="P8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Q8"/>
       <c r="R8"/>
-    </row>
-    <row r="9" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="157" t="s">
+      <c r="S8"/>
+    </row>
+    <row r="9" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="B9" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="159" t="s">
+      <c r="C9" s="161" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -2840,20 +3224,29 @@
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="22"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="24">
+      <c r="L9" s="23">
+        <f>F9</f>
+        <v>11</v>
+      </c>
+      <c r="M9" s="164"/>
+      <c r="N9" s="19">
+        <f>L9-M9</f>
+        <v>11</v>
+      </c>
+      <c r="O9" s="24">
         <f>49.18-(49.18*10/100)</f>
         <v>44.262</v>
       </c>
-      <c r="O9" s="25"/>
-      <c r="Q9" s="26"/>
-      <c r="R9"/>
-    </row>
-    <row r="10" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="157"/>
-      <c r="B10" s="158"/>
-      <c r="C10" s="159"/>
+      <c r="P9" s="180">
+        <v>105</v>
+      </c>
+      <c r="R9" s="26"/>
+      <c r="S9"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="159"/>
+      <c r="B10" s="160"/>
+      <c r="C10" s="161"/>
       <c r="D10" s="27" t="s">
         <v>27</v>
       </c>
@@ -2871,17 +3264,24 @@
         <v>3</v>
       </c>
       <c r="K10" s="30"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="33"/>
-      <c r="Q10" s="26"/>
-      <c r="R10"/>
-    </row>
-    <row r="11" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="157"/>
-      <c r="B11" s="158"/>
-      <c r="C11" s="159"/>
+      <c r="L10" s="31">
+        <f t="shared" ref="L10:L35" si="1">F10</f>
+        <v>15</v>
+      </c>
+      <c r="M10" s="165"/>
+      <c r="N10" s="27">
+        <f t="shared" ref="N10:N35" si="2">L10-M10</f>
+        <v>15</v>
+      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="181"/>
+      <c r="R10" s="26"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="159"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="161"/>
       <c r="D11" s="19" t="s">
         <v>28</v>
       </c>
@@ -2897,17 +3297,24 @@
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="22"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="25"/>
-      <c r="Q11" s="26"/>
-      <c r="R11"/>
-    </row>
-    <row r="12" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="157"/>
-      <c r="B12" s="158"/>
-      <c r="C12" s="159"/>
+      <c r="L11" s="23">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="M11" s="164"/>
+      <c r="N11" s="19">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O11" s="24"/>
+      <c r="P11" s="180"/>
+      <c r="R11" s="26"/>
+      <c r="S11"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="159"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="161"/>
       <c r="D12" s="34" t="s">
         <v>29</v>
       </c>
@@ -2925,17 +3332,24 @@
       <c r="K12" s="37">
         <v>2</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-      <c r="Q12" s="26"/>
-      <c r="R12"/>
-    </row>
-    <row r="13" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="157"/>
-      <c r="B13" s="158"/>
-      <c r="C13" s="160" t="s">
+      <c r="L12" s="38">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="M12" s="166"/>
+      <c r="N12" s="34">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O12" s="39"/>
+      <c r="P12" s="182"/>
+      <c r="R12" s="26"/>
+      <c r="S12"/>
+    </row>
+    <row r="13" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="159"/>
+      <c r="B13" s="160"/>
+      <c r="C13" s="154" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="41" t="s">
@@ -2955,20 +3369,29 @@
       </c>
       <c r="J13" s="41"/>
       <c r="K13" s="44"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="46">
+      <c r="L13" s="45">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M13" s="167"/>
+      <c r="N13" s="41">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="O13" s="46">
         <f>56.01-(56.01*10/100)</f>
         <v>50.408999999999999</v>
       </c>
-      <c r="O13" s="47"/>
-      <c r="Q13" s="26"/>
-      <c r="R13"/>
-    </row>
-    <row r="14" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="157"/>
-      <c r="B14" s="158"/>
-      <c r="C14" s="160"/>
+      <c r="P13" s="183">
+        <v>115</v>
+      </c>
+      <c r="R13" s="26"/>
+      <c r="S13"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="159"/>
+      <c r="B14" s="160"/>
+      <c r="C14" s="154"/>
       <c r="D14" s="48" t="s">
         <v>27</v>
       </c>
@@ -2988,16 +3411,23 @@
         <v>1</v>
       </c>
       <c r="K14" s="51"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="54"/>
-      <c r="R14"/>
-    </row>
-    <row r="15" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="157"/>
-      <c r="B15" s="158"/>
-      <c r="C15" s="160"/>
+      <c r="L14" s="52">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M14" s="168"/>
+      <c r="N14" s="48">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O14" s="53"/>
+      <c r="P14" s="184"/>
+      <c r="S14"/>
+    </row>
+    <row r="15" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="159"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="154"/>
       <c r="D15" s="55" t="s">
         <v>28</v>
       </c>
@@ -3013,16 +3443,23 @@
       <c r="I15" s="55"/>
       <c r="J15" s="55"/>
       <c r="K15" s="58"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="61"/>
-      <c r="R15"/>
-    </row>
-    <row r="16" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="157"/>
-      <c r="B16" s="158"/>
-      <c r="C16" s="160"/>
+      <c r="L15" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="169"/>
+      <c r="N15" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="60"/>
+      <c r="P15" s="185"/>
+      <c r="S15"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="159"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="154"/>
       <c r="D16" s="62" t="s">
         <v>29</v>
       </c>
@@ -3040,16 +3477,23 @@
       <c r="K16" s="65">
         <v>1</v>
       </c>
-      <c r="L16" s="66"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="68"/>
-      <c r="R16"/>
-    </row>
-    <row r="17" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="157"/>
-      <c r="B17" s="158"/>
-      <c r="C17" s="161" t="s">
+      <c r="L16" s="66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M16" s="170"/>
+      <c r="N16" s="62">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="67"/>
+      <c r="P16" s="186"/>
+      <c r="S16"/>
+    </row>
+    <row r="17" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="159"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="155" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="19" t="s">
@@ -3058,30 +3502,39 @@
       <c r="E17" s="69">
         <v>7</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="194">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19">
-        <v>1</v>
-      </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="24">
+      <c r="G17" s="195"/>
+      <c r="H17" s="195"/>
+      <c r="I17" s="195">
+        <v>1</v>
+      </c>
+      <c r="J17" s="195"/>
+      <c r="K17" s="196"/>
+      <c r="L17" s="164">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M17" s="164"/>
+      <c r="N17" s="19">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O17" s="24">
         <f>50.08-(50.08*10/100)</f>
         <v>45.072000000000003</v>
       </c>
-      <c r="O17" s="25"/>
-      <c r="R17"/>
-    </row>
-    <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="157"/>
-      <c r="B18" s="158"/>
-      <c r="C18" s="161"/>
+      <c r="P17" s="203">
+        <v>105</v>
+      </c>
+      <c r="S17"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="159"/>
+      <c r="B18" s="160"/>
+      <c r="C18" s="155"/>
       <c r="D18" s="70" t="s">
         <v>27</v>
       </c>
@@ -3092,23 +3545,30 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27">
         <v>2</v>
       </c>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="74"/>
-      <c r="O18" s="75"/>
-      <c r="R18"/>
-    </row>
-    <row r="19" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="157"/>
-      <c r="B19" s="158"/>
-      <c r="C19" s="161"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="165">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O18" s="27"/>
+      <c r="P18" s="33"/>
+      <c r="S18"/>
+    </row>
+    <row r="19" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="159"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="155"/>
       <c r="D19" s="76" t="s">
         <v>28</v>
       </c>
@@ -3126,16 +3586,23 @@
         <v>1</v>
       </c>
       <c r="K19" s="78"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="76"/>
-      <c r="N19" s="80"/>
-      <c r="O19" s="81"/>
-      <c r="R19"/>
-    </row>
-    <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="157"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="161"/>
+      <c r="L19" s="171">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M19" s="171"/>
+      <c r="N19" s="76">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O19" s="80"/>
+      <c r="P19" s="187"/>
+      <c r="S19"/>
+    </row>
+    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="159"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="155"/>
       <c r="D20" s="82" t="s">
         <v>29</v>
       </c>
@@ -3146,487 +3613,610 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82">
+      <c r="G20" s="197"/>
+      <c r="H20" s="197"/>
+      <c r="I20" s="197"/>
+      <c r="J20" s="197">
         <v>2</v>
       </c>
-      <c r="K20" s="85">
+      <c r="K20" s="198">
         <v>2</v>
       </c>
-      <c r="L20" s="86"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="87"/>
-      <c r="O20" s="88"/>
-      <c r="R20"/>
-    </row>
-    <row r="21" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="157"/>
-      <c r="B21" s="162" t="s">
+      <c r="L20" s="165">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O20" s="27"/>
+      <c r="P20" s="204"/>
+      <c r="S20"/>
+    </row>
+    <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="159"/>
+      <c r="B21" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="163" t="s">
+      <c r="C21" s="157" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="90">
+      <c r="E21" s="86">
         <v>5</v>
       </c>
-      <c r="F21" s="91">
+      <c r="F21" s="87">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G21" s="89">
+      <c r="G21" s="85">
         <v>2</v>
       </c>
-      <c r="H21" s="89"/>
-      <c r="I21" s="89"/>
-      <c r="J21" s="89"/>
-      <c r="K21" s="92"/>
-      <c r="L21" s="93"/>
-      <c r="M21" s="89"/>
-      <c r="N21" s="94">
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="89">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M21" s="172"/>
+      <c r="N21" s="85">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="O21" s="90">
         <f>48.02-(48.02*10/100)</f>
         <v>43.218000000000004</v>
       </c>
-      <c r="O21" s="95"/>
-      <c r="R21"/>
-    </row>
-    <row r="22" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="157"/>
-      <c r="B22" s="162"/>
-      <c r="C22" s="163"/>
-      <c r="D22" s="96" t="s">
+      <c r="P21" s="188">
+        <v>105</v>
+      </c>
+      <c r="S21"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="159"/>
+      <c r="B22" s="156"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="97">
+      <c r="E22" s="93">
         <v>5</v>
       </c>
-      <c r="F22" s="98">
+      <c r="F22" s="94">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96">
-        <v>1</v>
-      </c>
-      <c r="J22" s="96"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="100"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="102"/>
-      <c r="R22"/>
-    </row>
-    <row r="23" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="157"/>
-      <c r="B23" s="162"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="103" t="s">
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92">
+        <v>1</v>
+      </c>
+      <c r="J22" s="92"/>
+      <c r="K22" s="95"/>
+      <c r="L22" s="96">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M22" s="173"/>
+      <c r="N22" s="92">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O22" s="97"/>
+      <c r="P22" s="189"/>
+      <c r="S22"/>
+    </row>
+    <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="159"/>
+      <c r="B23" s="156"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="104">
+      <c r="E23" s="100">
         <v>5</v>
       </c>
-      <c r="F23" s="105">
+      <c r="F23" s="101">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G23" s="99">
+        <v>1</v>
+      </c>
+      <c r="H23" s="99">
+        <v>1</v>
+      </c>
+      <c r="I23" s="99">
+        <v>1</v>
+      </c>
+      <c r="J23" s="99"/>
+      <c r="K23" s="102"/>
+      <c r="L23" s="103">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M23" s="174"/>
+      <c r="N23" s="99">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O23" s="104"/>
+      <c r="P23" s="190"/>
+      <c r="S23"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="159"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="93">
+        <v>3</v>
+      </c>
+      <c r="F24" s="94">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="92">
+        <v>1</v>
+      </c>
+      <c r="K24" s="95"/>
+      <c r="L24" s="96">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M24" s="173"/>
+      <c r="N24" s="92">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O24" s="97"/>
+      <c r="P24" s="189"/>
+      <c r="S24"/>
+    </row>
+    <row r="25" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="159"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="157"/>
+      <c r="D25" s="106" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="107">
+        <v>2</v>
+      </c>
+      <c r="F25" s="108">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="106"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="106">
+        <v>1</v>
+      </c>
+      <c r="K25" s="109"/>
+      <c r="L25" s="110">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M25" s="175"/>
+      <c r="N25" s="106">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O25" s="111"/>
+      <c r="P25" s="191"/>
+      <c r="S25"/>
+    </row>
+    <row r="26" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="159"/>
+      <c r="B26" s="156"/>
+      <c r="C26" s="162" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="86">
+        <v>3</v>
+      </c>
+      <c r="F26" s="87">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G26" s="85">
+        <v>1</v>
+      </c>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="89">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M26" s="172"/>
+      <c r="N26" s="85">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O26" s="90">
+        <f>54.85-(54.85*10/100)</f>
+        <v>49.365000000000002</v>
+      </c>
+      <c r="P26" s="188">
+        <v>115</v>
+      </c>
+      <c r="S26"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="159"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="162"/>
+      <c r="D27" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="93">
+        <v>3</v>
+      </c>
+      <c r="F27" s="94">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G27" s="92"/>
+      <c r="H27" s="92"/>
+      <c r="I27" s="92">
+        <v>1</v>
+      </c>
+      <c r="J27" s="92"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="96">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M27" s="173"/>
+      <c r="N27" s="92">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O27" s="97"/>
+      <c r="P27" s="189"/>
+      <c r="S27"/>
+    </row>
+    <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="159"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="162"/>
+      <c r="D28" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="100">
+        <v>3</v>
+      </c>
+      <c r="F28" s="101">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G28" s="99"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="99">
+        <v>1</v>
+      </c>
+      <c r="J28" s="99"/>
+      <c r="K28" s="102"/>
+      <c r="L28" s="103">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M28" s="174"/>
+      <c r="N28" s="99">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O28" s="104"/>
+      <c r="P28" s="190"/>
+      <c r="S28"/>
+    </row>
+    <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="159"/>
+      <c r="B29" s="156"/>
+      <c r="C29" s="162"/>
+      <c r="D29" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="93">
+        <v>1</v>
+      </c>
+      <c r="F29" s="94">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G29" s="92"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="92"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="96">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M29" s="173"/>
+      <c r="N29" s="92">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O29" s="97"/>
+      <c r="P29" s="189"/>
+      <c r="S29"/>
+    </row>
+    <row r="30" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="159"/>
+      <c r="B30" s="156"/>
+      <c r="C30" s="162"/>
+      <c r="D30" s="113" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="114">
+        <v>0</v>
+      </c>
+      <c r="F30" s="115">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="113"/>
+      <c r="H30" s="113"/>
+      <c r="I30" s="113"/>
+      <c r="J30" s="113"/>
+      <c r="K30" s="116"/>
+      <c r="L30" s="117">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="176"/>
+      <c r="N30" s="113">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="118"/>
+      <c r="P30" s="192"/>
+      <c r="S30"/>
+    </row>
+    <row r="31" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="159"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="163" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="86">
+        <v>7</v>
+      </c>
+      <c r="F31" s="101">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G31" s="99">
+        <v>2</v>
+      </c>
+      <c r="H31" s="99"/>
+      <c r="I31" s="99"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="102"/>
+      <c r="L31" s="103">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="M31" s="174"/>
+      <c r="N31" s="99">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O31" s="104">
+        <f>38.88-(38.88*10/100)</f>
+        <v>34.992000000000004</v>
+      </c>
+      <c r="P31" s="190">
+        <v>95</v>
+      </c>
+      <c r="S31"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="159"/>
+      <c r="B32" s="156"/>
+      <c r="C32" s="163"/>
+      <c r="D32" s="92" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="93">
+        <v>6</v>
+      </c>
+      <c r="F32" s="94">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G32" s="92">
+        <v>1</v>
+      </c>
+      <c r="H32" s="92">
+        <v>1</v>
+      </c>
+      <c r="I32" s="92">
+        <v>2</v>
+      </c>
+      <c r="J32" s="92"/>
+      <c r="K32" s="95"/>
+      <c r="L32" s="96">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M32" s="173"/>
+      <c r="N32" s="92">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O32" s="97"/>
+      <c r="P32" s="189"/>
+      <c r="S32"/>
+    </row>
+    <row r="33" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="159"/>
+      <c r="B33" s="156"/>
+      <c r="C33" s="163"/>
+      <c r="D33" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="100">
+        <v>4</v>
+      </c>
+      <c r="F33" s="101">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G23" s="103">
-        <v>1</v>
-      </c>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103">
-        <v>1</v>
-      </c>
-      <c r="J23" s="103"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="107"/>
-      <c r="M23" s="103"/>
-      <c r="N23" s="108"/>
-      <c r="O23" s="109"/>
-      <c r="R23"/>
-    </row>
-    <row r="24" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="157"/>
-      <c r="B24" s="162"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="97">
+      <c r="G33" s="99"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="99">
+        <v>1</v>
+      </c>
+      <c r="K33" s="102"/>
+      <c r="L33" s="103">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F24" s="98">
+      <c r="M33" s="174"/>
+      <c r="N33" s="99">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="O33" s="104"/>
+      <c r="P33" s="190"/>
+      <c r="S33"/>
+    </row>
+    <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="159"/>
+      <c r="B34" s="156"/>
+      <c r="C34" s="163"/>
+      <c r="D34" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="93">
+        <v>2</v>
+      </c>
+      <c r="F34" s="94">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G34" s="92"/>
+      <c r="H34" s="92"/>
+      <c r="I34" s="92"/>
+      <c r="J34" s="92">
+        <v>1</v>
+      </c>
+      <c r="K34" s="95"/>
+      <c r="L34" s="96">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M34" s="173"/>
+      <c r="N34" s="92">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O34" s="97"/>
+      <c r="P34" s="189"/>
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="159"/>
+      <c r="B35" s="156"/>
+      <c r="C35" s="163"/>
+      <c r="D35" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="120">
+        <v>1</v>
+      </c>
+      <c r="F35" s="121">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G35" s="119"/>
+      <c r="H35" s="119"/>
+      <c r="I35" s="119"/>
+      <c r="J35" s="119"/>
+      <c r="K35" s="122"/>
+      <c r="L35" s="123">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M35" s="177"/>
+      <c r="N35" s="119">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O35" s="124"/>
+      <c r="P35" s="193"/>
+      <c r="S35"/>
+    </row>
+    <row r="36" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="151" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="152" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="153" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="126" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="127">
+        <v>10</v>
+      </c>
+      <c r="F36" s="128">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G36" s="126">
+        <v>1</v>
+      </c>
+      <c r="H36" s="126">
         <v>2</v>
       </c>
-      <c r="G24" s="96"/>
-      <c r="H24" s="96"/>
-      <c r="I24" s="96"/>
-      <c r="J24" s="96">
-        <v>1</v>
-      </c>
-      <c r="K24" s="99"/>
-      <c r="L24" s="100"/>
-      <c r="M24" s="96"/>
-      <c r="N24" s="101"/>
-      <c r="O24" s="102"/>
-      <c r="R24"/>
-    </row>
-    <row r="25" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="157"/>
-      <c r="B25" s="162"/>
-      <c r="C25" s="163"/>
-      <c r="D25" s="110" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="111">
+      <c r="I36" s="126">
         <v>2</v>
       </c>
-      <c r="F25" s="112">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="110">
-        <v>1</v>
-      </c>
-      <c r="K25" s="113"/>
-      <c r="L25" s="114"/>
-      <c r="M25" s="110"/>
-      <c r="N25" s="115"/>
-      <c r="O25" s="116"/>
-      <c r="R25"/>
-    </row>
-    <row r="26" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="157"/>
-      <c r="B26" s="162"/>
-      <c r="C26" s="164" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="89" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="90">
-        <v>3</v>
-      </c>
-      <c r="F26" s="91">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G26" s="89">
-        <v>1</v>
-      </c>
-      <c r="H26" s="89"/>
-      <c r="I26" s="89"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="93"/>
-      <c r="M26" s="89"/>
-      <c r="N26" s="94">
-        <f>54.85-(54.85*10/100)</f>
-        <v>49.365000000000002</v>
-      </c>
-      <c r="O26" s="95"/>
-      <c r="R26"/>
-    </row>
-    <row r="27" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="157"/>
-      <c r="B27" s="162"/>
-      <c r="C27" s="164"/>
-      <c r="D27" s="96" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="97">
-        <v>3</v>
-      </c>
-      <c r="F27" s="98">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G27" s="96"/>
-      <c r="H27" s="96"/>
-      <c r="I27" s="96">
-        <v>1</v>
-      </c>
-      <c r="J27" s="96"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="100"/>
-      <c r="M27" s="96"/>
-      <c r="N27" s="101"/>
-      <c r="O27" s="102"/>
-      <c r="R27"/>
-    </row>
-    <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="157"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="103" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="104">
-        <v>3</v>
-      </c>
-      <c r="F28" s="105">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G28" s="103"/>
-      <c r="H28" s="103"/>
-      <c r="I28" s="103">
-        <v>1</v>
-      </c>
-      <c r="J28" s="103"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="103"/>
-      <c r="N28" s="108"/>
-      <c r="O28" s="109"/>
-      <c r="R28"/>
-    </row>
-    <row r="29" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="157"/>
-      <c r="B29" s="162"/>
-      <c r="C29" s="164"/>
-      <c r="D29" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="97">
-        <v>1</v>
-      </c>
-      <c r="F29" s="98">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G29" s="96"/>
-      <c r="H29" s="96"/>
-      <c r="I29" s="96"/>
-      <c r="J29" s="96"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="100"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="101"/>
-      <c r="O29" s="102"/>
-      <c r="R29"/>
-    </row>
-    <row r="30" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="157"/>
-      <c r="B30" s="162"/>
-      <c r="C30" s="164"/>
-      <c r="D30" s="117" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="118">
-        <v>0</v>
-      </c>
-      <c r="F30" s="119">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="117"/>
-      <c r="H30" s="117"/>
-      <c r="I30" s="117"/>
-      <c r="J30" s="117"/>
-      <c r="K30" s="120"/>
-      <c r="L30" s="121"/>
-      <c r="M30" s="117"/>
-      <c r="N30" s="122"/>
-      <c r="O30" s="123"/>
-      <c r="R30"/>
-    </row>
-    <row r="31" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="157"/>
-      <c r="B31" s="162"/>
-      <c r="C31" s="165" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="89" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="90">
-        <v>7</v>
-      </c>
-      <c r="F31" s="105">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G31" s="103">
-        <v>2</v>
-      </c>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="106"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="103"/>
-      <c r="N31" s="108">
-        <f>38.88-(38.88*10/100)</f>
-        <v>34.992000000000004</v>
-      </c>
-      <c r="O31" s="109"/>
-      <c r="R31"/>
-    </row>
-    <row r="32" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="157"/>
-      <c r="B32" s="162"/>
-      <c r="C32" s="165"/>
-      <c r="D32" s="96" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="97">
-        <v>6</v>
-      </c>
-      <c r="F32" s="98">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G32" s="96">
-        <v>1</v>
-      </c>
-      <c r="H32" s="96"/>
-      <c r="I32" s="96">
-        <v>2</v>
-      </c>
-      <c r="J32" s="96"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="100"/>
-      <c r="M32" s="96"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="102"/>
-      <c r="R32"/>
-    </row>
-    <row r="33" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="157"/>
-      <c r="B33" s="162"/>
-      <c r="C33" s="165"/>
-      <c r="D33" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="104">
-        <v>4</v>
-      </c>
-      <c r="F33" s="105">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G33" s="103"/>
-      <c r="H33" s="103"/>
-      <c r="I33" s="103"/>
-      <c r="J33" s="103">
-        <v>1</v>
-      </c>
-      <c r="K33" s="106"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="103"/>
-      <c r="N33" s="108"/>
-      <c r="O33" s="109"/>
-      <c r="R33"/>
-    </row>
-    <row r="34" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="157"/>
-      <c r="B34" s="162"/>
-      <c r="C34" s="165"/>
-      <c r="D34" s="96" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="97">
-        <v>2</v>
-      </c>
-      <c r="F34" s="98">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G34" s="96"/>
-      <c r="H34" s="96"/>
-      <c r="I34" s="96"/>
-      <c r="J34" s="96">
-        <v>1</v>
-      </c>
-      <c r="K34" s="99"/>
-      <c r="L34" s="100"/>
-      <c r="M34" s="96"/>
-      <c r="N34" s="101"/>
-      <c r="O34" s="102"/>
-      <c r="R34"/>
-    </row>
-    <row r="35" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="157"/>
-      <c r="B35" s="162"/>
-      <c r="C35" s="165"/>
-      <c r="D35" s="124" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="125">
-        <v>1</v>
-      </c>
-      <c r="F35" s="126">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G35" s="124"/>
-      <c r="H35" s="124"/>
-      <c r="I35" s="124"/>
-      <c r="J35" s="124"/>
-      <c r="K35" s="127"/>
-      <c r="L35" s="128"/>
-      <c r="M35" s="124"/>
-      <c r="N35" s="129"/>
-      <c r="O35" s="130"/>
-      <c r="R35"/>
-    </row>
-    <row r="36" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="167" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="168" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="169" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="131" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="132">
-        <v>10</v>
-      </c>
-      <c r="F36" s="133">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G36" s="131">
-        <v>1</v>
-      </c>
-      <c r="H36" s="131">
-        <v>2</v>
-      </c>
-      <c r="I36" s="131">
-        <v>1</v>
-      </c>
-      <c r="J36" s="131">
-        <v>1</v>
-      </c>
-      <c r="K36" s="134"/>
-      <c r="L36" s="135"/>
-      <c r="M36" s="131"/>
-      <c r="N36" s="136">
+      <c r="J36" s="126">
+        <v>1</v>
+      </c>
+      <c r="K36" s="129"/>
+      <c r="L36" s="130"/>
+      <c r="M36" s="178"/>
+      <c r="N36" s="126"/>
+      <c r="O36" s="131">
         <f>49.18-(49.18*10/100)</f>
         <v>44.262</v>
       </c>
-      <c r="O36" s="137"/>
-      <c r="R36"/>
-    </row>
-    <row r="37" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="167"/>
-      <c r="B37" s="168"/>
-      <c r="C37" s="169"/>
+      <c r="P36" s="132"/>
+      <c r="S36"/>
+    </row>
+    <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="151"/>
+      <c r="B37" s="152"/>
+      <c r="C37" s="153"/>
       <c r="D37" s="27" t="s">
         <v>27</v>
       </c>
@@ -3647,15 +4237,16 @@
       </c>
       <c r="K37" s="30"/>
       <c r="L37" s="31"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="33"/>
-      <c r="R37"/>
-    </row>
-    <row r="38" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="167"/>
-      <c r="B38" s="168"/>
-      <c r="C38" s="169"/>
+      <c r="M37" s="165"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="33"/>
+      <c r="S37"/>
+    </row>
+    <row r="38" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="151"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="153"/>
       <c r="D38" s="19" t="s">
         <v>28</v>
       </c>
@@ -3672,15 +4263,16 @@
       <c r="J38" s="19"/>
       <c r="K38" s="22"/>
       <c r="L38" s="23"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="25"/>
-      <c r="R38"/>
-    </row>
-    <row r="39" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="167"/>
-      <c r="B39" s="168"/>
-      <c r="C39" s="169"/>
+      <c r="M38" s="164"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="25"/>
+      <c r="S38"/>
+    </row>
+    <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="151"/>
+      <c r="B39" s="152"/>
+      <c r="C39" s="153"/>
       <c r="D39" s="34" t="s">
         <v>29</v>
       </c>
@@ -3699,15 +4291,16 @@
         <v>2</v>
       </c>
       <c r="L39" s="38"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="39"/>
-      <c r="O39" s="40"/>
-      <c r="R39"/>
-    </row>
-    <row r="40" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="167"/>
-      <c r="B40" s="168"/>
-      <c r="C40" s="160" t="s">
+      <c r="M39" s="166"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="40"/>
+      <c r="S39"/>
+    </row>
+    <row r="40" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="151"/>
+      <c r="B40" s="152"/>
+      <c r="C40" s="154" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="41" t="s">
@@ -3728,18 +4321,19 @@
       <c r="J40" s="41"/>
       <c r="K40" s="44"/>
       <c r="L40" s="45"/>
-      <c r="M40" s="41"/>
-      <c r="N40" s="46">
+      <c r="M40" s="167"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="46">
         <f>56.01-(56.01*10/100)</f>
         <v>50.408999999999999</v>
       </c>
-      <c r="O40" s="47"/>
-      <c r="R40"/>
-    </row>
-    <row r="41" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="167"/>
-      <c r="B41" s="168"/>
-      <c r="C41" s="160"/>
+      <c r="P40" s="47"/>
+      <c r="S40"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="151"/>
+      <c r="B41" s="152"/>
+      <c r="C41" s="154"/>
       <c r="D41" s="48" t="s">
         <v>27</v>
       </c>
@@ -3747,7 +4341,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="50">
-        <f t="shared" ref="F41:F60" si="1">E41-G41-H41-I41-J41-K41</f>
+        <f t="shared" ref="F41:F60" si="3">E41-G41-H41-I41-J41-K41</f>
         <v>2</v>
       </c>
       <c r="G41" s="48"/>
@@ -3760,15 +4354,16 @@
       </c>
       <c r="K41" s="51"/>
       <c r="L41" s="52"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="53"/>
-      <c r="O41" s="54"/>
-      <c r="R41"/>
-    </row>
-    <row r="42" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="167"/>
-      <c r="B42" s="168"/>
-      <c r="C42" s="160"/>
+      <c r="M41" s="168"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="54"/>
+      <c r="S41"/>
+    </row>
+    <row r="42" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="151"/>
+      <c r="B42" s="152"/>
+      <c r="C42" s="154"/>
       <c r="D42" s="55" t="s">
         <v>28</v>
       </c>
@@ -3776,7 +4371,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G42" s="55"/>
@@ -3785,15 +4380,16 @@
       <c r="J42" s="55"/>
       <c r="K42" s="58"/>
       <c r="L42" s="59"/>
-      <c r="M42" s="55"/>
-      <c r="N42" s="60"/>
-      <c r="O42" s="61"/>
-      <c r="R42"/>
-    </row>
-    <row r="43" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="167"/>
-      <c r="B43" s="168"/>
-      <c r="C43" s="160"/>
+      <c r="M42" s="169"/>
+      <c r="N42" s="55"/>
+      <c r="O42" s="60"/>
+      <c r="P42" s="61"/>
+      <c r="S42"/>
+    </row>
+    <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="151"/>
+      <c r="B43" s="152"/>
+      <c r="C43" s="154"/>
       <c r="D43" s="62" t="s">
         <v>29</v>
       </c>
@@ -3801,7 +4397,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G43" s="62"/>
@@ -3812,15 +4408,16 @@
         <v>1</v>
       </c>
       <c r="L43" s="66"/>
-      <c r="M43" s="62"/>
-      <c r="N43" s="67"/>
-      <c r="O43" s="68"/>
-      <c r="R43"/>
-    </row>
-    <row r="44" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="167"/>
-      <c r="B44" s="168"/>
-      <c r="C44" s="161" t="s">
+      <c r="M43" s="170"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="67"/>
+      <c r="P43" s="68"/>
+      <c r="S43"/>
+    </row>
+    <row r="44" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="151"/>
+      <c r="B44" s="152"/>
+      <c r="C44" s="155" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="19" t="s">
@@ -3830,33 +4427,32 @@
         <v>3</v>
       </c>
       <c r="F44" s="21">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="G44" s="19">
         <v>2</v>
       </c>
       <c r="H44" s="19"/>
-      <c r="I44" s="19">
-        <v>1</v>
-      </c>
+      <c r="I44" s="19"/>
       <c r="J44" s="19">
         <v>1</v>
       </c>
       <c r="K44" s="22"/>
       <c r="L44" s="23"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="24">
+      <c r="M44" s="164"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="24">
         <f>50.08-(50.08*10/100)</f>
         <v>45.072000000000003</v>
       </c>
-      <c r="O44" s="25"/>
-      <c r="R44"/>
-    </row>
-    <row r="45" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="167"/>
-      <c r="B45" s="168"/>
-      <c r="C45" s="161"/>
+      <c r="P44" s="25"/>
+      <c r="S44"/>
+    </row>
+    <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="151"/>
+      <c r="B45" s="152"/>
+      <c r="C45" s="155"/>
       <c r="D45" s="70" t="s">
         <v>26</v>
       </c>
@@ -3864,28 +4460,31 @@
         <v>8</v>
       </c>
       <c r="F45" s="29">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G45" s="70">
         <v>1</v>
       </c>
       <c r="H45" s="70"/>
-      <c r="I45" s="70"/>
+      <c r="I45" s="70">
+        <v>2</v>
+      </c>
       <c r="J45" s="70">
         <v>1</v>
       </c>
       <c r="K45" s="72"/>
       <c r="L45" s="73"/>
       <c r="M45" s="70"/>
-      <c r="N45" s="74"/>
-      <c r="O45" s="75"/>
-      <c r="R45"/>
-    </row>
-    <row r="46" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="167"/>
-      <c r="B46" s="168"/>
-      <c r="C46" s="161"/>
+      <c r="N45" s="70"/>
+      <c r="O45" s="74"/>
+      <c r="P45" s="75"/>
+      <c r="S45"/>
+    </row>
+    <row r="46" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="151"/>
+      <c r="B46" s="152"/>
+      <c r="C46" s="155"/>
       <c r="D46" s="76" t="s">
         <v>27</v>
       </c>
@@ -3893,7 +4492,7 @@
         <v>13</v>
       </c>
       <c r="F46" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G46" s="76"/>
@@ -3906,15 +4505,16 @@
       </c>
       <c r="K46" s="78"/>
       <c r="L46" s="79"/>
-      <c r="M46" s="76"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="81"/>
-      <c r="R46"/>
-    </row>
-    <row r="47" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="167"/>
-      <c r="B47" s="168"/>
-      <c r="C47" s="161"/>
+      <c r="M46" s="171"/>
+      <c r="N46" s="76"/>
+      <c r="O46" s="80"/>
+      <c r="P46" s="81"/>
+      <c r="S46"/>
+    </row>
+    <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="151"/>
+      <c r="B47" s="152"/>
+      <c r="C47" s="155"/>
       <c r="D47" s="70" t="s">
         <v>28</v>
       </c>
@@ -3922,7 +4522,7 @@
         <v>7</v>
       </c>
       <c r="F47" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G47" s="70"/>
@@ -3934,14 +4534,15 @@
       <c r="K47" s="72"/>
       <c r="L47" s="73"/>
       <c r="M47" s="70"/>
-      <c r="N47" s="74"/>
-      <c r="O47" s="75"/>
-      <c r="R47"/>
-    </row>
-    <row r="48" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="167"/>
-      <c r="B48" s="168"/>
-      <c r="C48" s="161"/>
+      <c r="N47" s="70"/>
+      <c r="O47" s="74"/>
+      <c r="P47" s="75"/>
+      <c r="S47"/>
+    </row>
+    <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="151"/>
+      <c r="B48" s="152"/>
+      <c r="C48" s="155"/>
       <c r="D48" s="76" t="s">
         <v>29</v>
       </c>
@@ -3949,7 +4550,7 @@
         <v>7</v>
       </c>
       <c r="F48" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G48" s="76"/>
@@ -3962,358 +4563,371 @@
         <v>2</v>
       </c>
       <c r="L48" s="79"/>
-      <c r="M48" s="76"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="81"/>
-      <c r="R48"/>
-    </row>
-    <row r="49" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="167"/>
-      <c r="B49" s="162" t="s">
+      <c r="M48" s="171"/>
+      <c r="N48" s="76"/>
+      <c r="O48" s="80"/>
+      <c r="P48" s="81"/>
+      <c r="S48"/>
+    </row>
+    <row r="49" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="151"/>
+      <c r="B49" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="163" t="s">
+      <c r="C49" s="157" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="89" t="s">
+      <c r="D49" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="90">
+      <c r="E49" s="86">
         <v>4</v>
       </c>
-      <c r="F49" s="91">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G49" s="89">
+      <c r="F49" s="87">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G49" s="85">
         <v>2</v>
       </c>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89"/>
-      <c r="J49" s="89">
-        <v>1</v>
-      </c>
-      <c r="K49" s="92"/>
-      <c r="L49" s="93"/>
-      <c r="M49" s="89"/>
-      <c r="N49" s="94">
+      <c r="H49" s="85"/>
+      <c r="I49" s="85"/>
+      <c r="J49" s="85">
+        <v>1</v>
+      </c>
+      <c r="K49" s="88"/>
+      <c r="L49" s="89"/>
+      <c r="M49" s="172"/>
+      <c r="N49" s="85"/>
+      <c r="O49" s="90">
         <f>48.02-(48.02*10/100)</f>
         <v>43.218000000000004</v>
       </c>
-      <c r="O49" s="95"/>
-      <c r="R49"/>
-    </row>
-    <row r="50" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A50" s="167"/>
-      <c r="B50" s="162"/>
-      <c r="C50" s="163"/>
-      <c r="D50" s="96" t="s">
+      <c r="P49" s="91"/>
+      <c r="S49"/>
+    </row>
+    <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="151"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="157"/>
+      <c r="D50" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="97">
+      <c r="E50" s="93">
         <v>5</v>
       </c>
-      <c r="F50" s="98">
-        <f t="shared" si="1"/>
+      <c r="F50" s="94">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G50" s="96"/>
-      <c r="H50" s="96"/>
-      <c r="I50" s="96"/>
-      <c r="J50" s="96">
-        <v>1</v>
-      </c>
-      <c r="K50" s="99"/>
-      <c r="L50" s="100"/>
-      <c r="M50" s="96"/>
-      <c r="N50" s="101"/>
-      <c r="O50" s="102"/>
-      <c r="R50"/>
-    </row>
-    <row r="51" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="167"/>
-      <c r="B51" s="162"/>
-      <c r="C51" s="163"/>
-      <c r="D51" s="103" t="s">
+      <c r="G50" s="92"/>
+      <c r="H50" s="92"/>
+      <c r="I50" s="92"/>
+      <c r="J50" s="92">
+        <v>1</v>
+      </c>
+      <c r="K50" s="95"/>
+      <c r="L50" s="96"/>
+      <c r="M50" s="173"/>
+      <c r="N50" s="92"/>
+      <c r="O50" s="97"/>
+      <c r="P50" s="98"/>
+      <c r="S50"/>
+    </row>
+    <row r="51" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="151"/>
+      <c r="B51" s="156"/>
+      <c r="C51" s="157"/>
+      <c r="D51" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="104">
-        <v>1</v>
-      </c>
-      <c r="F51" s="105">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G51" s="103"/>
-      <c r="H51" s="103"/>
-      <c r="I51" s="103"/>
-      <c r="J51" s="103"/>
-      <c r="K51" s="106"/>
-      <c r="L51" s="107"/>
-      <c r="M51" s="103"/>
-      <c r="N51" s="108"/>
-      <c r="O51" s="109"/>
-      <c r="R51"/>
-    </row>
-    <row r="52" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A52" s="167"/>
-      <c r="B52" s="162"/>
-      <c r="C52" s="163"/>
-      <c r="D52" s="96" t="s">
+      <c r="E51" s="100">
+        <v>1</v>
+      </c>
+      <c r="F51" s="101">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G51" s="99"/>
+      <c r="H51" s="99"/>
+      <c r="I51" s="99"/>
+      <c r="J51" s="99"/>
+      <c r="K51" s="102"/>
+      <c r="L51" s="103"/>
+      <c r="M51" s="174"/>
+      <c r="N51" s="99"/>
+      <c r="O51" s="104"/>
+      <c r="P51" s="105"/>
+      <c r="S51"/>
+    </row>
+    <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="151"/>
+      <c r="B52" s="156"/>
+      <c r="C52" s="157"/>
+      <c r="D52" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="97">
+      <c r="E52" s="93">
         <v>0</v>
       </c>
-      <c r="F52" s="98">
-        <f t="shared" si="1"/>
+      <c r="F52" s="94">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G52" s="96"/>
-      <c r="H52" s="96"/>
-      <c r="I52" s="96"/>
-      <c r="J52" s="96"/>
-      <c r="K52" s="99"/>
-      <c r="L52" s="100"/>
-      <c r="M52" s="96"/>
-      <c r="N52" s="101"/>
-      <c r="O52" s="102"/>
-      <c r="R52"/>
-    </row>
-    <row r="53" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="167"/>
-      <c r="B53" s="162"/>
-      <c r="C53" s="163"/>
-      <c r="D53" s="110" t="s">
+      <c r="G52" s="92"/>
+      <c r="H52" s="92"/>
+      <c r="I52" s="92"/>
+      <c r="J52" s="92"/>
+      <c r="K52" s="95"/>
+      <c r="L52" s="96"/>
+      <c r="M52" s="173"/>
+      <c r="N52" s="92"/>
+      <c r="O52" s="97"/>
+      <c r="P52" s="98"/>
+      <c r="S52"/>
+    </row>
+    <row r="53" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="151"/>
+      <c r="B53" s="156"/>
+      <c r="C53" s="157"/>
+      <c r="D53" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="111">
+      <c r="E53" s="107">
         <v>0</v>
       </c>
-      <c r="F53" s="112">
-        <f t="shared" si="1"/>
+      <c r="F53" s="108">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G53" s="110"/>
-      <c r="H53" s="110"/>
-      <c r="I53" s="110"/>
-      <c r="J53" s="110"/>
-      <c r="K53" s="113"/>
-      <c r="L53" s="114"/>
-      <c r="M53" s="110"/>
-      <c r="N53" s="115"/>
-      <c r="O53" s="116"/>
-      <c r="R53"/>
-    </row>
-    <row r="54" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="167"/>
-      <c r="B54" s="162"/>
-      <c r="C54" s="170" t="s">
+      <c r="G53" s="106"/>
+      <c r="H53" s="106"/>
+      <c r="I53" s="106"/>
+      <c r="J53" s="106"/>
+      <c r="K53" s="109"/>
+      <c r="L53" s="110"/>
+      <c r="M53" s="175"/>
+      <c r="N53" s="106"/>
+      <c r="O53" s="111"/>
+      <c r="P53" s="112"/>
+      <c r="S53"/>
+    </row>
+    <row r="54" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="151"/>
+      <c r="B54" s="156"/>
+      <c r="C54" s="158" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="89" t="s">
+      <c r="D54" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="E54" s="90">
+      <c r="E54" s="86">
         <v>4</v>
       </c>
-      <c r="F54" s="91">
-        <f t="shared" si="1"/>
+      <c r="F54" s="87">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G54" s="89">
-        <v>1</v>
-      </c>
-      <c r="H54" s="89"/>
-      <c r="I54" s="89"/>
-      <c r="J54" s="89"/>
-      <c r="K54" s="92"/>
-      <c r="L54" s="93"/>
-      <c r="M54" s="89"/>
-      <c r="N54" s="94">
+      <c r="G54" s="85">
+        <v>1</v>
+      </c>
+      <c r="H54" s="85"/>
+      <c r="I54" s="85"/>
+      <c r="J54" s="85"/>
+      <c r="K54" s="88"/>
+      <c r="L54" s="89"/>
+      <c r="M54" s="172"/>
+      <c r="N54" s="85"/>
+      <c r="O54" s="90">
         <f>54.85-(54.85*10/100)</f>
         <v>49.365000000000002</v>
       </c>
-      <c r="O54" s="95"/>
-      <c r="R54"/>
-    </row>
-    <row r="55" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="167"/>
-      <c r="B55" s="162"/>
-      <c r="C55" s="170"/>
-      <c r="D55" s="96" t="s">
+      <c r="P54" s="91"/>
+      <c r="S54"/>
+    </row>
+    <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="151"/>
+      <c r="B55" s="156"/>
+      <c r="C55" s="158"/>
+      <c r="D55" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E55" s="97">
+      <c r="E55" s="93">
         <v>5</v>
       </c>
-      <c r="F55" s="98">
-        <f t="shared" si="1"/>
+      <c r="F55" s="94">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G55" s="96"/>
-      <c r="H55" s="96"/>
-      <c r="I55" s="96"/>
-      <c r="J55" s="96">
-        <v>1</v>
-      </c>
-      <c r="K55" s="99"/>
-      <c r="L55" s="100"/>
-      <c r="M55" s="96"/>
-      <c r="N55" s="101"/>
-      <c r="O55" s="102"/>
-      <c r="R55"/>
-    </row>
-    <row r="56" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A56" s="167"/>
-      <c r="B56" s="162"/>
-      <c r="C56" s="170"/>
-      <c r="D56" s="103" t="s">
+      <c r="G55" s="92"/>
+      <c r="H55" s="92"/>
+      <c r="I55" s="92"/>
+      <c r="J55" s="92">
+        <v>1</v>
+      </c>
+      <c r="K55" s="95"/>
+      <c r="L55" s="96"/>
+      <c r="M55" s="173"/>
+      <c r="N55" s="92"/>
+      <c r="O55" s="97"/>
+      <c r="P55" s="98"/>
+      <c r="S55"/>
+    </row>
+    <row r="56" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="151"/>
+      <c r="B56" s="156"/>
+      <c r="C56" s="158"/>
+      <c r="D56" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="104">
-        <v>1</v>
-      </c>
-      <c r="F56" s="105">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G56" s="103"/>
-      <c r="H56" s="103"/>
-      <c r="I56" s="103"/>
-      <c r="J56" s="103"/>
-      <c r="K56" s="106"/>
-      <c r="L56" s="107"/>
-      <c r="M56" s="103"/>
-      <c r="N56" s="108"/>
-      <c r="O56" s="109"/>
-      <c r="R56"/>
-    </row>
-    <row r="57" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A57" s="167"/>
-      <c r="B57" s="162"/>
-      <c r="C57" s="170"/>
-      <c r="D57" s="96" t="s">
+      <c r="E56" s="100">
+        <v>1</v>
+      </c>
+      <c r="F56" s="101">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G56" s="99"/>
+      <c r="H56" s="99"/>
+      <c r="I56" s="99"/>
+      <c r="J56" s="99"/>
+      <c r="K56" s="102"/>
+      <c r="L56" s="103"/>
+      <c r="M56" s="174"/>
+      <c r="N56" s="99"/>
+      <c r="O56" s="104"/>
+      <c r="P56" s="105"/>
+      <c r="S56"/>
+    </row>
+    <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="151"/>
+      <c r="B57" s="156"/>
+      <c r="C57" s="158"/>
+      <c r="D57" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E57" s="97">
+      <c r="E57" s="93">
         <v>0</v>
       </c>
-      <c r="F57" s="98">
-        <f t="shared" si="1"/>
+      <c r="F57" s="94">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G57" s="96"/>
-      <c r="H57" s="96"/>
-      <c r="I57" s="96"/>
-      <c r="J57" s="96"/>
-      <c r="K57" s="99"/>
-      <c r="L57" s="100"/>
-      <c r="M57" s="96"/>
-      <c r="N57" s="101"/>
-      <c r="O57" s="102"/>
-      <c r="R57"/>
-    </row>
-    <row r="58" spans="1:18" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="167"/>
-      <c r="B58" s="162"/>
-      <c r="C58" s="170"/>
-      <c r="D58" s="110" t="s">
+      <c r="G57" s="92"/>
+      <c r="H57" s="92"/>
+      <c r="I57" s="92"/>
+      <c r="J57" s="92"/>
+      <c r="K57" s="95"/>
+      <c r="L57" s="96"/>
+      <c r="M57" s="173"/>
+      <c r="N57" s="92"/>
+      <c r="O57" s="97"/>
+      <c r="P57" s="98"/>
+      <c r="S57"/>
+    </row>
+    <row r="58" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="151"/>
+      <c r="B58" s="156"/>
+      <c r="C58" s="205"/>
+      <c r="D58" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="E58" s="111">
+      <c r="E58" s="120">
         <v>0</v>
       </c>
-      <c r="F58" s="112">
-        <f t="shared" si="1"/>
+      <c r="F58" s="121">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G58" s="110"/>
-      <c r="H58" s="110"/>
-      <c r="I58" s="110"/>
-      <c r="J58" s="110"/>
-      <c r="K58" s="113"/>
-      <c r="L58" s="114"/>
-      <c r="M58" s="110"/>
-      <c r="N58" s="115"/>
-      <c r="O58" s="116"/>
-      <c r="R58"/>
-    </row>
-    <row r="59" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G58" s="119"/>
+      <c r="H58" s="119"/>
+      <c r="I58" s="119"/>
+      <c r="J58" s="119"/>
+      <c r="K58" s="122"/>
+      <c r="L58" s="123"/>
+      <c r="M58" s="177"/>
+      <c r="N58" s="119"/>
+      <c r="O58" s="124"/>
+      <c r="P58" s="125"/>
+      <c r="S58"/>
+    </row>
+    <row r="59" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59"/>
-      <c r="C59" s="166" t="s">
+      <c r="C59" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="D59" s="138" t="s">
+      <c r="D59" s="133" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="139">
+      <c r="E59" s="134">
         <v>36</v>
       </c>
-      <c r="F59" s="140">
-        <f t="shared" si="1"/>
+      <c r="F59" s="135">
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="G59" s="141">
+      <c r="G59" s="136">
         <v>2</v>
       </c>
-      <c r="H59" s="141"/>
-      <c r="I59" s="141">
+      <c r="H59" s="136"/>
+      <c r="I59" s="136">
         <v>10</v>
       </c>
-      <c r="J59" s="141">
+      <c r="J59" s="136">
         <v>2</v>
       </c>
-      <c r="K59" s="142"/>
-      <c r="L59" s="143"/>
-      <c r="M59" s="141"/>
-      <c r="N59" s="144">
+      <c r="K59" s="137"/>
+      <c r="L59" s="138"/>
+      <c r="M59" s="138"/>
+      <c r="N59" s="136"/>
+      <c r="O59" s="139">
         <v>4.6500000000000004</v>
       </c>
-      <c r="O59" s="145"/>
-      <c r="R59" s="26"/>
-    </row>
-    <row r="60" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P59" s="140"/>
+      <c r="S59" s="26"/>
+    </row>
+    <row r="60" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
-      <c r="C60" s="166"/>
-      <c r="D60" s="146" t="s">
+      <c r="C60" s="150"/>
+      <c r="D60" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="147">
+      <c r="E60" s="142">
         <v>64</v>
       </c>
-      <c r="F60" s="148">
-        <f t="shared" si="1"/>
+      <c r="F60" s="143">
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="G60" s="149"/>
-      <c r="H60" s="149">
+      <c r="G60" s="144"/>
+      <c r="H60" s="144">
         <v>5</v>
       </c>
-      <c r="I60" s="149"/>
-      <c r="J60" s="149">
+      <c r="I60" s="144"/>
+      <c r="J60" s="144">
         <v>8</v>
       </c>
-      <c r="K60" s="150">
+      <c r="K60" s="145">
         <v>2</v>
       </c>
-      <c r="L60" s="151"/>
-      <c r="M60" s="152"/>
-      <c r="N60" s="153"/>
-      <c r="O60" s="154"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L60" s="146"/>
+      <c r="M60" s="146"/>
+      <c r="N60" s="147"/>
+      <c r="O60" s="148"/>
+      <c r="P60" s="149"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -4345,6 +4959,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="A9:A35"/>
+    <mergeCell ref="B9:B20"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="B21:B35"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="C31:C35"/>
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="A36:A58"/>
     <mergeCell ref="B36:B48"/>
@@ -4354,22 +4980,10 @@
     <mergeCell ref="B49:B58"/>
     <mergeCell ref="C49:C53"/>
     <mergeCell ref="C54:C58"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="A9:A35"/>
-    <mergeCell ref="B9:B20"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B21:B35"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="C31:C35"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="65" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="92" firstPageNumber="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Inventarbestand aktualisiert; Bestellung Volker Laabs #1565
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -31,11 +31,83 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
     <author/>
-    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="G23" authorId="0" shapeId="0">
+    <comment ref="M10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Volker Laabs #1565</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Volker Laabs #1565</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Volker Laabs #1565</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G23" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="1" shapeId="0">
+    <comment ref="H23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G32" authorId="0" shapeId="0">
+    <comment ref="G32" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H32" authorId="1" shapeId="0">
+    <comment ref="H32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G36" authorId="0" shapeId="0">
+    <comment ref="G36" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I36" authorId="1" shapeId="0">
+    <comment ref="I36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G45" authorId="0" shapeId="0">
+    <comment ref="G45" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I45" authorId="1" shapeId="0">
+    <comment ref="I45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -370,8 +442,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00\ _€"/>
-    <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2218,6 +2290,159 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="72" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="74" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="75" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="77" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="80" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="81" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="10" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="10" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="11" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="13" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="11" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="13" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="16" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="49" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="52" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2230,164 +2455,11 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="74" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="75" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="77" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="80" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="81" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="10" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="10" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="13" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="13" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="15" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="16" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="15" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="15" borderId="49" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="15" borderId="52" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="15" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2980,8 +3052,8 @@
   <dimension ref="A1:IX69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3054,9 +3126,9 @@
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="205">
+      <c r="B4" s="186">
         <f ca="1">TODAY()</f>
-        <v>42699</v>
+        <v>42710</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -3116,30 +3188,30 @@
       <c r="S6"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="198" t="s">
+      <c r="A7" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="199"/>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="200" t="s">
+      <c r="B7" s="188"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="188"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="189" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="200"/>
-      <c r="H7" s="200"/>
-      <c r="I7" s="200"/>
-      <c r="J7" s="200"/>
-      <c r="K7" s="200"/>
-      <c r="L7" s="200" t="s">
+      <c r="G7" s="189"/>
+      <c r="H7" s="189"/>
+      <c r="I7" s="189"/>
+      <c r="J7" s="189"/>
+      <c r="K7" s="189"/>
+      <c r="L7" s="189" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="200"/>
-      <c r="N7" s="200" t="s">
+      <c r="M7" s="189"/>
+      <c r="N7" s="189" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="200"/>
-      <c r="P7" s="201"/>
+      <c r="O7" s="189"/>
+      <c r="P7" s="190"/>
       <c r="R7"/>
       <c r="S7"/>
     </row>
@@ -3177,10 +3249,10 @@
       <c r="K8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="178" t="s">
+      <c r="L8" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="M8" s="178" t="s">
+      <c r="M8" s="164" t="s">
         <v>19</v>
       </c>
       <c r="N8" s="16" t="s">
@@ -3196,13 +3268,13 @@
       <c r="S8"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="158" t="s">
+      <c r="A9" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="159" t="s">
+      <c r="B9" s="192" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="160" t="s">
+      <c r="C9" s="193" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -3228,7 +3300,7 @@
         <f>F9</f>
         <v>11</v>
       </c>
-      <c r="M9" s="163"/>
+      <c r="M9" s="149"/>
       <c r="N9" s="18">
         <f>L9-M9</f>
         <v>11</v>
@@ -3237,16 +3309,16 @@
         <f>49.18-(49.18*10/100)</f>
         <v>44.262</v>
       </c>
-      <c r="P9" s="179">
+      <c r="P9" s="165">
         <v>105</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="158"/>
-      <c r="B10" s="159"/>
-      <c r="C10" s="160"/>
+      <c r="A10" s="191"/>
+      <c r="B10" s="192"/>
+      <c r="C10" s="193"/>
       <c r="D10" s="26" t="s">
         <v>27</v>
       </c>
@@ -3268,20 +3340,22 @@
         <f t="shared" ref="L10:L35" si="1">F10</f>
         <v>15</v>
       </c>
-      <c r="M10" s="164"/>
+      <c r="M10" s="150">
+        <v>1</v>
+      </c>
       <c r="N10" s="26">
         <f t="shared" ref="N10:N35" si="2">L10-M10</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O10" s="31"/>
-      <c r="P10" s="180"/>
+      <c r="P10" s="166"/>
       <c r="R10" s="25"/>
       <c r="S10"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="158"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="160"/>
+      <c r="A11" s="191"/>
+      <c r="B11" s="192"/>
+      <c r="C11" s="193"/>
       <c r="D11" s="18" t="s">
         <v>28</v>
       </c>
@@ -3301,20 +3375,20 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="M11" s="163"/>
+      <c r="M11" s="149"/>
       <c r="N11" s="18">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="O11" s="23"/>
-      <c r="P11" s="179"/>
+      <c r="P11" s="165"/>
       <c r="R11" s="25"/>
       <c r="S11"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="158"/>
-      <c r="B12" s="159"/>
-      <c r="C12" s="160"/>
+      <c r="A12" s="191"/>
+      <c r="B12" s="192"/>
+      <c r="C12" s="193"/>
       <c r="D12" s="33" t="s">
         <v>29</v>
       </c>
@@ -3336,20 +3410,20 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M12" s="165"/>
+      <c r="M12" s="151"/>
       <c r="N12" s="33">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O12" s="38"/>
-      <c r="P12" s="181"/>
+      <c r="P12" s="167"/>
       <c r="R12" s="25"/>
       <c r="S12"/>
     </row>
     <row r="13" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="158"/>
-      <c r="B13" s="159"/>
-      <c r="C13" s="153" t="s">
+      <c r="A13" s="191"/>
+      <c r="B13" s="192"/>
+      <c r="C13" s="194" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="40" t="s">
@@ -3373,7 +3447,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M13" s="166"/>
+      <c r="M13" s="152"/>
       <c r="N13" s="40">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -3382,16 +3456,16 @@
         <f>56.01-(56.01*10/100)</f>
         <v>50.408999999999999</v>
       </c>
-      <c r="P13" s="182">
+      <c r="P13" s="168">
         <v>115</v>
       </c>
       <c r="R13" s="25"/>
       <c r="S13"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="158"/>
-      <c r="B14" s="159"/>
-      <c r="C14" s="153"/>
+      <c r="A14" s="191"/>
+      <c r="B14" s="192"/>
+      <c r="C14" s="194"/>
       <c r="D14" s="47" t="s">
         <v>27</v>
       </c>
@@ -3415,19 +3489,21 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M14" s="167"/>
+      <c r="M14" s="153">
+        <v>1</v>
+      </c>
       <c r="N14" s="47">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14" s="52"/>
-      <c r="P14" s="183"/>
+      <c r="P14" s="169"/>
       <c r="S14"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="158"/>
-      <c r="B15" s="159"/>
-      <c r="C15" s="153"/>
+      <c r="A15" s="191"/>
+      <c r="B15" s="192"/>
+      <c r="C15" s="194"/>
       <c r="D15" s="54" t="s">
         <v>28</v>
       </c>
@@ -3447,19 +3523,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M15" s="168"/>
+      <c r="M15" s="154"/>
       <c r="N15" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O15" s="59"/>
-      <c r="P15" s="184"/>
+      <c r="P15" s="170"/>
       <c r="S15"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="158"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="153"/>
+      <c r="A16" s="191"/>
+      <c r="B16" s="192"/>
+      <c r="C16" s="194"/>
       <c r="D16" s="61" t="s">
         <v>29</v>
       </c>
@@ -3481,19 +3557,19 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M16" s="169"/>
+      <c r="M16" s="155"/>
       <c r="N16" s="61">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O16" s="66"/>
-      <c r="P16" s="185"/>
+      <c r="P16" s="171"/>
       <c r="S16"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="158"/>
-      <c r="B17" s="159"/>
-      <c r="C17" s="154" t="s">
+      <c r="A17" s="191"/>
+      <c r="B17" s="192"/>
+      <c r="C17" s="195" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -3502,22 +3578,22 @@
       <c r="E17" s="68">
         <v>7</v>
       </c>
-      <c r="F17" s="193">
+      <c r="F17" s="179">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G17" s="194"/>
-      <c r="H17" s="194"/>
-      <c r="I17" s="194">
-        <v>1</v>
-      </c>
-      <c r="J17" s="194"/>
-      <c r="K17" s="195"/>
-      <c r="L17" s="163">
+      <c r="G17" s="180"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="180">
+        <v>1</v>
+      </c>
+      <c r="J17" s="180"/>
+      <c r="K17" s="181"/>
+      <c r="L17" s="149">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M17" s="163"/>
+      <c r="M17" s="149"/>
       <c r="N17" s="18">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -3526,15 +3602,15 @@
         <f>50.08-(50.08*10/100)</f>
         <v>45.072000000000003</v>
       </c>
-      <c r="P17" s="202">
+      <c r="P17" s="184">
         <v>105</v>
       </c>
       <c r="S17"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="158"/>
-      <c r="B18" s="159"/>
-      <c r="C18" s="154"/>
+      <c r="A18" s="191"/>
+      <c r="B18" s="192"/>
+      <c r="C18" s="195"/>
       <c r="D18" s="69" t="s">
         <v>27</v>
       </c>
@@ -3552,23 +3628,25 @@
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="29"/>
-      <c r="L18" s="164">
+      <c r="L18" s="150">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="M18" s="26"/>
+      <c r="M18" s="26">
+        <v>1</v>
+      </c>
       <c r="N18" s="26">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O18" s="26"/>
       <c r="P18" s="32"/>
       <c r="S18"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="158"/>
-      <c r="B19" s="159"/>
-      <c r="C19" s="154"/>
+      <c r="A19" s="191"/>
+      <c r="B19" s="192"/>
+      <c r="C19" s="195"/>
       <c r="D19" s="75" t="s">
         <v>28</v>
       </c>
@@ -3586,23 +3664,23 @@
         <v>1</v>
       </c>
       <c r="K19" s="77"/>
-      <c r="L19" s="170">
+      <c r="L19" s="156">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="M19" s="170"/>
+      <c r="M19" s="156"/>
       <c r="N19" s="75">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="O19" s="79"/>
-      <c r="P19" s="186"/>
+      <c r="P19" s="172"/>
       <c r="S19"/>
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="158"/>
-      <c r="B20" s="159"/>
-      <c r="C20" s="154"/>
+      <c r="A20" s="191"/>
+      <c r="B20" s="192"/>
+      <c r="C20" s="195"/>
       <c r="D20" s="81" t="s">
         <v>29</v>
       </c>
@@ -3613,16 +3691,16 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G20" s="196"/>
-      <c r="H20" s="196"/>
-      <c r="I20" s="196"/>
-      <c r="J20" s="196">
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="182">
         <v>2</v>
       </c>
-      <c r="K20" s="197">
+      <c r="K20" s="183">
         <v>2</v>
       </c>
-      <c r="L20" s="164">
+      <c r="L20" s="150">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3632,15 +3710,15 @@
         <v>5</v>
       </c>
       <c r="O20" s="26"/>
-      <c r="P20" s="203"/>
+      <c r="P20" s="185"/>
       <c r="S20"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="158"/>
-      <c r="B21" s="155" t="s">
+      <c r="A21" s="191"/>
+      <c r="B21" s="196" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="156" t="s">
+      <c r="C21" s="197" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="84" t="s">
@@ -3664,7 +3742,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M21" s="171"/>
+      <c r="M21" s="157"/>
       <c r="N21" s="84">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -3673,15 +3751,15 @@
         <f>48.02-(48.02*10/100)</f>
         <v>43.218000000000004</v>
       </c>
-      <c r="P21" s="187">
+      <c r="P21" s="173">
         <v>105</v>
       </c>
       <c r="S21"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="158"/>
-      <c r="B22" s="155"/>
-      <c r="C22" s="156"/>
+      <c r="A22" s="191"/>
+      <c r="B22" s="196"/>
+      <c r="C22" s="197"/>
       <c r="D22" s="91" t="s">
         <v>34</v>
       </c>
@@ -3703,19 +3781,19 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M22" s="172"/>
+      <c r="M22" s="158"/>
       <c r="N22" s="91">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O22" s="96"/>
-      <c r="P22" s="188"/>
+      <c r="P22" s="174"/>
       <c r="S22"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="158"/>
-      <c r="B23" s="155"/>
-      <c r="C23" s="156"/>
+      <c r="A23" s="191"/>
+      <c r="B23" s="196"/>
+      <c r="C23" s="197"/>
       <c r="D23" s="98" t="s">
         <v>26</v>
       </c>
@@ -3741,19 +3819,19 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M23" s="173"/>
+      <c r="M23" s="159"/>
       <c r="N23" s="98">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O23" s="103"/>
-      <c r="P23" s="189"/>
+      <c r="P23" s="175"/>
       <c r="S23"/>
     </row>
     <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="158"/>
-      <c r="B24" s="155"/>
-      <c r="C24" s="156"/>
+      <c r="A24" s="191"/>
+      <c r="B24" s="196"/>
+      <c r="C24" s="197"/>
       <c r="D24" s="91" t="s">
         <v>27</v>
       </c>
@@ -3775,19 +3853,19 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M24" s="172"/>
+      <c r="M24" s="158"/>
       <c r="N24" s="91">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O24" s="96"/>
-      <c r="P24" s="188"/>
+      <c r="P24" s="174"/>
       <c r="S24"/>
     </row>
     <row r="25" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="158"/>
-      <c r="B25" s="155"/>
-      <c r="C25" s="156"/>
+      <c r="A25" s="191"/>
+      <c r="B25" s="196"/>
+      <c r="C25" s="197"/>
       <c r="D25" s="105" t="s">
         <v>28</v>
       </c>
@@ -3809,19 +3887,19 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M25" s="174"/>
+      <c r="M25" s="160"/>
       <c r="N25" s="105">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O25" s="110"/>
-      <c r="P25" s="190"/>
+      <c r="P25" s="176"/>
       <c r="S25"/>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="158"/>
-      <c r="B26" s="155"/>
-      <c r="C26" s="161" t="s">
+      <c r="A26" s="191"/>
+      <c r="B26" s="196"/>
+      <c r="C26" s="198" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="84" t="s">
@@ -3845,7 +3923,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M26" s="171"/>
+      <c r="M26" s="157"/>
       <c r="N26" s="84">
         <f t="shared" si="2"/>
         <v>2</v>
@@ -3854,15 +3932,15 @@
         <f>54.85-(54.85*10/100)</f>
         <v>49.365000000000002</v>
       </c>
-      <c r="P26" s="187">
+      <c r="P26" s="173">
         <v>115</v>
       </c>
       <c r="S26"/>
     </row>
     <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="158"/>
-      <c r="B27" s="155"/>
-      <c r="C27" s="161"/>
+      <c r="A27" s="191"/>
+      <c r="B27" s="196"/>
+      <c r="C27" s="198"/>
       <c r="D27" s="91" t="s">
         <v>34</v>
       </c>
@@ -3884,19 +3962,19 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M27" s="172"/>
+      <c r="M27" s="158"/>
       <c r="N27" s="91">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O27" s="96"/>
-      <c r="P27" s="188"/>
+      <c r="P27" s="174"/>
       <c r="S27"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="158"/>
-      <c r="B28" s="155"/>
-      <c r="C28" s="161"/>
+      <c r="A28" s="191"/>
+      <c r="B28" s="196"/>
+      <c r="C28" s="198"/>
       <c r="D28" s="98" t="s">
         <v>26</v>
       </c>
@@ -3918,19 +3996,19 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M28" s="173"/>
+      <c r="M28" s="159"/>
       <c r="N28" s="98">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O28" s="103"/>
-      <c r="P28" s="189"/>
+      <c r="P28" s="175"/>
       <c r="S28"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="158"/>
-      <c r="B29" s="155"/>
-      <c r="C29" s="161"/>
+      <c r="A29" s="191"/>
+      <c r="B29" s="196"/>
+      <c r="C29" s="198"/>
       <c r="D29" s="91" t="s">
         <v>27</v>
       </c>
@@ -3950,19 +4028,19 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M29" s="172"/>
+      <c r="M29" s="158"/>
       <c r="N29" s="91">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O29" s="96"/>
-      <c r="P29" s="188"/>
+      <c r="P29" s="174"/>
       <c r="S29"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="158"/>
-      <c r="B30" s="155"/>
-      <c r="C30" s="161"/>
+      <c r="A30" s="191"/>
+      <c r="B30" s="196"/>
+      <c r="C30" s="198"/>
       <c r="D30" s="112" t="s">
         <v>28</v>
       </c>
@@ -3982,19 +4060,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M30" s="175"/>
+      <c r="M30" s="161"/>
       <c r="N30" s="112">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O30" s="117"/>
-      <c r="P30" s="191"/>
+      <c r="P30" s="177"/>
       <c r="S30"/>
     </row>
     <row r="31" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="158"/>
-      <c r="B31" s="155"/>
-      <c r="C31" s="162" t="s">
+      <c r="A31" s="191"/>
+      <c r="B31" s="196"/>
+      <c r="C31" s="199" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="84" t="s">
@@ -4018,7 +4096,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M31" s="173"/>
+      <c r="M31" s="159"/>
       <c r="N31" s="98">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -4027,15 +4105,15 @@
         <f>38.88-(38.88*10/100)</f>
         <v>34.992000000000004</v>
       </c>
-      <c r="P31" s="189">
+      <c r="P31" s="175">
         <v>95</v>
       </c>
       <c r="S31"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="158"/>
-      <c r="B32" s="155"/>
-      <c r="C32" s="162"/>
+      <c r="A32" s="191"/>
+      <c r="B32" s="196"/>
+      <c r="C32" s="199"/>
       <c r="D32" s="91" t="s">
         <v>26</v>
       </c>
@@ -4061,19 +4139,19 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M32" s="172"/>
+      <c r="M32" s="158"/>
       <c r="N32" s="91">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O32" s="96"/>
-      <c r="P32" s="188"/>
+      <c r="P32" s="174"/>
       <c r="S32"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="158"/>
-      <c r="B33" s="155"/>
-      <c r="C33" s="162"/>
+      <c r="A33" s="191"/>
+      <c r="B33" s="196"/>
+      <c r="C33" s="199"/>
       <c r="D33" s="98" t="s">
         <v>27</v>
       </c>
@@ -4095,19 +4173,19 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M33" s="173"/>
+      <c r="M33" s="159"/>
       <c r="N33" s="98">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O33" s="103"/>
-      <c r="P33" s="189"/>
+      <c r="P33" s="175"/>
       <c r="S33"/>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="158"/>
-      <c r="B34" s="155"/>
-      <c r="C34" s="162"/>
+      <c r="A34" s="191"/>
+      <c r="B34" s="196"/>
+      <c r="C34" s="199"/>
       <c r="D34" s="91" t="s">
         <v>28</v>
       </c>
@@ -4129,19 +4207,19 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M34" s="172"/>
+      <c r="M34" s="158"/>
       <c r="N34" s="91">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O34" s="96"/>
-      <c r="P34" s="188"/>
+      <c r="P34" s="174"/>
       <c r="S34"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="158"/>
-      <c r="B35" s="155"/>
-      <c r="C35" s="162"/>
+      <c r="A35" s="191"/>
+      <c r="B35" s="196"/>
+      <c r="C35" s="199"/>
       <c r="D35" s="118" t="s">
         <v>29</v>
       </c>
@@ -4161,23 +4239,23 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M35" s="176"/>
+      <c r="M35" s="162"/>
       <c r="N35" s="118">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O35" s="123"/>
-      <c r="P35" s="192"/>
+      <c r="P35" s="178"/>
       <c r="S35"/>
     </row>
     <row r="36" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150" t="s">
+      <c r="A36" s="201" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="151" t="s">
+      <c r="B36" s="202" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="152" t="s">
+      <c r="C36" s="203" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="125" t="s">
@@ -4204,7 +4282,7 @@
       </c>
       <c r="K36" s="128"/>
       <c r="L36" s="129"/>
-      <c r="M36" s="177"/>
+      <c r="M36" s="163"/>
       <c r="N36" s="125"/>
       <c r="O36" s="130">
         <f>49.18-(49.18*10/100)</f>
@@ -4214,9 +4292,9 @@
       <c r="S36"/>
     </row>
     <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="150"/>
-      <c r="B37" s="151"/>
-      <c r="C37" s="152"/>
+      <c r="A37" s="201"/>
+      <c r="B37" s="202"/>
+      <c r="C37" s="203"/>
       <c r="D37" s="26" t="s">
         <v>27</v>
       </c>
@@ -4237,16 +4315,16 @@
       </c>
       <c r="K37" s="29"/>
       <c r="L37" s="30"/>
-      <c r="M37" s="164"/>
+      <c r="M37" s="150"/>
       <c r="N37" s="26"/>
       <c r="O37" s="31"/>
       <c r="P37" s="32"/>
       <c r="S37"/>
     </row>
     <row r="38" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="150"/>
-      <c r="B38" s="151"/>
-      <c r="C38" s="152"/>
+      <c r="A38" s="201"/>
+      <c r="B38" s="202"/>
+      <c r="C38" s="203"/>
       <c r="D38" s="18" t="s">
         <v>28</v>
       </c>
@@ -4263,16 +4341,16 @@
       <c r="J38" s="18"/>
       <c r="K38" s="21"/>
       <c r="L38" s="22"/>
-      <c r="M38" s="163"/>
+      <c r="M38" s="149"/>
       <c r="N38" s="18"/>
       <c r="O38" s="23"/>
       <c r="P38" s="24"/>
       <c r="S38"/>
     </row>
     <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="150"/>
-      <c r="B39" s="151"/>
-      <c r="C39" s="152"/>
+      <c r="A39" s="201"/>
+      <c r="B39" s="202"/>
+      <c r="C39" s="203"/>
       <c r="D39" s="33" t="s">
         <v>29</v>
       </c>
@@ -4291,16 +4369,16 @@
         <v>2</v>
       </c>
       <c r="L39" s="37"/>
-      <c r="M39" s="165"/>
+      <c r="M39" s="151"/>
       <c r="N39" s="33"/>
       <c r="O39" s="38"/>
       <c r="P39" s="39"/>
       <c r="S39"/>
     </row>
     <row r="40" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="150"/>
-      <c r="B40" s="151"/>
-      <c r="C40" s="153" t="s">
+      <c r="A40" s="201"/>
+      <c r="B40" s="202"/>
+      <c r="C40" s="194" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="40" t="s">
@@ -4321,7 +4399,7 @@
       <c r="J40" s="40"/>
       <c r="K40" s="43"/>
       <c r="L40" s="44"/>
-      <c r="M40" s="166"/>
+      <c r="M40" s="152"/>
       <c r="N40" s="40"/>
       <c r="O40" s="45">
         <f>56.01-(56.01*10/100)</f>
@@ -4331,9 +4409,9 @@
       <c r="S40"/>
     </row>
     <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="150"/>
-      <c r="B41" s="151"/>
-      <c r="C41" s="153"/>
+      <c r="A41" s="201"/>
+      <c r="B41" s="202"/>
+      <c r="C41" s="194"/>
       <c r="D41" s="47" t="s">
         <v>27</v>
       </c>
@@ -4354,16 +4432,16 @@
       </c>
       <c r="K41" s="50"/>
       <c r="L41" s="51"/>
-      <c r="M41" s="167"/>
+      <c r="M41" s="153"/>
       <c r="N41" s="47"/>
       <c r="O41" s="52"/>
       <c r="P41" s="53"/>
       <c r="S41"/>
     </row>
     <row r="42" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="150"/>
-      <c r="B42" s="151"/>
-      <c r="C42" s="153"/>
+      <c r="A42" s="201"/>
+      <c r="B42" s="202"/>
+      <c r="C42" s="194"/>
       <c r="D42" s="54" t="s">
         <v>28</v>
       </c>
@@ -4380,16 +4458,16 @@
       <c r="J42" s="54"/>
       <c r="K42" s="57"/>
       <c r="L42" s="58"/>
-      <c r="M42" s="168"/>
+      <c r="M42" s="154"/>
       <c r="N42" s="54"/>
       <c r="O42" s="59"/>
       <c r="P42" s="60"/>
       <c r="S42"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="150"/>
-      <c r="B43" s="151"/>
-      <c r="C43" s="153"/>
+      <c r="A43" s="201"/>
+      <c r="B43" s="202"/>
+      <c r="C43" s="194"/>
       <c r="D43" s="61" t="s">
         <v>29</v>
       </c>
@@ -4408,16 +4486,16 @@
         <v>1</v>
       </c>
       <c r="L43" s="65"/>
-      <c r="M43" s="169"/>
+      <c r="M43" s="155"/>
       <c r="N43" s="61"/>
       <c r="O43" s="66"/>
       <c r="P43" s="67"/>
       <c r="S43"/>
     </row>
     <row r="44" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="150"/>
-      <c r="B44" s="151"/>
-      <c r="C44" s="154" t="s">
+      <c r="A44" s="201"/>
+      <c r="B44" s="202"/>
+      <c r="C44" s="195" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="18" t="s">
@@ -4440,7 +4518,7 @@
       </c>
       <c r="K44" s="21"/>
       <c r="L44" s="22"/>
-      <c r="M44" s="163"/>
+      <c r="M44" s="149"/>
       <c r="N44" s="18"/>
       <c r="O44" s="23">
         <f>50.08-(50.08*10/100)</f>
@@ -4450,9 +4528,9 @@
       <c r="S44"/>
     </row>
     <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="150"/>
-      <c r="B45" s="151"/>
-      <c r="C45" s="154"/>
+      <c r="A45" s="201"/>
+      <c r="B45" s="202"/>
+      <c r="C45" s="195"/>
       <c r="D45" s="69" t="s">
         <v>26</v>
       </c>
@@ -4482,9 +4560,9 @@
       <c r="S45"/>
     </row>
     <row r="46" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="150"/>
-      <c r="B46" s="151"/>
-      <c r="C46" s="154"/>
+      <c r="A46" s="201"/>
+      <c r="B46" s="202"/>
+      <c r="C46" s="195"/>
       <c r="D46" s="75" t="s">
         <v>27</v>
       </c>
@@ -4505,16 +4583,16 @@
       </c>
       <c r="K46" s="77"/>
       <c r="L46" s="78"/>
-      <c r="M46" s="170"/>
+      <c r="M46" s="156"/>
       <c r="N46" s="75"/>
       <c r="O46" s="79"/>
       <c r="P46" s="80"/>
       <c r="S46"/>
     </row>
     <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="150"/>
-      <c r="B47" s="151"/>
-      <c r="C47" s="154"/>
+      <c r="A47" s="201"/>
+      <c r="B47" s="202"/>
+      <c r="C47" s="195"/>
       <c r="D47" s="69" t="s">
         <v>28</v>
       </c>
@@ -4540,9 +4618,9 @@
       <c r="S47"/>
     </row>
     <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="150"/>
-      <c r="B48" s="151"/>
-      <c r="C48" s="154"/>
+      <c r="A48" s="201"/>
+      <c r="B48" s="202"/>
+      <c r="C48" s="195"/>
       <c r="D48" s="75" t="s">
         <v>29</v>
       </c>
@@ -4563,18 +4641,18 @@
         <v>2</v>
       </c>
       <c r="L48" s="78"/>
-      <c r="M48" s="170"/>
+      <c r="M48" s="156"/>
       <c r="N48" s="75"/>
       <c r="O48" s="79"/>
       <c r="P48" s="80"/>
       <c r="S48"/>
     </row>
     <row r="49" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="150"/>
-      <c r="B49" s="155" t="s">
+      <c r="A49" s="201"/>
+      <c r="B49" s="196" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="156" t="s">
+      <c r="C49" s="197" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="84" t="s">
@@ -4597,7 +4675,7 @@
       </c>
       <c r="K49" s="87"/>
       <c r="L49" s="88"/>
-      <c r="M49" s="171"/>
+      <c r="M49" s="157"/>
       <c r="N49" s="84"/>
       <c r="O49" s="89">
         <f>48.02-(48.02*10/100)</f>
@@ -4607,9 +4685,9 @@
       <c r="S49"/>
     </row>
     <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="150"/>
-      <c r="B50" s="155"/>
-      <c r="C50" s="156"/>
+      <c r="A50" s="201"/>
+      <c r="B50" s="196"/>
+      <c r="C50" s="197"/>
       <c r="D50" s="91" t="s">
         <v>34</v>
       </c>
@@ -4628,16 +4706,16 @@
       </c>
       <c r="K50" s="94"/>
       <c r="L50" s="95"/>
-      <c r="M50" s="172"/>
+      <c r="M50" s="158"/>
       <c r="N50" s="91"/>
       <c r="O50" s="96"/>
       <c r="P50" s="97"/>
       <c r="S50"/>
     </row>
     <row r="51" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="150"/>
-      <c r="B51" s="155"/>
-      <c r="C51" s="156"/>
+      <c r="A51" s="201"/>
+      <c r="B51" s="196"/>
+      <c r="C51" s="197"/>
       <c r="D51" s="98" t="s">
         <v>26</v>
       </c>
@@ -4654,16 +4732,16 @@
       <c r="J51" s="98"/>
       <c r="K51" s="101"/>
       <c r="L51" s="102"/>
-      <c r="M51" s="173"/>
+      <c r="M51" s="159"/>
       <c r="N51" s="98"/>
       <c r="O51" s="103"/>
       <c r="P51" s="104"/>
       <c r="S51"/>
     </row>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="150"/>
-      <c r="B52" s="155"/>
-      <c r="C52" s="156"/>
+      <c r="A52" s="201"/>
+      <c r="B52" s="196"/>
+      <c r="C52" s="197"/>
       <c r="D52" s="91" t="s">
         <v>27</v>
       </c>
@@ -4680,16 +4758,16 @@
       <c r="J52" s="91"/>
       <c r="K52" s="94"/>
       <c r="L52" s="95"/>
-      <c r="M52" s="172"/>
+      <c r="M52" s="158"/>
       <c r="N52" s="91"/>
       <c r="O52" s="96"/>
       <c r="P52" s="97"/>
       <c r="S52"/>
     </row>
     <row r="53" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="150"/>
-      <c r="B53" s="155"/>
-      <c r="C53" s="156"/>
+      <c r="A53" s="201"/>
+      <c r="B53" s="196"/>
+      <c r="C53" s="197"/>
       <c r="D53" s="105" t="s">
         <v>28</v>
       </c>
@@ -4706,16 +4784,16 @@
       <c r="J53" s="105"/>
       <c r="K53" s="108"/>
       <c r="L53" s="109"/>
-      <c r="M53" s="174"/>
+      <c r="M53" s="160"/>
       <c r="N53" s="105"/>
       <c r="O53" s="110"/>
       <c r="P53" s="111"/>
       <c r="S53"/>
     </row>
     <row r="54" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="150"/>
-      <c r="B54" s="155"/>
-      <c r="C54" s="157" t="s">
+      <c r="A54" s="201"/>
+      <c r="B54" s="196"/>
+      <c r="C54" s="204" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="84" t="s">
@@ -4736,7 +4814,7 @@
       <c r="J54" s="84"/>
       <c r="K54" s="87"/>
       <c r="L54" s="88"/>
-      <c r="M54" s="171"/>
+      <c r="M54" s="157"/>
       <c r="N54" s="84"/>
       <c r="O54" s="89">
         <f>54.85-(54.85*10/100)</f>
@@ -4746,9 +4824,9 @@
       <c r="S54"/>
     </row>
     <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="150"/>
-      <c r="B55" s="155"/>
-      <c r="C55" s="157"/>
+      <c r="A55" s="201"/>
+      <c r="B55" s="196"/>
+      <c r="C55" s="204"/>
       <c r="D55" s="91" t="s">
         <v>34</v>
       </c>
@@ -4767,16 +4845,16 @@
       </c>
       <c r="K55" s="94"/>
       <c r="L55" s="95"/>
-      <c r="M55" s="172"/>
+      <c r="M55" s="158"/>
       <c r="N55" s="91"/>
       <c r="O55" s="96"/>
       <c r="P55" s="97"/>
       <c r="S55"/>
     </row>
     <row r="56" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="150"/>
-      <c r="B56" s="155"/>
-      <c r="C56" s="157"/>
+      <c r="A56" s="201"/>
+      <c r="B56" s="196"/>
+      <c r="C56" s="204"/>
       <c r="D56" s="98" t="s">
         <v>26</v>
       </c>
@@ -4793,16 +4871,16 @@
       <c r="J56" s="98"/>
       <c r="K56" s="101"/>
       <c r="L56" s="102"/>
-      <c r="M56" s="173"/>
+      <c r="M56" s="159"/>
       <c r="N56" s="98"/>
       <c r="O56" s="103"/>
       <c r="P56" s="104"/>
       <c r="S56"/>
     </row>
     <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="150"/>
-      <c r="B57" s="155"/>
-      <c r="C57" s="157"/>
+      <c r="A57" s="201"/>
+      <c r="B57" s="196"/>
+      <c r="C57" s="204"/>
       <c r="D57" s="91" t="s">
         <v>27</v>
       </c>
@@ -4819,16 +4897,16 @@
       <c r="J57" s="91"/>
       <c r="K57" s="94"/>
       <c r="L57" s="95"/>
-      <c r="M57" s="172"/>
+      <c r="M57" s="158"/>
       <c r="N57" s="91"/>
       <c r="O57" s="96"/>
       <c r="P57" s="97"/>
       <c r="S57"/>
     </row>
     <row r="58" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="150"/>
-      <c r="B58" s="155"/>
-      <c r="C58" s="204"/>
+      <c r="A58" s="201"/>
+      <c r="B58" s="196"/>
+      <c r="C58" s="205"/>
       <c r="D58" s="118" t="s">
         <v>28</v>
       </c>
@@ -4845,7 +4923,7 @@
       <c r="J58" s="118"/>
       <c r="K58" s="121"/>
       <c r="L58" s="122"/>
-      <c r="M58" s="176"/>
+      <c r="M58" s="162"/>
       <c r="N58" s="118"/>
       <c r="O58" s="123"/>
       <c r="P58" s="124"/>
@@ -4853,7 +4931,7 @@
     </row>
     <row r="59" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59"/>
-      <c r="C59" s="149" t="s">
+      <c r="C59" s="200" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="132" t="s">
@@ -4888,7 +4966,7 @@
     </row>
     <row r="60" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
-      <c r="C60" s="149"/>
+      <c r="C60" s="200"/>
       <c r="D60" s="140" t="s">
         <v>38</v>
       </c>
@@ -4959,6 +5037,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A36:A58"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C58"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:P7"/>
@@ -4971,15 +5058,6 @@
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C35"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A36:A58"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Lagerbestand aktualisiert, Guiding Team
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -15,16 +15,11 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$36:$P$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$7:$P$35</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Tabelle1!$7:$8</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -221,6 +216,56 @@
         </r>
       </text>
     </comment>
+    <comment ref="I37" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Beat
+Reto x2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Adrian
+Manuel</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G45" authorId="1" shapeId="0">
       <text>
         <r>
@@ -256,6 +301,79 @@
           </rPr>
           <t xml:space="preserve">
 für simon, muss noch übergeben werden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Beat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Adrian
+Reto x2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Manuel</t>
         </r>
       </text>
     </comment>
@@ -1856,610 +1974,825 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="74" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="10" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="75" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="10" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="10" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="11" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="11" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="77" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="13" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="13" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="11" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="13" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="13" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="16" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="80" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="49" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="81" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="52" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="15" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="16" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="61" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="11" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="69" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="70" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="69" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="69" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="70" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="69" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="68" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="72" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="74" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="75" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="77" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="76" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="80" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="81" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="10" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="10" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="11" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="13" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="11" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="13" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="8" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="15" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="16" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="15" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="15" borderId="49" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="15" borderId="52" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="15" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="8" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="72" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3052,207 +3385,208 @@
   <dimension ref="A1:IX69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S21" sqref="S21"/>
+      <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1"/>
-    <col min="2" max="2" width="10.42578125" style="1"/>
-    <col min="3" max="3" width="13.140625" style="1"/>
-    <col min="4" max="4" width="7.42578125" style="2"/>
-    <col min="5" max="5" width="11" style="3"/>
-    <col min="6" max="11" width="6.5703125" style="1"/>
-    <col min="12" max="12" width="10.42578125" style="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="10.42578125" style="1"/>
-    <col min="15" max="15" width="10.5703125" style="4"/>
-    <col min="16" max="258" width="10.42578125" style="1"/>
-    <col min="259" max="1026" width="8.28515625"/>
+    <col min="1" max="1" width="12.28515625" style="3"/>
+    <col min="2" max="2" width="10.42578125" style="3"/>
+    <col min="3" max="3" width="13.140625" style="3"/>
+    <col min="4" max="4" width="7.42578125" style="185"/>
+    <col min="5" max="5" width="11" style="186"/>
+    <col min="6" max="11" width="6.5703125" style="3"/>
+    <col min="12" max="12" width="10.42578125" style="3"/>
+    <col min="13" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="10.42578125" style="3"/>
+    <col min="15" max="15" width="10.5703125" style="187"/>
+    <col min="16" max="258" width="10.42578125" style="3"/>
+    <col min="259" max="1026" width="8.28515625" style="5"/>
+    <col min="1027" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="R2"/>
-      <c r="S2"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="R3"/>
-      <c r="S3"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
     </row>
     <row r="4" spans="1:19" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="186">
+      <c r="B4" s="8">
         <f ca="1">TODAY()</f>
-        <v>42710</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="R4"/>
-      <c r="S4"/>
+        <v>42724</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="R5"/>
-      <c r="S5"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="R6"/>
-      <c r="S6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="R6" s="188"/>
+      <c r="S6" s="5"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="187" t="s">
+      <c r="A7" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="188"/>
-      <c r="C7" s="188"/>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188"/>
-      <c r="F7" s="189" t="s">
+      <c r="B7" s="200"/>
+      <c r="C7" s="200"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="189"/>
-      <c r="H7" s="189"/>
-      <c r="I7" s="189"/>
-      <c r="J7" s="189"/>
-      <c r="K7" s="189"/>
-      <c r="L7" s="189" t="s">
+      <c r="G7" s="201"/>
+      <c r="H7" s="201"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="201"/>
+      <c r="L7" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="189"/>
-      <c r="N7" s="189" t="s">
+      <c r="M7" s="201"/>
+      <c r="N7" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="189"/>
-      <c r="P7" s="190"/>
-      <c r="R7"/>
-      <c r="S7"/>
+      <c r="O7" s="201"/>
+      <c r="P7" s="202"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
     </row>
     <row r="8" spans="1:19" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="164" t="s">
+      <c r="L8" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="M8" s="164" t="s">
+      <c r="M8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="N8" s="16" t="s">
@@ -3264,17 +3598,17 @@
       <c r="P8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="R8"/>
-      <c r="S8"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="191" t="s">
+      <c r="A9" s="203" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="192" t="s">
+      <c r="B9" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="193" t="s">
+      <c r="C9" s="205" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -3300,69 +3634,69 @@
         <f>F9</f>
         <v>11</v>
       </c>
-      <c r="M9" s="149"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="18">
         <f>L9-M9</f>
         <v>11</v>
       </c>
-      <c r="O9" s="23">
+      <c r="O9" s="24">
         <f>49.18-(49.18*10/100)</f>
         <v>44.262</v>
       </c>
-      <c r="P9" s="165">
+      <c r="P9" s="25">
         <v>105</v>
       </c>
-      <c r="R9" s="25"/>
-      <c r="S9"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="191"/>
-      <c r="B10" s="192"/>
-      <c r="C10" s="193"/>
-      <c r="D10" s="26" t="s">
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="28">
         <v>18</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26">
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27">
         <v>3</v>
       </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30">
+      <c r="K10" s="30"/>
+      <c r="L10" s="31">
         <f t="shared" ref="L10:L35" si="1">F10</f>
         <v>15</v>
       </c>
-      <c r="M10" s="150">
-        <v>1</v>
-      </c>
-      <c r="N10" s="26">
+      <c r="M10" s="32">
+        <v>1</v>
+      </c>
+      <c r="N10" s="27">
         <f t="shared" ref="N10:N35" si="2">L10-M10</f>
         <v>14</v>
       </c>
-      <c r="O10" s="31"/>
-      <c r="P10" s="166"/>
-      <c r="R10" s="25"/>
-      <c r="S10"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="34"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="5"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="191"/>
-      <c r="B11" s="192"/>
-      <c r="C11" s="193"/>
+      <c r="A11" s="203"/>
+      <c r="B11" s="204"/>
+      <c r="C11" s="205"/>
       <c r="D11" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="19">
         <v>20</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="29">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -3375,1133 +3709,1137 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="M11" s="149"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="18">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="165"/>
-      <c r="R11" s="25"/>
-      <c r="S11"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="25"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="5"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="191"/>
-      <c r="B12" s="192"/>
-      <c r="C12" s="193"/>
-      <c r="D12" s="33" t="s">
+      <c r="A12" s="203"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="205"/>
+      <c r="D12" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="36">
         <v>7</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="36">
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="38">
         <v>2</v>
       </c>
-      <c r="L12" s="37">
+      <c r="L12" s="39">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M12" s="151"/>
-      <c r="N12" s="33">
+      <c r="M12" s="40"/>
+      <c r="N12" s="35">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="O12" s="38"/>
-      <c r="P12" s="167"/>
-      <c r="R12" s="25"/>
-      <c r="S12"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="42"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="5"/>
     </row>
     <row r="13" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="191"/>
-      <c r="B13" s="192"/>
-      <c r="C13" s="194" t="s">
+      <c r="A13" s="203"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="193" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="44">
         <v>4</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="45">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40">
-        <v>1</v>
-      </c>
-      <c r="J13" s="40"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="44">
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43">
+        <v>1</v>
+      </c>
+      <c r="J13" s="43"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="47">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M13" s="152"/>
-      <c r="N13" s="40">
+      <c r="M13" s="48"/>
+      <c r="N13" s="43">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="O13" s="45">
+      <c r="O13" s="49">
         <f>56.01-(56.01*10/100)</f>
         <v>50.408999999999999</v>
       </c>
-      <c r="P13" s="168">
+      <c r="P13" s="50">
         <v>115</v>
       </c>
-      <c r="R13" s="25"/>
-      <c r="S13"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="5"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="191"/>
-      <c r="B14" s="192"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="47" t="s">
+      <c r="A14" s="203"/>
+      <c r="B14" s="204"/>
+      <c r="C14" s="193"/>
+      <c r="D14" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="52">
         <v>4</v>
       </c>
-      <c r="F14" s="49">
+      <c r="F14" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47">
-        <v>1</v>
-      </c>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47">
-        <v>1</v>
-      </c>
-      <c r="K14" s="50"/>
-      <c r="L14" s="51">
+      <c r="G14" s="51"/>
+      <c r="H14" s="51">
+        <v>1</v>
+      </c>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51">
+        <v>1</v>
+      </c>
+      <c r="K14" s="54"/>
+      <c r="L14" s="55">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M14" s="153">
-        <v>1</v>
-      </c>
-      <c r="N14" s="47">
+      <c r="M14" s="56">
+        <v>1</v>
+      </c>
+      <c r="N14" s="51">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O14" s="52"/>
-      <c r="P14" s="169"/>
-      <c r="S14"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="58"/>
+      <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="191"/>
-      <c r="B15" s="192"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="54" t="s">
+      <c r="A15" s="203"/>
+      <c r="B15" s="204"/>
+      <c r="C15" s="193"/>
+      <c r="D15" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="55">
+      <c r="E15" s="60">
         <v>0</v>
       </c>
-      <c r="F15" s="56">
+      <c r="F15" s="61">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="58">
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="63">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M15" s="154"/>
-      <c r="N15" s="54">
+      <c r="M15" s="64"/>
+      <c r="N15" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O15" s="59"/>
-      <c r="P15" s="170"/>
-      <c r="S15"/>
+      <c r="O15" s="65"/>
+      <c r="P15" s="66"/>
+      <c r="S15" s="5"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="191"/>
-      <c r="B16" s="192"/>
-      <c r="C16" s="194"/>
-      <c r="D16" s="61" t="s">
+      <c r="A16" s="203"/>
+      <c r="B16" s="204"/>
+      <c r="C16" s="193"/>
+      <c r="D16" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="62">
+      <c r="E16" s="68">
         <v>2</v>
       </c>
-      <c r="F16" s="63">
+      <c r="F16" s="69">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="64">
-        <v>1</v>
-      </c>
-      <c r="L16" s="65">
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="70">
+        <v>1</v>
+      </c>
+      <c r="L16" s="71">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M16" s="155"/>
-      <c r="N16" s="61">
+      <c r="M16" s="72"/>
+      <c r="N16" s="67">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O16" s="66"/>
-      <c r="P16" s="171"/>
-      <c r="S16"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="74"/>
+      <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="191"/>
-      <c r="B17" s="192"/>
-      <c r="C17" s="195" t="s">
+      <c r="A17" s="203"/>
+      <c r="B17" s="204"/>
+      <c r="C17" s="194" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="68">
+      <c r="E17" s="75">
         <v>7</v>
       </c>
-      <c r="F17" s="179">
+      <c r="F17" s="76">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G17" s="180"/>
-      <c r="H17" s="180"/>
-      <c r="I17" s="180">
-        <v>1</v>
-      </c>
-      <c r="J17" s="180"/>
-      <c r="K17" s="181"/>
-      <c r="L17" s="149">
+      <c r="G17" s="77"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="77">
+        <v>1</v>
+      </c>
+      <c r="J17" s="77"/>
+      <c r="K17" s="78"/>
+      <c r="L17" s="23">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M17" s="149"/>
+      <c r="M17" s="23"/>
       <c r="N17" s="18">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="O17" s="23">
+      <c r="O17" s="24">
         <f>50.08-(50.08*10/100)</f>
         <v>45.072000000000003</v>
       </c>
-      <c r="P17" s="184">
+      <c r="P17" s="79">
         <v>105</v>
       </c>
-      <c r="S17"/>
+      <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="191"/>
-      <c r="B18" s="192"/>
-      <c r="C18" s="195"/>
-      <c r="D18" s="69" t="s">
+      <c r="A18" s="203"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="194"/>
+      <c r="D18" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="81">
         <v>13</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27">
         <v>2</v>
       </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="150">
+      <c r="I18" s="51"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="32">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="M18" s="26">
-        <v>1</v>
-      </c>
-      <c r="N18" s="26">
+      <c r="M18" s="27">
+        <v>1</v>
+      </c>
+      <c r="N18" s="27">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="O18" s="26"/>
-      <c r="P18" s="32"/>
-      <c r="S18"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="82"/>
+      <c r="S18" s="5"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="191"/>
-      <c r="B19" s="192"/>
-      <c r="C19" s="195"/>
-      <c r="D19" s="75" t="s">
+      <c r="A19" s="203"/>
+      <c r="B19" s="204"/>
+      <c r="C19" s="194"/>
+      <c r="D19" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="76">
+      <c r="E19" s="84">
         <v>10</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75">
-        <v>1</v>
-      </c>
-      <c r="K19" s="77"/>
-      <c r="L19" s="156">
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="83">
+        <v>1</v>
+      </c>
+      <c r="K19" s="85"/>
+      <c r="L19" s="86">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="M19" s="156"/>
-      <c r="N19" s="75">
+      <c r="M19" s="86"/>
+      <c r="N19" s="83">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="O19" s="79"/>
-      <c r="P19" s="172"/>
-      <c r="S19"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="88"/>
+      <c r="S19" s="5"/>
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="191"/>
-      <c r="B20" s="192"/>
-      <c r="C20" s="195"/>
-      <c r="D20" s="81" t="s">
+      <c r="A20" s="203"/>
+      <c r="B20" s="204"/>
+      <c r="C20" s="194"/>
+      <c r="D20" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="82">
+      <c r="E20" s="90">
         <v>9</v>
       </c>
-      <c r="F20" s="83">
+      <c r="F20" s="91">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G20" s="182"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="182"/>
-      <c r="J20" s="182">
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92"/>
+      <c r="J20" s="92">
         <v>2</v>
       </c>
-      <c r="K20" s="183">
+      <c r="K20" s="93">
         <v>2</v>
       </c>
-      <c r="L20" s="150">
+      <c r="L20" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26">
+      <c r="M20" s="27"/>
+      <c r="N20" s="27">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="O20" s="26"/>
-      <c r="P20" s="185"/>
-      <c r="S20"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="94"/>
+      <c r="S20" s="5"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="191"/>
-      <c r="B21" s="196" t="s">
+      <c r="A21" s="203"/>
+      <c r="B21" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="197" t="s">
+      <c r="C21" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="84" t="s">
+      <c r="D21" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="85">
+      <c r="E21" s="96">
         <v>5</v>
       </c>
-      <c r="F21" s="86">
+      <c r="F21" s="97">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G21" s="84">
+      <c r="G21" s="95">
         <v>2</v>
       </c>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="88">
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="99">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M21" s="157"/>
-      <c r="N21" s="84">
+      <c r="M21" s="100"/>
+      <c r="N21" s="95">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="O21" s="89">
+      <c r="O21" s="101">
         <f>48.02-(48.02*10/100)</f>
         <v>43.218000000000004</v>
       </c>
-      <c r="P21" s="173">
+      <c r="P21" s="102">
         <v>105</v>
       </c>
-      <c r="S21"/>
+      <c r="S21" s="5"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="191"/>
-      <c r="B22" s="196"/>
-      <c r="C22" s="197"/>
-      <c r="D22" s="91" t="s">
+      <c r="A22" s="203"/>
+      <c r="B22" s="195"/>
+      <c r="C22" s="196"/>
+      <c r="D22" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="92">
+      <c r="E22" s="104">
         <v>5</v>
       </c>
-      <c r="F22" s="93">
+      <c r="F22" s="105">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91">
-        <v>1</v>
-      </c>
-      <c r="J22" s="91"/>
-      <c r="K22" s="94"/>
-      <c r="L22" s="95">
+      <c r="G22" s="103"/>
+      <c r="H22" s="103"/>
+      <c r="I22" s="103">
+        <v>1</v>
+      </c>
+      <c r="J22" s="103"/>
+      <c r="K22" s="106"/>
+      <c r="L22" s="107">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M22" s="158"/>
-      <c r="N22" s="91">
+      <c r="M22" s="108"/>
+      <c r="N22" s="103">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="O22" s="96"/>
-      <c r="P22" s="174"/>
-      <c r="S22"/>
+      <c r="O22" s="109"/>
+      <c r="P22" s="110"/>
+      <c r="S22" s="5"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="191"/>
-      <c r="B23" s="196"/>
-      <c r="C23" s="197"/>
-      <c r="D23" s="98" t="s">
+      <c r="A23" s="203"/>
+      <c r="B23" s="195"/>
+      <c r="C23" s="196"/>
+      <c r="D23" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="99">
+      <c r="E23" s="112">
         <v>5</v>
       </c>
-      <c r="F23" s="100">
+      <c r="F23" s="113">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G23" s="98">
-        <v>1</v>
-      </c>
-      <c r="H23" s="98">
-        <v>1</v>
-      </c>
-      <c r="I23" s="98">
-        <v>1</v>
-      </c>
-      <c r="J23" s="98"/>
-      <c r="K23" s="101"/>
-      <c r="L23" s="102">
+      <c r="G23" s="111">
+        <v>1</v>
+      </c>
+      <c r="H23" s="111">
+        <v>1</v>
+      </c>
+      <c r="I23" s="111">
+        <v>1</v>
+      </c>
+      <c r="J23" s="111"/>
+      <c r="K23" s="114"/>
+      <c r="L23" s="115">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M23" s="159"/>
-      <c r="N23" s="98">
+      <c r="M23" s="116"/>
+      <c r="N23" s="111">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O23" s="103"/>
-      <c r="P23" s="175"/>
-      <c r="S23"/>
+      <c r="O23" s="117"/>
+      <c r="P23" s="118"/>
+      <c r="S23" s="5"/>
     </row>
     <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="191"/>
-      <c r="B24" s="196"/>
-      <c r="C24" s="197"/>
-      <c r="D24" s="91" t="s">
+      <c r="A24" s="203"/>
+      <c r="B24" s="195"/>
+      <c r="C24" s="196"/>
+      <c r="D24" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="92">
+      <c r="E24" s="104">
         <v>3</v>
       </c>
-      <c r="F24" s="93">
+      <c r="F24" s="105">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G24" s="91"/>
-      <c r="H24" s="91"/>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91">
-        <v>1</v>
-      </c>
-      <c r="K24" s="94"/>
-      <c r="L24" s="95">
+      <c r="G24" s="103"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="103"/>
+      <c r="J24" s="103">
+        <v>1</v>
+      </c>
+      <c r="K24" s="106"/>
+      <c r="L24" s="107">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M24" s="158"/>
-      <c r="N24" s="91">
+      <c r="M24" s="108"/>
+      <c r="N24" s="103">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O24" s="96"/>
-      <c r="P24" s="174"/>
-      <c r="S24"/>
+      <c r="O24" s="109"/>
+      <c r="P24" s="110"/>
+      <c r="S24" s="5"/>
     </row>
     <row r="25" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="191"/>
-      <c r="B25" s="196"/>
-      <c r="C25" s="197"/>
-      <c r="D25" s="105" t="s">
+      <c r="A25" s="203"/>
+      <c r="B25" s="195"/>
+      <c r="C25" s="196"/>
+      <c r="D25" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="106">
+      <c r="E25" s="120">
         <v>2</v>
       </c>
-      <c r="F25" s="107">
+      <c r="F25" s="121">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
-      <c r="I25" s="105"/>
-      <c r="J25" s="105">
-        <v>1</v>
-      </c>
-      <c r="K25" s="108"/>
-      <c r="L25" s="109">
+      <c r="G25" s="119"/>
+      <c r="H25" s="119"/>
+      <c r="I25" s="119"/>
+      <c r="J25" s="119">
+        <v>1</v>
+      </c>
+      <c r="K25" s="122"/>
+      <c r="L25" s="123">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M25" s="160"/>
-      <c r="N25" s="105">
+      <c r="M25" s="124"/>
+      <c r="N25" s="119">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O25" s="110"/>
-      <c r="P25" s="176"/>
-      <c r="S25"/>
+      <c r="O25" s="125"/>
+      <c r="P25" s="126"/>
+      <c r="S25" s="5"/>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="191"/>
-      <c r="B26" s="196"/>
-      <c r="C26" s="198" t="s">
+      <c r="A26" s="203"/>
+      <c r="B26" s="195"/>
+      <c r="C26" s="206" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="84" t="s">
+      <c r="D26" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="85">
+      <c r="E26" s="96">
         <v>3</v>
       </c>
-      <c r="F26" s="86">
+      <c r="F26" s="97">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G26" s="84">
-        <v>1</v>
-      </c>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="88">
+      <c r="G26" s="95">
+        <v>1</v>
+      </c>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="99">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M26" s="157"/>
-      <c r="N26" s="84">
+      <c r="M26" s="100"/>
+      <c r="N26" s="95">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O26" s="89">
+      <c r="O26" s="101">
         <f>54.85-(54.85*10/100)</f>
         <v>49.365000000000002</v>
       </c>
-      <c r="P26" s="173">
+      <c r="P26" s="102">
         <v>115</v>
       </c>
-      <c r="S26"/>
+      <c r="S26" s="5"/>
     </row>
     <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="191"/>
-      <c r="B27" s="196"/>
-      <c r="C27" s="198"/>
-      <c r="D27" s="91" t="s">
+      <c r="A27" s="203"/>
+      <c r="B27" s="195"/>
+      <c r="C27" s="206"/>
+      <c r="D27" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="92">
+      <c r="E27" s="104">
         <v>3</v>
       </c>
-      <c r="F27" s="93">
+      <c r="F27" s="105">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91">
-        <v>1</v>
-      </c>
-      <c r="J27" s="91"/>
-      <c r="K27" s="94"/>
-      <c r="L27" s="95">
+      <c r="G27" s="103"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103">
+        <v>1</v>
+      </c>
+      <c r="J27" s="103"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="107">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M27" s="158"/>
-      <c r="N27" s="91">
+      <c r="M27" s="108"/>
+      <c r="N27" s="103">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O27" s="96"/>
-      <c r="P27" s="174"/>
-      <c r="S27"/>
+      <c r="O27" s="109"/>
+      <c r="P27" s="110"/>
+      <c r="S27" s="5"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="191"/>
-      <c r="B28" s="196"/>
-      <c r="C28" s="198"/>
-      <c r="D28" s="98" t="s">
+      <c r="A28" s="203"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="206"/>
+      <c r="D28" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="99">
+      <c r="E28" s="112">
         <v>3</v>
       </c>
-      <c r="F28" s="100">
+      <c r="F28" s="113">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98">
-        <v>1</v>
-      </c>
-      <c r="J28" s="98"/>
-      <c r="K28" s="101"/>
-      <c r="L28" s="102">
+      <c r="G28" s="111"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="111">
+        <v>1</v>
+      </c>
+      <c r="J28" s="111"/>
+      <c r="K28" s="114"/>
+      <c r="L28" s="115">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M28" s="159"/>
-      <c r="N28" s="98">
+      <c r="M28" s="116"/>
+      <c r="N28" s="111">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O28" s="103"/>
-      <c r="P28" s="175"/>
-      <c r="S28"/>
+      <c r="O28" s="117"/>
+      <c r="P28" s="118"/>
+      <c r="S28" s="5"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="191"/>
-      <c r="B29" s="196"/>
-      <c r="C29" s="198"/>
-      <c r="D29" s="91" t="s">
+      <c r="A29" s="203"/>
+      <c r="B29" s="195"/>
+      <c r="C29" s="206"/>
+      <c r="D29" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="92">
-        <v>1</v>
-      </c>
-      <c r="F29" s="93">
+      <c r="E29" s="104">
+        <v>1</v>
+      </c>
+      <c r="F29" s="105">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G29" s="91"/>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
-      <c r="K29" s="94"/>
-      <c r="L29" s="95">
+      <c r="G29" s="103"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="103"/>
+      <c r="K29" s="106"/>
+      <c r="L29" s="107">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M29" s="158"/>
-      <c r="N29" s="91">
+      <c r="M29" s="108"/>
+      <c r="N29" s="103">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O29" s="96"/>
-      <c r="P29" s="174"/>
-      <c r="S29"/>
+      <c r="O29" s="109"/>
+      <c r="P29" s="110"/>
+      <c r="S29" s="5"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="191"/>
-      <c r="B30" s="196"/>
-      <c r="C30" s="198"/>
-      <c r="D30" s="112" t="s">
+      <c r="A30" s="203"/>
+      <c r="B30" s="195"/>
+      <c r="C30" s="206"/>
+      <c r="D30" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="113">
+      <c r="E30" s="128">
         <v>0</v>
       </c>
-      <c r="F30" s="114">
+      <c r="F30" s="129">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="112"/>
-      <c r="H30" s="112"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="112"/>
-      <c r="K30" s="115"/>
-      <c r="L30" s="116">
+      <c r="G30" s="127"/>
+      <c r="H30" s="127"/>
+      <c r="I30" s="127"/>
+      <c r="J30" s="127"/>
+      <c r="K30" s="130"/>
+      <c r="L30" s="131">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M30" s="161"/>
-      <c r="N30" s="112">
+      <c r="M30" s="132"/>
+      <c r="N30" s="127">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O30" s="117"/>
-      <c r="P30" s="177"/>
-      <c r="S30"/>
+      <c r="O30" s="133"/>
+      <c r="P30" s="134"/>
+      <c r="S30" s="5"/>
     </row>
     <row r="31" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="191"/>
-      <c r="B31" s="196"/>
-      <c r="C31" s="199" t="s">
+      <c r="A31" s="203"/>
+      <c r="B31" s="195"/>
+      <c r="C31" s="207" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="84" t="s">
+      <c r="D31" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="85">
+      <c r="E31" s="96">
         <v>7</v>
       </c>
-      <c r="F31" s="100">
+      <c r="F31" s="113">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G31" s="98">
+      <c r="G31" s="111">
         <v>2</v>
       </c>
-      <c r="H31" s="98"/>
-      <c r="I31" s="98"/>
-      <c r="J31" s="98"/>
-      <c r="K31" s="101"/>
-      <c r="L31" s="102">
+      <c r="H31" s="111"/>
+      <c r="I31" s="111"/>
+      <c r="J31" s="111"/>
+      <c r="K31" s="114"/>
+      <c r="L31" s="115">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M31" s="159"/>
-      <c r="N31" s="98">
+      <c r="M31" s="116"/>
+      <c r="N31" s="111">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="O31" s="103">
+      <c r="O31" s="117">
         <f>38.88-(38.88*10/100)</f>
         <v>34.992000000000004</v>
       </c>
-      <c r="P31" s="175">
+      <c r="P31" s="118">
         <v>95</v>
       </c>
-      <c r="S31"/>
+      <c r="S31" s="5"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="191"/>
-      <c r="B32" s="196"/>
-      <c r="C32" s="199"/>
-      <c r="D32" s="91" t="s">
+      <c r="A32" s="203"/>
+      <c r="B32" s="195"/>
+      <c r="C32" s="207"/>
+      <c r="D32" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="92">
+      <c r="E32" s="104">
         <v>6</v>
       </c>
-      <c r="F32" s="93">
+      <c r="F32" s="105">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G32" s="91">
-        <v>1</v>
-      </c>
-      <c r="H32" s="91">
-        <v>1</v>
-      </c>
-      <c r="I32" s="91">
+      <c r="G32" s="103">
+        <v>1</v>
+      </c>
+      <c r="H32" s="103">
+        <v>1</v>
+      </c>
+      <c r="I32" s="103">
         <v>2</v>
       </c>
-      <c r="J32" s="91"/>
-      <c r="K32" s="94"/>
-      <c r="L32" s="95">
+      <c r="J32" s="103"/>
+      <c r="K32" s="106"/>
+      <c r="L32" s="107">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M32" s="158"/>
-      <c r="N32" s="91">
+      <c r="M32" s="108"/>
+      <c r="N32" s="103">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O32" s="96"/>
-      <c r="P32" s="174"/>
-      <c r="S32"/>
+      <c r="O32" s="109"/>
+      <c r="P32" s="110"/>
+      <c r="S32" s="5"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="191"/>
-      <c r="B33" s="196"/>
-      <c r="C33" s="199"/>
-      <c r="D33" s="98" t="s">
+      <c r="A33" s="203"/>
+      <c r="B33" s="195"/>
+      <c r="C33" s="207"/>
+      <c r="D33" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="99">
+      <c r="E33" s="112">
         <v>4</v>
       </c>
-      <c r="F33" s="100">
+      <c r="F33" s="113">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G33" s="98"/>
-      <c r="H33" s="98"/>
-      <c r="I33" s="98"/>
-      <c r="J33" s="98">
-        <v>1</v>
-      </c>
-      <c r="K33" s="101"/>
-      <c r="L33" s="102">
+      <c r="G33" s="111"/>
+      <c r="H33" s="111"/>
+      <c r="I33" s="111"/>
+      <c r="J33" s="111">
+        <v>1</v>
+      </c>
+      <c r="K33" s="114"/>
+      <c r="L33" s="115">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M33" s="159"/>
-      <c r="N33" s="98">
+      <c r="M33" s="116"/>
+      <c r="N33" s="111">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="O33" s="103"/>
-      <c r="P33" s="175"/>
-      <c r="S33"/>
+      <c r="O33" s="117"/>
+      <c r="P33" s="118"/>
+      <c r="S33" s="5"/>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="191"/>
-      <c r="B34" s="196"/>
-      <c r="C34" s="199"/>
-      <c r="D34" s="91" t="s">
+      <c r="A34" s="203"/>
+      <c r="B34" s="195"/>
+      <c r="C34" s="207"/>
+      <c r="D34" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="92">
+      <c r="E34" s="104">
         <v>2</v>
       </c>
-      <c r="F34" s="93">
+      <c r="F34" s="105">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G34" s="91"/>
-      <c r="H34" s="91"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="91">
-        <v>1</v>
-      </c>
-      <c r="K34" s="94"/>
-      <c r="L34" s="95">
+      <c r="G34" s="103"/>
+      <c r="H34" s="103"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="103">
+        <v>1</v>
+      </c>
+      <c r="K34" s="106"/>
+      <c r="L34" s="107">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M34" s="158"/>
-      <c r="N34" s="91">
+      <c r="M34" s="108"/>
+      <c r="N34" s="103">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O34" s="96"/>
-      <c r="P34" s="174"/>
-      <c r="S34"/>
+      <c r="O34" s="109"/>
+      <c r="P34" s="110"/>
+      <c r="S34" s="5"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="191"/>
-      <c r="B35" s="196"/>
-      <c r="C35" s="199"/>
-      <c r="D35" s="118" t="s">
+      <c r="A35" s="203"/>
+      <c r="B35" s="195"/>
+      <c r="C35" s="207"/>
+      <c r="D35" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="119">
-        <v>1</v>
-      </c>
-      <c r="F35" s="120">
+      <c r="E35" s="136">
+        <v>1</v>
+      </c>
+      <c r="F35" s="137">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="121"/>
-      <c r="L35" s="122">
+      <c r="G35" s="135"/>
+      <c r="H35" s="135"/>
+      <c r="I35" s="135"/>
+      <c r="J35" s="135"/>
+      <c r="K35" s="138"/>
+      <c r="L35" s="139">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M35" s="162"/>
-      <c r="N35" s="118">
+      <c r="M35" s="140"/>
+      <c r="N35" s="135">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O35" s="123"/>
-      <c r="P35" s="178"/>
-      <c r="S35"/>
+      <c r="O35" s="141"/>
+      <c r="P35" s="142"/>
+      <c r="S35" s="5"/>
     </row>
     <row r="36" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="201" t="s">
+      <c r="A36" s="190" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="202" t="s">
+      <c r="B36" s="191" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="203" t="s">
+      <c r="C36" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="125" t="s">
+      <c r="D36" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="126">
+      <c r="E36" s="144">
         <v>10</v>
       </c>
-      <c r="F36" s="127">
+      <c r="F36" s="145">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G36" s="125">
-        <v>1</v>
-      </c>
-      <c r="H36" s="125">
+      <c r="G36" s="143">
+        <v>1</v>
+      </c>
+      <c r="H36" s="143">
         <v>2</v>
       </c>
-      <c r="I36" s="125">
+      <c r="I36" s="143">
         <v>2</v>
       </c>
-      <c r="J36" s="125">
-        <v>1</v>
-      </c>
-      <c r="K36" s="128"/>
-      <c r="L36" s="129"/>
-      <c r="M36" s="163"/>
-      <c r="N36" s="125"/>
-      <c r="O36" s="130">
+      <c r="J36" s="143">
+        <v>1</v>
+      </c>
+      <c r="K36" s="146"/>
+      <c r="L36" s="147"/>
+      <c r="M36" s="148"/>
+      <c r="N36" s="143"/>
+      <c r="O36" s="149">
         <f>49.18-(49.18*10/100)</f>
         <v>44.262</v>
       </c>
-      <c r="P36" s="131"/>
-      <c r="S36"/>
+      <c r="P36" s="150"/>
+      <c r="S36" s="5"/>
     </row>
     <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="201"/>
-      <c r="B37" s="202"/>
-      <c r="C37" s="203"/>
-      <c r="D37" s="26" t="s">
+      <c r="A37" s="190"/>
+      <c r="B37" s="191"/>
+      <c r="C37" s="192"/>
+      <c r="D37" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="27">
+      <c r="E37" s="28">
         <v>13</v>
       </c>
       <c r="F37" s="20">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26">
-        <v>1</v>
-      </c>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26">
+        <v>5</v>
+      </c>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27">
+        <v>1</v>
+      </c>
+      <c r="I37" s="27">
+        <v>3</v>
+      </c>
+      <c r="J37" s="27">
         <v>4</v>
       </c>
-      <c r="K37" s="29"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="150"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="32"/>
-      <c r="S37"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="82"/>
+      <c r="S37" s="5"/>
     </row>
     <row r="38" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="201"/>
-      <c r="B38" s="202"/>
-      <c r="C38" s="203"/>
+      <c r="A38" s="190"/>
+      <c r="B38" s="191"/>
+      <c r="C38" s="192"/>
       <c r="D38" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="19">
         <v>6</v>
       </c>
-      <c r="F38" s="28">
+      <c r="F38" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="I38" s="18">
+        <v>2</v>
+      </c>
       <c r="J38" s="18"/>
       <c r="K38" s="21"/>
       <c r="L38" s="22"/>
-      <c r="M38" s="149"/>
+      <c r="M38" s="23"/>
       <c r="N38" s="18"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="24"/>
-      <c r="S38"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="151"/>
+      <c r="S38" s="5"/>
     </row>
     <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="201"/>
-      <c r="B39" s="202"/>
-      <c r="C39" s="203"/>
-      <c r="D39" s="33" t="s">
+      <c r="A39" s="190"/>
+      <c r="B39" s="191"/>
+      <c r="C39" s="192"/>
+      <c r="D39" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E39" s="36">
         <v>3</v>
       </c>
-      <c r="F39" s="35">
+      <c r="F39" s="37">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="36">
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="38">
         <v>2</v>
       </c>
-      <c r="L39" s="37"/>
-      <c r="M39" s="151"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="38"/>
-      <c r="P39" s="39"/>
-      <c r="S39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="152"/>
+      <c r="S39" s="5"/>
     </row>
     <row r="40" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="201"/>
-      <c r="B40" s="202"/>
-      <c r="C40" s="194" t="s">
+      <c r="A40" s="190"/>
+      <c r="B40" s="191"/>
+      <c r="C40" s="193" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="41">
+      <c r="E40" s="44">
         <v>4</v>
       </c>
-      <c r="F40" s="42">
+      <c r="F40" s="45">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40">
-        <v>1</v>
-      </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="152"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="45">
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43">
+        <v>1</v>
+      </c>
+      <c r="J40" s="43"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="49">
         <f>56.01-(56.01*10/100)</f>
         <v>50.408999999999999</v>
       </c>
-      <c r="P40" s="46"/>
-      <c r="S40"/>
+      <c r="P40" s="153"/>
+      <c r="S40" s="5"/>
     </row>
     <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="201"/>
-      <c r="B41" s="202"/>
-      <c r="C41" s="194"/>
-      <c r="D41" s="47" t="s">
+      <c r="A41" s="190"/>
+      <c r="B41" s="191"/>
+      <c r="C41" s="193"/>
+      <c r="D41" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="48">
+      <c r="E41" s="52">
         <v>4</v>
       </c>
-      <c r="F41" s="49">
+      <c r="F41" s="53">
         <f t="shared" ref="F41:F60" si="3">E41-G41-H41-I41-J41-K41</f>
         <v>2</v>
       </c>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47">
-        <v>1</v>
-      </c>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47">
-        <v>1</v>
-      </c>
-      <c r="K41" s="50"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="153"/>
-      <c r="N41" s="47"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="53"/>
-      <c r="S41"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51">
+        <v>1</v>
+      </c>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51">
+        <v>1</v>
+      </c>
+      <c r="K41" s="54"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="51"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="154"/>
+      <c r="S41" s="5"/>
     </row>
     <row r="42" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="201"/>
-      <c r="B42" s="202"/>
-      <c r="C42" s="194"/>
-      <c r="D42" s="54" t="s">
+      <c r="A42" s="190"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="193"/>
+      <c r="D42" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="55">
+      <c r="E42" s="60">
         <v>0</v>
       </c>
-      <c r="F42" s="56">
+      <c r="F42" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="57"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="154"/>
-      <c r="N42" s="54"/>
-      <c r="O42" s="59"/>
-      <c r="P42" s="60"/>
-      <c r="S42"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="64"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="65"/>
+      <c r="P42" s="155"/>
+      <c r="S42" s="5"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="201"/>
-      <c r="B43" s="202"/>
-      <c r="C43" s="194"/>
-      <c r="D43" s="61" t="s">
+      <c r="A43" s="190"/>
+      <c r="B43" s="191"/>
+      <c r="C43" s="193"/>
+      <c r="D43" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="62">
+      <c r="E43" s="68">
         <v>2</v>
       </c>
-      <c r="F43" s="63">
+      <c r="F43" s="69">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="64">
-        <v>1</v>
-      </c>
-      <c r="L43" s="65"/>
-      <c r="M43" s="155"/>
-      <c r="N43" s="61"/>
-      <c r="O43" s="66"/>
-      <c r="P43" s="67"/>
-      <c r="S43"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="70">
+        <v>1</v>
+      </c>
+      <c r="L43" s="71"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="67"/>
+      <c r="O43" s="73"/>
+      <c r="P43" s="156"/>
+      <c r="S43" s="5"/>
     </row>
     <row r="44" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="201"/>
-      <c r="B44" s="202"/>
-      <c r="C44" s="195" t="s">
+      <c r="A44" s="190"/>
+      <c r="B44" s="191"/>
+      <c r="C44" s="194" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="68">
+      <c r="E44" s="75">
         <v>3</v>
       </c>
       <c r="F44" s="20">
@@ -4518,534 +4856,531 @@
       </c>
       <c r="K44" s="21"/>
       <c r="L44" s="22"/>
-      <c r="M44" s="149"/>
+      <c r="M44" s="23"/>
       <c r="N44" s="18"/>
-      <c r="O44" s="23">
+      <c r="O44" s="24">
         <f>50.08-(50.08*10/100)</f>
         <v>45.072000000000003</v>
       </c>
-      <c r="P44" s="24"/>
-      <c r="S44"/>
+      <c r="P44" s="151"/>
+      <c r="S44" s="5"/>
     </row>
     <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="201"/>
-      <c r="B45" s="202"/>
-      <c r="C45" s="195"/>
-      <c r="D45" s="69" t="s">
+      <c r="A45" s="190"/>
+      <c r="B45" s="191"/>
+      <c r="C45" s="194"/>
+      <c r="D45" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="70">
+      <c r="E45" s="81">
         <v>8</v>
       </c>
-      <c r="F45" s="28">
+      <c r="F45" s="29">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G45" s="69">
-        <v>1</v>
-      </c>
-      <c r="H45" s="69"/>
-      <c r="I45" s="69">
+      <c r="G45" s="80">
+        <v>1</v>
+      </c>
+      <c r="H45" s="80"/>
+      <c r="I45" s="80">
         <v>2</v>
       </c>
-      <c r="J45" s="69">
-        <v>1</v>
-      </c>
-      <c r="K45" s="71"/>
-      <c r="L45" s="72"/>
-      <c r="M45" s="69"/>
-      <c r="N45" s="69"/>
-      <c r="O45" s="73"/>
-      <c r="P45" s="74"/>
-      <c r="S45"/>
+      <c r="J45" s="80">
+        <v>1</v>
+      </c>
+      <c r="K45" s="157"/>
+      <c r="L45" s="158"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="159"/>
+      <c r="P45" s="160"/>
+      <c r="S45" s="5"/>
     </row>
     <row r="46" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="201"/>
-      <c r="B46" s="202"/>
-      <c r="C46" s="195"/>
-      <c r="D46" s="75" t="s">
+      <c r="A46" s="190"/>
+      <c r="B46" s="191"/>
+      <c r="C46" s="194"/>
+      <c r="D46" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="76">
+      <c r="E46" s="84">
         <v>13</v>
       </c>
-      <c r="F46" s="28">
+      <c r="F46" s="29">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="G46" s="75"/>
-      <c r="H46" s="75">
+        <v>7</v>
+      </c>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83">
         <v>3</v>
       </c>
-      <c r="I46" s="75"/>
-      <c r="J46" s="75">
+      <c r="I46" s="83">
+        <v>1</v>
+      </c>
+      <c r="J46" s="83">
         <v>2</v>
       </c>
-      <c r="K46" s="77"/>
-      <c r="L46" s="78"/>
-      <c r="M46" s="156"/>
-      <c r="N46" s="75"/>
-      <c r="O46" s="79"/>
-      <c r="P46" s="80"/>
-      <c r="S46"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="161"/>
+      <c r="M46" s="86"/>
+      <c r="N46" s="83"/>
+      <c r="O46" s="87"/>
+      <c r="P46" s="162"/>
+      <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="201"/>
-      <c r="B47" s="202"/>
-      <c r="C47" s="195"/>
-      <c r="D47" s="69" t="s">
+      <c r="A47" s="190"/>
+      <c r="B47" s="191"/>
+      <c r="C47" s="194"/>
+      <c r="D47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="70">
+      <c r="E47" s="81">
         <v>7</v>
       </c>
-      <c r="F47" s="28">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="G47" s="69"/>
-      <c r="H47" s="69"/>
-      <c r="I47" s="69"/>
-      <c r="J47" s="69">
-        <v>1</v>
-      </c>
-      <c r="K47" s="71"/>
-      <c r="L47" s="72"/>
-      <c r="M47" s="69"/>
-      <c r="N47" s="69"/>
-      <c r="O47" s="73"/>
-      <c r="P47" s="74"/>
-      <c r="S47"/>
-    </row>
-    <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="201"/>
-      <c r="B48" s="202"/>
-      <c r="C48" s="195"/>
-      <c r="D48" s="75" t="s">
-        <v>29</v>
-      </c>
-      <c r="E48" s="76">
-        <v>7</v>
-      </c>
-      <c r="F48" s="28">
+      <c r="F47" s="29">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G48" s="75"/>
-      <c r="H48" s="75"/>
-      <c r="I48" s="75"/>
-      <c r="J48" s="75">
+      <c r="G47" s="80"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="80">
+        <v>3</v>
+      </c>
+      <c r="J47" s="80">
+        <v>1</v>
+      </c>
+      <c r="K47" s="157"/>
+      <c r="L47" s="158"/>
+      <c r="M47" s="80"/>
+      <c r="N47" s="80"/>
+      <c r="O47" s="159"/>
+      <c r="P47" s="160"/>
+      <c r="S47" s="5"/>
+    </row>
+    <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="190"/>
+      <c r="B48" s="191"/>
+      <c r="C48" s="194"/>
+      <c r="D48" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="84">
+        <v>7</v>
+      </c>
+      <c r="F48" s="29">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="K48" s="77">
+      <c r="G48" s="83"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="83">
+        <v>1</v>
+      </c>
+      <c r="J48" s="83">
         <v>2</v>
       </c>
-      <c r="L48" s="78"/>
-      <c r="M48" s="156"/>
-      <c r="N48" s="75"/>
-      <c r="O48" s="79"/>
-      <c r="P48" s="80"/>
-      <c r="S48"/>
+      <c r="K48" s="85">
+        <v>2</v>
+      </c>
+      <c r="L48" s="161"/>
+      <c r="M48" s="86"/>
+      <c r="N48" s="83"/>
+      <c r="O48" s="87"/>
+      <c r="P48" s="162"/>
+      <c r="S48" s="5"/>
     </row>
     <row r="49" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="201"/>
-      <c r="B49" s="196" t="s">
+      <c r="A49" s="190"/>
+      <c r="B49" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="197" t="s">
+      <c r="C49" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="84" t="s">
+      <c r="D49" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="85">
+      <c r="E49" s="96">
         <v>4</v>
       </c>
-      <c r="F49" s="86">
+      <c r="F49" s="97">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G49" s="84">
+      <c r="G49" s="95">
         <v>2</v>
       </c>
-      <c r="H49" s="84"/>
-      <c r="I49" s="84"/>
-      <c r="J49" s="84">
-        <v>1</v>
-      </c>
-      <c r="K49" s="87"/>
-      <c r="L49" s="88"/>
-      <c r="M49" s="157"/>
-      <c r="N49" s="84"/>
-      <c r="O49" s="89">
+      <c r="H49" s="95"/>
+      <c r="I49" s="95"/>
+      <c r="J49" s="95">
+        <v>1</v>
+      </c>
+      <c r="K49" s="98"/>
+      <c r="L49" s="99"/>
+      <c r="M49" s="100"/>
+      <c r="N49" s="95"/>
+      <c r="O49" s="101">
         <f>48.02-(48.02*10/100)</f>
         <v>43.218000000000004</v>
       </c>
-      <c r="P49" s="90"/>
-      <c r="S49"/>
+      <c r="P49" s="163"/>
+      <c r="S49" s="5"/>
     </row>
     <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="201"/>
-      <c r="B50" s="196"/>
-      <c r="C50" s="197"/>
-      <c r="D50" s="91" t="s">
+      <c r="A50" s="190"/>
+      <c r="B50" s="195"/>
+      <c r="C50" s="196"/>
+      <c r="D50" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="92">
+      <c r="E50" s="104">
         <v>5</v>
       </c>
-      <c r="F50" s="93">
+      <c r="F50" s="105">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G50" s="91"/>
-      <c r="H50" s="91"/>
-      <c r="I50" s="91"/>
-      <c r="J50" s="91">
-        <v>1</v>
-      </c>
-      <c r="K50" s="94"/>
-      <c r="L50" s="95"/>
-      <c r="M50" s="158"/>
-      <c r="N50" s="91"/>
-      <c r="O50" s="96"/>
-      <c r="P50" s="97"/>
-      <c r="S50"/>
+      <c r="G50" s="103"/>
+      <c r="H50" s="103"/>
+      <c r="I50" s="103"/>
+      <c r="J50" s="103">
+        <v>1</v>
+      </c>
+      <c r="K50" s="106"/>
+      <c r="L50" s="107"/>
+      <c r="M50" s="108"/>
+      <c r="N50" s="103"/>
+      <c r="O50" s="109"/>
+      <c r="P50" s="164"/>
+      <c r="S50" s="5"/>
     </row>
     <row r="51" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="201"/>
-      <c r="B51" s="196"/>
-      <c r="C51" s="197"/>
-      <c r="D51" s="98" t="s">
+      <c r="A51" s="190"/>
+      <c r="B51" s="195"/>
+      <c r="C51" s="196"/>
+      <c r="D51" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="99">
-        <v>1</v>
-      </c>
-      <c r="F51" s="100">
+      <c r="E51" s="112">
+        <v>1</v>
+      </c>
+      <c r="F51" s="113">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G51" s="98"/>
-      <c r="H51" s="98"/>
-      <c r="I51" s="98"/>
-      <c r="J51" s="98"/>
-      <c r="K51" s="101"/>
-      <c r="L51" s="102"/>
-      <c r="M51" s="159"/>
-      <c r="N51" s="98"/>
-      <c r="O51" s="103"/>
-      <c r="P51" s="104"/>
-      <c r="S51"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="111"/>
+      <c r="K51" s="114"/>
+      <c r="L51" s="115"/>
+      <c r="M51" s="116"/>
+      <c r="N51" s="111"/>
+      <c r="O51" s="117"/>
+      <c r="P51" s="165"/>
+      <c r="S51" s="5"/>
     </row>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="201"/>
-      <c r="B52" s="196"/>
-      <c r="C52" s="197"/>
-      <c r="D52" s="91" t="s">
+      <c r="A52" s="190"/>
+      <c r="B52" s="195"/>
+      <c r="C52" s="196"/>
+      <c r="D52" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="92">
+      <c r="E52" s="104">
         <v>0</v>
       </c>
-      <c r="F52" s="93">
+      <c r="F52" s="105">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G52" s="91"/>
-      <c r="H52" s="91"/>
-      <c r="I52" s="91"/>
-      <c r="J52" s="91"/>
-      <c r="K52" s="94"/>
-      <c r="L52" s="95"/>
-      <c r="M52" s="158"/>
-      <c r="N52" s="91"/>
-      <c r="O52" s="96"/>
-      <c r="P52" s="97"/>
-      <c r="S52"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="103"/>
+      <c r="J52" s="103"/>
+      <c r="K52" s="106"/>
+      <c r="L52" s="107"/>
+      <c r="M52" s="108"/>
+      <c r="N52" s="103"/>
+      <c r="O52" s="109"/>
+      <c r="P52" s="164"/>
+      <c r="S52" s="5"/>
     </row>
     <row r="53" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="201"/>
-      <c r="B53" s="196"/>
-      <c r="C53" s="197"/>
-      <c r="D53" s="105" t="s">
+      <c r="A53" s="190"/>
+      <c r="B53" s="195"/>
+      <c r="C53" s="196"/>
+      <c r="D53" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="106">
+      <c r="E53" s="120">
         <v>0</v>
       </c>
-      <c r="F53" s="107">
+      <c r="F53" s="121">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G53" s="105"/>
-      <c r="H53" s="105"/>
-      <c r="I53" s="105"/>
-      <c r="J53" s="105"/>
-      <c r="K53" s="108"/>
-      <c r="L53" s="109"/>
-      <c r="M53" s="160"/>
-      <c r="N53" s="105"/>
-      <c r="O53" s="110"/>
-      <c r="P53" s="111"/>
-      <c r="S53"/>
+      <c r="G53" s="119"/>
+      <c r="H53" s="119"/>
+      <c r="I53" s="119"/>
+      <c r="J53" s="119"/>
+      <c r="K53" s="122"/>
+      <c r="L53" s="123"/>
+      <c r="M53" s="124"/>
+      <c r="N53" s="119"/>
+      <c r="O53" s="125"/>
+      <c r="P53" s="166"/>
+      <c r="S53" s="5"/>
     </row>
     <row r="54" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="201"/>
-      <c r="B54" s="196"/>
-      <c r="C54" s="204" t="s">
+      <c r="A54" s="190"/>
+      <c r="B54" s="195"/>
+      <c r="C54" s="197" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="84" t="s">
+      <c r="D54" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="E54" s="85">
+      <c r="E54" s="96">
         <v>4</v>
       </c>
-      <c r="F54" s="86">
+      <c r="F54" s="97">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G54" s="84">
-        <v>1</v>
-      </c>
-      <c r="H54" s="84"/>
-      <c r="I54" s="84"/>
-      <c r="J54" s="84"/>
-      <c r="K54" s="87"/>
-      <c r="L54" s="88"/>
-      <c r="M54" s="157"/>
-      <c r="N54" s="84"/>
-      <c r="O54" s="89">
+      <c r="G54" s="95">
+        <v>1</v>
+      </c>
+      <c r="H54" s="95"/>
+      <c r="I54" s="95"/>
+      <c r="J54" s="95"/>
+      <c r="K54" s="98"/>
+      <c r="L54" s="99"/>
+      <c r="M54" s="100"/>
+      <c r="N54" s="95"/>
+      <c r="O54" s="101">
         <f>54.85-(54.85*10/100)</f>
         <v>49.365000000000002</v>
       </c>
-      <c r="P54" s="90"/>
-      <c r="S54"/>
+      <c r="P54" s="163"/>
+      <c r="S54" s="5"/>
     </row>
     <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="201"/>
-      <c r="B55" s="196"/>
-      <c r="C55" s="204"/>
-      <c r="D55" s="91" t="s">
+      <c r="A55" s="190"/>
+      <c r="B55" s="195"/>
+      <c r="C55" s="197"/>
+      <c r="D55" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="E55" s="92">
+      <c r="E55" s="104">
         <v>5</v>
       </c>
-      <c r="F55" s="93">
+      <c r="F55" s="105">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G55" s="91"/>
-      <c r="H55" s="91"/>
-      <c r="I55" s="91"/>
-      <c r="J55" s="91">
-        <v>1</v>
-      </c>
-      <c r="K55" s="94"/>
-      <c r="L55" s="95"/>
-      <c r="M55" s="158"/>
-      <c r="N55" s="91"/>
-      <c r="O55" s="96"/>
-      <c r="P55" s="97"/>
-      <c r="S55"/>
+      <c r="G55" s="103"/>
+      <c r="H55" s="103"/>
+      <c r="I55" s="103"/>
+      <c r="J55" s="103">
+        <v>1</v>
+      </c>
+      <c r="K55" s="106"/>
+      <c r="L55" s="107"/>
+      <c r="M55" s="108"/>
+      <c r="N55" s="103"/>
+      <c r="O55" s="109"/>
+      <c r="P55" s="164"/>
+      <c r="S55" s="5"/>
     </row>
     <row r="56" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="201"/>
-      <c r="B56" s="196"/>
-      <c r="C56" s="204"/>
-      <c r="D56" s="98" t="s">
+      <c r="A56" s="190"/>
+      <c r="B56" s="195"/>
+      <c r="C56" s="197"/>
+      <c r="D56" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="99">
-        <v>1</v>
-      </c>
-      <c r="F56" s="100">
+      <c r="E56" s="112">
+        <v>1</v>
+      </c>
+      <c r="F56" s="113">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G56" s="98"/>
-      <c r="H56" s="98"/>
-      <c r="I56" s="98"/>
-      <c r="J56" s="98"/>
-      <c r="K56" s="101"/>
-      <c r="L56" s="102"/>
-      <c r="M56" s="159"/>
-      <c r="N56" s="98"/>
-      <c r="O56" s="103"/>
-      <c r="P56" s="104"/>
-      <c r="S56"/>
+      <c r="G56" s="111"/>
+      <c r="H56" s="111"/>
+      <c r="I56" s="111"/>
+      <c r="J56" s="111"/>
+      <c r="K56" s="114"/>
+      <c r="L56" s="115"/>
+      <c r="M56" s="116"/>
+      <c r="N56" s="111"/>
+      <c r="O56" s="117"/>
+      <c r="P56" s="165"/>
+      <c r="S56" s="5"/>
     </row>
     <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="201"/>
-      <c r="B57" s="196"/>
-      <c r="C57" s="204"/>
-      <c r="D57" s="91" t="s">
+      <c r="A57" s="190"/>
+      <c r="B57" s="195"/>
+      <c r="C57" s="197"/>
+      <c r="D57" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E57" s="92">
+      <c r="E57" s="104">
         <v>0</v>
       </c>
-      <c r="F57" s="93">
+      <c r="F57" s="105">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G57" s="91"/>
-      <c r="H57" s="91"/>
-      <c r="I57" s="91"/>
-      <c r="J57" s="91"/>
-      <c r="K57" s="94"/>
-      <c r="L57" s="95"/>
-      <c r="M57" s="158"/>
-      <c r="N57" s="91"/>
-      <c r="O57" s="96"/>
-      <c r="P57" s="97"/>
-      <c r="S57"/>
+      <c r="G57" s="103"/>
+      <c r="H57" s="103"/>
+      <c r="I57" s="103"/>
+      <c r="J57" s="103"/>
+      <c r="K57" s="106"/>
+      <c r="L57" s="107"/>
+      <c r="M57" s="108"/>
+      <c r="N57" s="103"/>
+      <c r="O57" s="109"/>
+      <c r="P57" s="164"/>
+      <c r="S57" s="5"/>
     </row>
     <row r="58" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="201"/>
-      <c r="B58" s="196"/>
-      <c r="C58" s="205"/>
-      <c r="D58" s="118" t="s">
+      <c r="A58" s="190"/>
+      <c r="B58" s="195"/>
+      <c r="C58" s="198"/>
+      <c r="D58" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="E58" s="119">
+      <c r="E58" s="136">
         <v>0</v>
       </c>
-      <c r="F58" s="120">
+      <c r="F58" s="137">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G58" s="118"/>
-      <c r="H58" s="118"/>
-      <c r="I58" s="118"/>
-      <c r="J58" s="118"/>
-      <c r="K58" s="121"/>
-      <c r="L58" s="122"/>
-      <c r="M58" s="162"/>
-      <c r="N58" s="118"/>
-      <c r="O58" s="123"/>
-      <c r="P58" s="124"/>
-      <c r="S58"/>
+      <c r="G58" s="135"/>
+      <c r="H58" s="135"/>
+      <c r="I58" s="135"/>
+      <c r="J58" s="135"/>
+      <c r="K58" s="138"/>
+      <c r="L58" s="139"/>
+      <c r="M58" s="140"/>
+      <c r="N58" s="135"/>
+      <c r="O58" s="141"/>
+      <c r="P58" s="167"/>
+      <c r="S58" s="5"/>
     </row>
     <row r="59" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="C59" s="200" t="s">
+      <c r="A59" s="5"/>
+      <c r="C59" s="189" t="s">
         <v>36</v>
       </c>
-      <c r="D59" s="132" t="s">
+      <c r="D59" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="133">
+      <c r="E59" s="169">
         <v>36</v>
       </c>
-      <c r="F59" s="134">
+      <c r="F59" s="170">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="G59" s="135">
+      <c r="G59" s="171">
         <v>2</v>
       </c>
-      <c r="H59" s="135"/>
-      <c r="I59" s="135">
+      <c r="H59" s="171"/>
+      <c r="I59" s="171">
         <v>10</v>
       </c>
-      <c r="J59" s="135">
+      <c r="J59" s="171">
         <v>2</v>
       </c>
-      <c r="K59" s="136"/>
-      <c r="L59" s="137"/>
-      <c r="M59" s="137"/>
-      <c r="N59" s="135"/>
-      <c r="O59" s="138">
+      <c r="K59" s="172"/>
+      <c r="L59" s="173"/>
+      <c r="M59" s="173"/>
+      <c r="N59" s="171"/>
+      <c r="O59" s="174">
         <v>4.6500000000000004</v>
       </c>
-      <c r="P59" s="139"/>
-      <c r="S59" s="25"/>
+      <c r="P59" s="175"/>
+      <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60"/>
-      <c r="C60" s="200"/>
-      <c r="D60" s="140" t="s">
+      <c r="A60" s="5"/>
+      <c r="C60" s="189"/>
+      <c r="D60" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="141">
+      <c r="E60" s="177">
         <v>64</v>
       </c>
-      <c r="F60" s="142">
+      <c r="F60" s="178">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="G60" s="143"/>
-      <c r="H60" s="143">
+      <c r="G60" s="179"/>
+      <c r="H60" s="179">
         <v>5</v>
       </c>
-      <c r="I60" s="143"/>
-      <c r="J60" s="143">
+      <c r="I60" s="179"/>
+      <c r="J60" s="179">
         <v>8</v>
       </c>
-      <c r="K60" s="144">
+      <c r="K60" s="180">
         <v>2</v>
       </c>
-      <c r="L60" s="145"/>
-      <c r="M60" s="145"/>
-      <c r="N60" s="146"/>
-      <c r="O60" s="147"/>
-      <c r="P60" s="148"/>
+      <c r="L60" s="181"/>
+      <c r="M60" s="181"/>
+      <c r="N60" s="182"/>
+      <c r="O60" s="183"/>
+      <c r="P60" s="184"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61"/>
+      <c r="A61" s="5"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A62"/>
+      <c r="A62" s="5"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A36:A58"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:P7"/>
@@ -5058,6 +5393,15 @@
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C35"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A36:A58"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Inventar aktualisiert, Christoph Birnbaum Trikot L für Gewinnspiel
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\___MYDATA\__KLINK\webprojects\cycling-adventures.org\2017 Reisen\"/>
@@ -50,7 +50,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Volker Laabs #1565</t>
+Volker Laabs #1565
+Gewinnspiel: Christoph Birnbaum</t>
         </r>
       </text>
     </comment>
@@ -2718,6 +2719,58 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2734,63 +2787,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3385,8 +3386,8 @@
   <dimension ref="A1:IX69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3462,7 +3463,7 @@
       </c>
       <c r="B4" s="8">
         <f ca="1">TODAY()</f>
-        <v>42724</v>
+        <v>42774</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -3522,30 +3523,30 @@
       <c r="S6" s="5"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="199" t="s">
+      <c r="A7" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="200"/>
-      <c r="C7" s="200"/>
-      <c r="D7" s="200"/>
-      <c r="E7" s="200"/>
-      <c r="F7" s="201" t="s">
+      <c r="B7" s="190"/>
+      <c r="C7" s="190"/>
+      <c r="D7" s="190"/>
+      <c r="E7" s="190"/>
+      <c r="F7" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="201"/>
-      <c r="H7" s="201"/>
-      <c r="I7" s="201"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="201"/>
-      <c r="L7" s="201" t="s">
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
+      <c r="L7" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="201"/>
-      <c r="N7" s="201" t="s">
+      <c r="M7" s="191"/>
+      <c r="N7" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="201"/>
-      <c r="P7" s="202"/>
+      <c r="O7" s="191"/>
+      <c r="P7" s="192"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
@@ -3602,13 +3603,13 @@
       <c r="S8" s="5"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="203" t="s">
+      <c r="A9" s="193" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="205" t="s">
+      <c r="C9" s="195" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -3650,9 +3651,9 @@
       <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
-      <c r="C10" s="205"/>
+      <c r="A10" s="193"/>
+      <c r="B10" s="194"/>
+      <c r="C10" s="195"/>
       <c r="D10" s="27" t="s">
         <v>27</v>
       </c>
@@ -3675,11 +3676,11 @@
         <v>15</v>
       </c>
       <c r="M10" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="27">
         <f t="shared" ref="N10:N35" si="2">L10-M10</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O10" s="33"/>
       <c r="P10" s="34"/>
@@ -3687,9 +3688,9 @@
       <c r="S10" s="5"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="203"/>
-      <c r="B11" s="204"/>
-      <c r="C11" s="205"/>
+      <c r="A11" s="193"/>
+      <c r="B11" s="194"/>
+      <c r="C11" s="195"/>
       <c r="D11" s="18" t="s">
         <v>28</v>
       </c>
@@ -3698,21 +3699,23 @@
       </c>
       <c r="F11" s="29">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="J11" s="18">
+        <v>2</v>
+      </c>
       <c r="K11" s="21"/>
       <c r="L11" s="22">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M11" s="23"/>
       <c r="N11" s="18">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O11" s="24"/>
       <c r="P11" s="25"/>
@@ -3720,9 +3723,9 @@
       <c r="S11" s="5"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="203"/>
-      <c r="B12" s="204"/>
-      <c r="C12" s="205"/>
+      <c r="A12" s="193"/>
+      <c r="B12" s="194"/>
+      <c r="C12" s="195"/>
       <c r="D12" s="35" t="s">
         <v>29</v>
       </c>
@@ -3755,9 +3758,9 @@
       <c r="S12" s="5"/>
     </row>
     <row r="13" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="203"/>
-      <c r="B13" s="204"/>
-      <c r="C13" s="193" t="s">
+      <c r="A13" s="193"/>
+      <c r="B13" s="194"/>
+      <c r="C13" s="196" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="43" t="s">
@@ -3797,9 +3800,9 @@
       <c r="S13" s="5"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="203"/>
-      <c r="B14" s="204"/>
-      <c r="C14" s="193"/>
+      <c r="A14" s="193"/>
+      <c r="B14" s="194"/>
+      <c r="C14" s="196"/>
       <c r="D14" s="51" t="s">
         <v>27</v>
       </c>
@@ -3835,9 +3838,9 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="203"/>
-      <c r="B15" s="204"/>
-      <c r="C15" s="193"/>
+      <c r="A15" s="193"/>
+      <c r="B15" s="194"/>
+      <c r="C15" s="196"/>
       <c r="D15" s="59" t="s">
         <v>28</v>
       </c>
@@ -3867,9 +3870,9 @@
       <c r="S15" s="5"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="203"/>
-      <c r="B16" s="204"/>
-      <c r="C16" s="193"/>
+      <c r="A16" s="193"/>
+      <c r="B16" s="194"/>
+      <c r="C16" s="196"/>
       <c r="D16" s="67" t="s">
         <v>29</v>
       </c>
@@ -3901,9 +3904,9 @@
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="203"/>
-      <c r="B17" s="204"/>
-      <c r="C17" s="194" t="s">
+      <c r="A17" s="193"/>
+      <c r="B17" s="194"/>
+      <c r="C17" s="197" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -3942,9 +3945,9 @@
       <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="203"/>
-      <c r="B18" s="204"/>
-      <c r="C18" s="194"/>
+      <c r="A18" s="193"/>
+      <c r="B18" s="194"/>
+      <c r="C18" s="197"/>
       <c r="D18" s="80" t="s">
         <v>27</v>
       </c>
@@ -3978,9 +3981,9 @@
       <c r="S18" s="5"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="203"/>
-      <c r="B19" s="204"/>
-      <c r="C19" s="194"/>
+      <c r="A19" s="193"/>
+      <c r="B19" s="194"/>
+      <c r="C19" s="197"/>
       <c r="D19" s="83" t="s">
         <v>28</v>
       </c>
@@ -3989,32 +3992,32 @@
       </c>
       <c r="F19" s="29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G19" s="83"/>
       <c r="H19" s="83"/>
       <c r="I19" s="83"/>
       <c r="J19" s="83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K19" s="85"/>
       <c r="L19" s="86">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M19" s="86"/>
       <c r="N19" s="83">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O19" s="87"/>
       <c r="P19" s="88"/>
       <c r="S19" s="5"/>
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="203"/>
-      <c r="B20" s="204"/>
-      <c r="C20" s="194"/>
+      <c r="A20" s="193"/>
+      <c r="B20" s="194"/>
+      <c r="C20" s="197"/>
       <c r="D20" s="89" t="s">
         <v>29</v>
       </c>
@@ -4048,11 +4051,11 @@
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="203"/>
-      <c r="B21" s="195" t="s">
+      <c r="A21" s="193"/>
+      <c r="B21" s="198" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="196" t="s">
+      <c r="C21" s="199" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="95" t="s">
@@ -4091,9 +4094,9 @@
       <c r="S21" s="5"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="203"/>
-      <c r="B22" s="195"/>
-      <c r="C22" s="196"/>
+      <c r="A22" s="193"/>
+      <c r="B22" s="198"/>
+      <c r="C22" s="199"/>
       <c r="D22" s="103" t="s">
         <v>34</v>
       </c>
@@ -4125,9 +4128,9 @@
       <c r="S22" s="5"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="203"/>
-      <c r="B23" s="195"/>
-      <c r="C23" s="196"/>
+      <c r="A23" s="193"/>
+      <c r="B23" s="198"/>
+      <c r="C23" s="199"/>
       <c r="D23" s="111" t="s">
         <v>26</v>
       </c>
@@ -4163,9 +4166,9 @@
       <c r="S23" s="5"/>
     </row>
     <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="203"/>
-      <c r="B24" s="195"/>
-      <c r="C24" s="196"/>
+      <c r="A24" s="193"/>
+      <c r="B24" s="198"/>
+      <c r="C24" s="199"/>
       <c r="D24" s="103" t="s">
         <v>27</v>
       </c>
@@ -4197,9 +4200,9 @@
       <c r="S24" s="5"/>
     </row>
     <row r="25" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="203"/>
-      <c r="B25" s="195"/>
-      <c r="C25" s="196"/>
+      <c r="A25" s="193"/>
+      <c r="B25" s="198"/>
+      <c r="C25" s="199"/>
       <c r="D25" s="119" t="s">
         <v>28</v>
       </c>
@@ -4231,9 +4234,9 @@
       <c r="S25" s="5"/>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="203"/>
-      <c r="B26" s="195"/>
-      <c r="C26" s="206" t="s">
+      <c r="A26" s="193"/>
+      <c r="B26" s="198"/>
+      <c r="C26" s="200" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="95" t="s">
@@ -4272,9 +4275,9 @@
       <c r="S26" s="5"/>
     </row>
     <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="203"/>
-      <c r="B27" s="195"/>
-      <c r="C27" s="206"/>
+      <c r="A27" s="193"/>
+      <c r="B27" s="198"/>
+      <c r="C27" s="200"/>
       <c r="D27" s="103" t="s">
         <v>34</v>
       </c>
@@ -4306,9 +4309,9 @@
       <c r="S27" s="5"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="203"/>
-      <c r="B28" s="195"/>
-      <c r="C28" s="206"/>
+      <c r="A28" s="193"/>
+      <c r="B28" s="198"/>
+      <c r="C28" s="200"/>
       <c r="D28" s="111" t="s">
         <v>26</v>
       </c>
@@ -4340,9 +4343,9 @@
       <c r="S28" s="5"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="203"/>
-      <c r="B29" s="195"/>
-      <c r="C29" s="206"/>
+      <c r="A29" s="193"/>
+      <c r="B29" s="198"/>
+      <c r="C29" s="200"/>
       <c r="D29" s="103" t="s">
         <v>27</v>
       </c>
@@ -4372,9 +4375,9 @@
       <c r="S29" s="5"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="203"/>
-      <c r="B30" s="195"/>
-      <c r="C30" s="206"/>
+      <c r="A30" s="193"/>
+      <c r="B30" s="198"/>
+      <c r="C30" s="200"/>
       <c r="D30" s="127" t="s">
         <v>28</v>
       </c>
@@ -4404,9 +4407,9 @@
       <c r="S30" s="5"/>
     </row>
     <row r="31" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="203"/>
-      <c r="B31" s="195"/>
-      <c r="C31" s="207" t="s">
+      <c r="A31" s="193"/>
+      <c r="B31" s="198"/>
+      <c r="C31" s="201" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="95" t="s">
@@ -4445,9 +4448,9 @@
       <c r="S31" s="5"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="203"/>
-      <c r="B32" s="195"/>
-      <c r="C32" s="207"/>
+      <c r="A32" s="193"/>
+      <c r="B32" s="198"/>
+      <c r="C32" s="201"/>
       <c r="D32" s="103" t="s">
         <v>26</v>
       </c>
@@ -4483,9 +4486,9 @@
       <c r="S32" s="5"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="203"/>
-      <c r="B33" s="195"/>
-      <c r="C33" s="207"/>
+      <c r="A33" s="193"/>
+      <c r="B33" s="198"/>
+      <c r="C33" s="201"/>
       <c r="D33" s="111" t="s">
         <v>27</v>
       </c>
@@ -4517,9 +4520,9 @@
       <c r="S33" s="5"/>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="203"/>
-      <c r="B34" s="195"/>
-      <c r="C34" s="207"/>
+      <c r="A34" s="193"/>
+      <c r="B34" s="198"/>
+      <c r="C34" s="201"/>
       <c r="D34" s="103" t="s">
         <v>28</v>
       </c>
@@ -4551,9 +4554,9 @@
       <c r="S34" s="5"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="203"/>
-      <c r="B35" s="195"/>
-      <c r="C35" s="207"/>
+      <c r="A35" s="193"/>
+      <c r="B35" s="198"/>
+      <c r="C35" s="201"/>
       <c r="D35" s="135" t="s">
         <v>29</v>
       </c>
@@ -4583,13 +4586,13 @@
       <c r="S35" s="5"/>
     </row>
     <row r="36" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="190" t="s">
+      <c r="A36" s="203" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="191" t="s">
+      <c r="B36" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="192" t="s">
+      <c r="C36" s="205" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="143" t="s">
@@ -4626,9 +4629,9 @@
       <c r="S36" s="5"/>
     </row>
     <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="190"/>
-      <c r="B37" s="191"/>
-      <c r="C37" s="192"/>
+      <c r="A37" s="203"/>
+      <c r="B37" s="204"/>
+      <c r="C37" s="205"/>
       <c r="D37" s="27" t="s">
         <v>27</v>
       </c>
@@ -4658,9 +4661,9 @@
       <c r="S37" s="5"/>
     </row>
     <row r="38" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="190"/>
-      <c r="B38" s="191"/>
-      <c r="C38" s="192"/>
+      <c r="A38" s="203"/>
+      <c r="B38" s="204"/>
+      <c r="C38" s="205"/>
       <c r="D38" s="18" t="s">
         <v>28</v>
       </c>
@@ -4686,9 +4689,9 @@
       <c r="S38" s="5"/>
     </row>
     <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="190"/>
-      <c r="B39" s="191"/>
-      <c r="C39" s="192"/>
+      <c r="A39" s="203"/>
+      <c r="B39" s="204"/>
+      <c r="C39" s="205"/>
       <c r="D39" s="35" t="s">
         <v>29</v>
       </c>
@@ -4714,9 +4717,9 @@
       <c r="S39" s="5"/>
     </row>
     <row r="40" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="190"/>
-      <c r="B40" s="191"/>
-      <c r="C40" s="193" t="s">
+      <c r="A40" s="203"/>
+      <c r="B40" s="204"/>
+      <c r="C40" s="196" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="43" t="s">
@@ -4747,9 +4750,9 @@
       <c r="S40" s="5"/>
     </row>
     <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="190"/>
-      <c r="B41" s="191"/>
-      <c r="C41" s="193"/>
+      <c r="A41" s="203"/>
+      <c r="B41" s="204"/>
+      <c r="C41" s="196"/>
       <c r="D41" s="51" t="s">
         <v>27</v>
       </c>
@@ -4777,9 +4780,9 @@
       <c r="S41" s="5"/>
     </row>
     <row r="42" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="190"/>
-      <c r="B42" s="191"/>
-      <c r="C42" s="193"/>
+      <c r="A42" s="203"/>
+      <c r="B42" s="204"/>
+      <c r="C42" s="196"/>
       <c r="D42" s="59" t="s">
         <v>28</v>
       </c>
@@ -4803,9 +4806,9 @@
       <c r="S42" s="5"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="190"/>
-      <c r="B43" s="191"/>
-      <c r="C43" s="193"/>
+      <c r="A43" s="203"/>
+      <c r="B43" s="204"/>
+      <c r="C43" s="196"/>
       <c r="D43" s="67" t="s">
         <v>29</v>
       </c>
@@ -4831,9 +4834,9 @@
       <c r="S43" s="5"/>
     </row>
     <row r="44" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="190"/>
-      <c r="B44" s="191"/>
-      <c r="C44" s="194" t="s">
+      <c r="A44" s="203"/>
+      <c r="B44" s="204"/>
+      <c r="C44" s="197" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="18" t="s">
@@ -4866,9 +4869,9 @@
       <c r="S44" s="5"/>
     </row>
     <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="190"/>
-      <c r="B45" s="191"/>
-      <c r="C45" s="194"/>
+      <c r="A45" s="203"/>
+      <c r="B45" s="204"/>
+      <c r="C45" s="197"/>
       <c r="D45" s="80" t="s">
         <v>26</v>
       </c>
@@ -4898,9 +4901,9 @@
       <c r="S45" s="5"/>
     </row>
     <row r="46" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="190"/>
-      <c r="B46" s="191"/>
-      <c r="C46" s="194"/>
+      <c r="A46" s="203"/>
+      <c r="B46" s="204"/>
+      <c r="C46" s="197"/>
       <c r="D46" s="83" t="s">
         <v>27</v>
       </c>
@@ -4930,9 +4933,9 @@
       <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="190"/>
-      <c r="B47" s="191"/>
-      <c r="C47" s="194"/>
+      <c r="A47" s="203"/>
+      <c r="B47" s="204"/>
+      <c r="C47" s="197"/>
       <c r="D47" s="80" t="s">
         <v>28</v>
       </c>
@@ -4960,9 +4963,9 @@
       <c r="S47" s="5"/>
     </row>
     <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="190"/>
-      <c r="B48" s="191"/>
-      <c r="C48" s="194"/>
+      <c r="A48" s="203"/>
+      <c r="B48" s="204"/>
+      <c r="C48" s="197"/>
       <c r="D48" s="83" t="s">
         <v>29</v>
       </c>
@@ -4992,11 +4995,11 @@
       <c r="S48" s="5"/>
     </row>
     <row r="49" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="190"/>
-      <c r="B49" s="195" t="s">
+      <c r="A49" s="203"/>
+      <c r="B49" s="198" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="196" t="s">
+      <c r="C49" s="199" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="95" t="s">
@@ -5029,9 +5032,9 @@
       <c r="S49" s="5"/>
     </row>
     <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="190"/>
-      <c r="B50" s="195"/>
-      <c r="C50" s="196"/>
+      <c r="A50" s="203"/>
+      <c r="B50" s="198"/>
+      <c r="C50" s="199"/>
       <c r="D50" s="103" t="s">
         <v>34</v>
       </c>
@@ -5057,9 +5060,9 @@
       <c r="S50" s="5"/>
     </row>
     <row r="51" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="190"/>
-      <c r="B51" s="195"/>
-      <c r="C51" s="196"/>
+      <c r="A51" s="203"/>
+      <c r="B51" s="198"/>
+      <c r="C51" s="199"/>
       <c r="D51" s="111" t="s">
         <v>26</v>
       </c>
@@ -5083,9 +5086,9 @@
       <c r="S51" s="5"/>
     </row>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="190"/>
-      <c r="B52" s="195"/>
-      <c r="C52" s="196"/>
+      <c r="A52" s="203"/>
+      <c r="B52" s="198"/>
+      <c r="C52" s="199"/>
       <c r="D52" s="103" t="s">
         <v>27</v>
       </c>
@@ -5109,9 +5112,9 @@
       <c r="S52" s="5"/>
     </row>
     <row r="53" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="190"/>
-      <c r="B53" s="195"/>
-      <c r="C53" s="196"/>
+      <c r="A53" s="203"/>
+      <c r="B53" s="198"/>
+      <c r="C53" s="199"/>
       <c r="D53" s="119" t="s">
         <v>28</v>
       </c>
@@ -5135,9 +5138,9 @@
       <c r="S53" s="5"/>
     </row>
     <row r="54" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="190"/>
-      <c r="B54" s="195"/>
-      <c r="C54" s="197" t="s">
+      <c r="A54" s="203"/>
+      <c r="B54" s="198"/>
+      <c r="C54" s="206" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="95" t="s">
@@ -5168,9 +5171,9 @@
       <c r="S54" s="5"/>
     </row>
     <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="190"/>
-      <c r="B55" s="195"/>
-      <c r="C55" s="197"/>
+      <c r="A55" s="203"/>
+      <c r="B55" s="198"/>
+      <c r="C55" s="206"/>
       <c r="D55" s="103" t="s">
         <v>34</v>
       </c>
@@ -5196,9 +5199,9 @@
       <c r="S55" s="5"/>
     </row>
     <row r="56" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="190"/>
-      <c r="B56" s="195"/>
-      <c r="C56" s="197"/>
+      <c r="A56" s="203"/>
+      <c r="B56" s="198"/>
+      <c r="C56" s="206"/>
       <c r="D56" s="111" t="s">
         <v>26</v>
       </c>
@@ -5222,9 +5225,9 @@
       <c r="S56" s="5"/>
     </row>
     <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="190"/>
-      <c r="B57" s="195"/>
-      <c r="C57" s="197"/>
+      <c r="A57" s="203"/>
+      <c r="B57" s="198"/>
+      <c r="C57" s="206"/>
       <c r="D57" s="103" t="s">
         <v>27</v>
       </c>
@@ -5248,9 +5251,9 @@
       <c r="S57" s="5"/>
     </row>
     <row r="58" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="190"/>
-      <c r="B58" s="195"/>
-      <c r="C58" s="198"/>
+      <c r="A58" s="203"/>
+      <c r="B58" s="198"/>
+      <c r="C58" s="207"/>
       <c r="D58" s="135" t="s">
         <v>28</v>
       </c>
@@ -5275,7 +5278,7 @@
     </row>
     <row r="59" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="C59" s="189" t="s">
+      <c r="C59" s="202" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="168" t="s">
@@ -5310,7 +5313,7 @@
     </row>
     <row r="60" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
-      <c r="C60" s="189"/>
+      <c r="C60" s="202"/>
       <c r="D60" s="176" t="s">
         <v>38</v>
       </c>
@@ -5381,6 +5384,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A36:A58"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C58"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:P7"/>
@@ -5393,15 +5405,6 @@
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C35"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A36:A58"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Aktualisierung Inventar: Adrian, Susanne
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -203,7 +203,8 @@
             <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t>Ruth:</t>
+          <t>Ruth:
+2x Lukas</t>
         </r>
         <r>
           <rPr>
@@ -238,7 +239,8 @@
           </rPr>
           <t xml:space="preserve">
 Beat
-Reto x2</t>
+Reto x2
+Adrian</t>
         </r>
       </text>
     </comment>
@@ -281,6 +283,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="H45" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Susanne</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I45" authorId="0" shapeId="0">
       <text>
         <r>
@@ -291,7 +317,8 @@
             <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t>Ruth:</t>
+          <t>Ruth:
+2x Lukas</t>
         </r>
         <r>
           <rPr>
@@ -349,7 +376,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Adrian
+Adrian x2
 Reto x2</t>
         </r>
       </text>
@@ -375,6 +402,30 @@
           </rPr>
           <t xml:space="preserve">
 Manuel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H50" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Susanne</t>
         </r>
       </text>
     </comment>
@@ -2719,6 +2770,46 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2747,51 +2838,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3386,8 +3437,8 @@
   <dimension ref="A1:IX69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <pane ySplit="8" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3463,7 +3514,7 @@
       </c>
       <c r="B4" s="8">
         <f ca="1">TODAY()</f>
-        <v>42774</v>
+        <v>42807</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -3523,30 +3574,30 @@
       <c r="S6" s="5"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="189" t="s">
+      <c r="A7" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="190"/>
-      <c r="C7" s="190"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="190"/>
-      <c r="F7" s="191" t="s">
+      <c r="B7" s="200"/>
+      <c r="C7" s="200"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="191"/>
-      <c r="H7" s="191"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="191"/>
-      <c r="K7" s="191"/>
-      <c r="L7" s="191" t="s">
+      <c r="G7" s="201"/>
+      <c r="H7" s="201"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="201"/>
+      <c r="L7" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="191"/>
-      <c r="N7" s="191" t="s">
+      <c r="M7" s="201"/>
+      <c r="N7" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="191"/>
-      <c r="P7" s="192"/>
+      <c r="O7" s="201"/>
+      <c r="P7" s="202"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
@@ -3603,13 +3654,13 @@
       <c r="S8" s="5"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="203" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="194" t="s">
+      <c r="B9" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="195" t="s">
+      <c r="C9" s="205" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -3651,9 +3702,9 @@
       <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="193"/>
-      <c r="B10" s="194"/>
-      <c r="C10" s="195"/>
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
+      <c r="C10" s="205"/>
       <c r="D10" s="27" t="s">
         <v>27</v>
       </c>
@@ -3688,9 +3739,9 @@
       <c r="S10" s="5"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="193"/>
-      <c r="B11" s="194"/>
-      <c r="C11" s="195"/>
+      <c r="A11" s="203"/>
+      <c r="B11" s="204"/>
+      <c r="C11" s="205"/>
       <c r="D11" s="18" t="s">
         <v>28</v>
       </c>
@@ -3723,9 +3774,9 @@
       <c r="S11" s="5"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="193"/>
-      <c r="B12" s="194"/>
-      <c r="C12" s="195"/>
+      <c r="A12" s="203"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="205"/>
       <c r="D12" s="35" t="s">
         <v>29</v>
       </c>
@@ -3758,9 +3809,9 @@
       <c r="S12" s="5"/>
     </row>
     <row r="13" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="193"/>
-      <c r="B13" s="194"/>
-      <c r="C13" s="196" t="s">
+      <c r="A13" s="203"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="193" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="43" t="s">
@@ -3800,9 +3851,9 @@
       <c r="S13" s="5"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="193"/>
-      <c r="B14" s="194"/>
-      <c r="C14" s="196"/>
+      <c r="A14" s="203"/>
+      <c r="B14" s="204"/>
+      <c r="C14" s="193"/>
       <c r="D14" s="51" t="s">
         <v>27</v>
       </c>
@@ -3838,9 +3889,9 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="193"/>
-      <c r="B15" s="194"/>
-      <c r="C15" s="196"/>
+      <c r="A15" s="203"/>
+      <c r="B15" s="204"/>
+      <c r="C15" s="193"/>
       <c r="D15" s="59" t="s">
         <v>28</v>
       </c>
@@ -3870,9 +3921,9 @@
       <c r="S15" s="5"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="193"/>
-      <c r="B16" s="194"/>
-      <c r="C16" s="196"/>
+      <c r="A16" s="203"/>
+      <c r="B16" s="204"/>
+      <c r="C16" s="193"/>
       <c r="D16" s="67" t="s">
         <v>29</v>
       </c>
@@ -3904,9 +3955,9 @@
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
-      <c r="B17" s="194"/>
-      <c r="C17" s="197" t="s">
+      <c r="A17" s="203"/>
+      <c r="B17" s="204"/>
+      <c r="C17" s="194" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -3945,9 +3996,9 @@
       <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="193"/>
-      <c r="B18" s="194"/>
-      <c r="C18" s="197"/>
+      <c r="A18" s="203"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="194"/>
       <c r="D18" s="80" t="s">
         <v>27</v>
       </c>
@@ -3981,9 +4032,9 @@
       <c r="S18" s="5"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="193"/>
-      <c r="B19" s="194"/>
-      <c r="C19" s="197"/>
+      <c r="A19" s="203"/>
+      <c r="B19" s="204"/>
+      <c r="C19" s="194"/>
       <c r="D19" s="83" t="s">
         <v>28</v>
       </c>
@@ -4015,9 +4066,9 @@
       <c r="S19" s="5"/>
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="193"/>
-      <c r="B20" s="194"/>
-      <c r="C20" s="197"/>
+      <c r="A20" s="203"/>
+      <c r="B20" s="204"/>
+      <c r="C20" s="194"/>
       <c r="D20" s="89" t="s">
         <v>29</v>
       </c>
@@ -4051,11 +4102,11 @@
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="193"/>
-      <c r="B21" s="198" t="s">
+      <c r="A21" s="203"/>
+      <c r="B21" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="199" t="s">
+      <c r="C21" s="196" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="95" t="s">
@@ -4094,9 +4145,9 @@
       <c r="S21" s="5"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="193"/>
-      <c r="B22" s="198"/>
-      <c r="C22" s="199"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="195"/>
+      <c r="C22" s="196"/>
       <c r="D22" s="103" t="s">
         <v>34</v>
       </c>
@@ -4128,9 +4179,9 @@
       <c r="S22" s="5"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="193"/>
-      <c r="B23" s="198"/>
-      <c r="C23" s="199"/>
+      <c r="A23" s="203"/>
+      <c r="B23" s="195"/>
+      <c r="C23" s="196"/>
       <c r="D23" s="111" t="s">
         <v>26</v>
       </c>
@@ -4166,9 +4217,9 @@
       <c r="S23" s="5"/>
     </row>
     <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="193"/>
-      <c r="B24" s="198"/>
-      <c r="C24" s="199"/>
+      <c r="A24" s="203"/>
+      <c r="B24" s="195"/>
+      <c r="C24" s="196"/>
       <c r="D24" s="103" t="s">
         <v>27</v>
       </c>
@@ -4200,9 +4251,9 @@
       <c r="S24" s="5"/>
     </row>
     <row r="25" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="193"/>
-      <c r="B25" s="198"/>
-      <c r="C25" s="199"/>
+      <c r="A25" s="203"/>
+      <c r="B25" s="195"/>
+      <c r="C25" s="196"/>
       <c r="D25" s="119" t="s">
         <v>28</v>
       </c>
@@ -4234,9 +4285,9 @@
       <c r="S25" s="5"/>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="193"/>
-      <c r="B26" s="198"/>
-      <c r="C26" s="200" t="s">
+      <c r="A26" s="203"/>
+      <c r="B26" s="195"/>
+      <c r="C26" s="206" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="95" t="s">
@@ -4275,9 +4326,9 @@
       <c r="S26" s="5"/>
     </row>
     <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="193"/>
-      <c r="B27" s="198"/>
-      <c r="C27" s="200"/>
+      <c r="A27" s="203"/>
+      <c r="B27" s="195"/>
+      <c r="C27" s="206"/>
       <c r="D27" s="103" t="s">
         <v>34</v>
       </c>
@@ -4309,9 +4360,9 @@
       <c r="S27" s="5"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="193"/>
-      <c r="B28" s="198"/>
-      <c r="C28" s="200"/>
+      <c r="A28" s="203"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="206"/>
       <c r="D28" s="111" t="s">
         <v>26</v>
       </c>
@@ -4343,9 +4394,9 @@
       <c r="S28" s="5"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="193"/>
-      <c r="B29" s="198"/>
-      <c r="C29" s="200"/>
+      <c r="A29" s="203"/>
+      <c r="B29" s="195"/>
+      <c r="C29" s="206"/>
       <c r="D29" s="103" t="s">
         <v>27</v>
       </c>
@@ -4375,9 +4426,9 @@
       <c r="S29" s="5"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="193"/>
-      <c r="B30" s="198"/>
-      <c r="C30" s="200"/>
+      <c r="A30" s="203"/>
+      <c r="B30" s="195"/>
+      <c r="C30" s="206"/>
       <c r="D30" s="127" t="s">
         <v>28</v>
       </c>
@@ -4407,9 +4458,9 @@
       <c r="S30" s="5"/>
     </row>
     <row r="31" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="193"/>
-      <c r="B31" s="198"/>
-      <c r="C31" s="201" t="s">
+      <c r="A31" s="203"/>
+      <c r="B31" s="195"/>
+      <c r="C31" s="207" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="95" t="s">
@@ -4448,9 +4499,9 @@
       <c r="S31" s="5"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="193"/>
-      <c r="B32" s="198"/>
-      <c r="C32" s="201"/>
+      <c r="A32" s="203"/>
+      <c r="B32" s="195"/>
+      <c r="C32" s="207"/>
       <c r="D32" s="103" t="s">
         <v>26</v>
       </c>
@@ -4486,9 +4537,9 @@
       <c r="S32" s="5"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="193"/>
-      <c r="B33" s="198"/>
-      <c r="C33" s="201"/>
+      <c r="A33" s="203"/>
+      <c r="B33" s="195"/>
+      <c r="C33" s="207"/>
       <c r="D33" s="111" t="s">
         <v>27</v>
       </c>
@@ -4520,9 +4571,9 @@
       <c r="S33" s="5"/>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="193"/>
-      <c r="B34" s="198"/>
-      <c r="C34" s="201"/>
+      <c r="A34" s="203"/>
+      <c r="B34" s="195"/>
+      <c r="C34" s="207"/>
       <c r="D34" s="103" t="s">
         <v>28</v>
       </c>
@@ -4554,9 +4605,9 @@
       <c r="S34" s="5"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="193"/>
-      <c r="B35" s="198"/>
-      <c r="C35" s="201"/>
+      <c r="A35" s="203"/>
+      <c r="B35" s="195"/>
+      <c r="C35" s="207"/>
       <c r="D35" s="135" t="s">
         <v>29</v>
       </c>
@@ -4586,13 +4637,13 @@
       <c r="S35" s="5"/>
     </row>
     <row r="36" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="203" t="s">
+      <c r="A36" s="190" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="204" t="s">
+      <c r="B36" s="191" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="205" t="s">
+      <c r="C36" s="192" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="143" t="s">
@@ -4603,7 +4654,7 @@
       </c>
       <c r="F36" s="145">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G36" s="143">
         <v>1</v>
@@ -4612,7 +4663,7 @@
         <v>2</v>
       </c>
       <c r="I36" s="143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J36" s="143">
         <v>1</v>
@@ -4629,9 +4680,9 @@
       <c r="S36" s="5"/>
     </row>
     <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="203"/>
-      <c r="B37" s="204"/>
-      <c r="C37" s="205"/>
+      <c r="A37" s="190"/>
+      <c r="B37" s="191"/>
+      <c r="C37" s="192"/>
       <c r="D37" s="27" t="s">
         <v>27</v>
       </c>
@@ -4640,14 +4691,14 @@
       </c>
       <c r="F37" s="20">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="27">
         <v>1</v>
       </c>
       <c r="I37" s="27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J37" s="27">
         <v>4</v>
@@ -4661,9 +4712,9 @@
       <c r="S37" s="5"/>
     </row>
     <row r="38" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="203"/>
-      <c r="B38" s="204"/>
-      <c r="C38" s="205"/>
+      <c r="A38" s="190"/>
+      <c r="B38" s="191"/>
+      <c r="C38" s="192"/>
       <c r="D38" s="18" t="s">
         <v>28</v>
       </c>
@@ -4689,9 +4740,9 @@
       <c r="S38" s="5"/>
     </row>
     <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="203"/>
-      <c r="B39" s="204"/>
-      <c r="C39" s="205"/>
+      <c r="A39" s="190"/>
+      <c r="B39" s="191"/>
+      <c r="C39" s="192"/>
       <c r="D39" s="35" t="s">
         <v>29</v>
       </c>
@@ -4717,9 +4768,9 @@
       <c r="S39" s="5"/>
     </row>
     <row r="40" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="203"/>
-      <c r="B40" s="204"/>
-      <c r="C40" s="196" t="s">
+      <c r="A40" s="190"/>
+      <c r="B40" s="191"/>
+      <c r="C40" s="193" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="43" t="s">
@@ -4750,9 +4801,9 @@
       <c r="S40" s="5"/>
     </row>
     <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="203"/>
-      <c r="B41" s="204"/>
-      <c r="C41" s="196"/>
+      <c r="A41" s="190"/>
+      <c r="B41" s="191"/>
+      <c r="C41" s="193"/>
       <c r="D41" s="51" t="s">
         <v>27</v>
       </c>
@@ -4780,9 +4831,9 @@
       <c r="S41" s="5"/>
     </row>
     <row r="42" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="203"/>
-      <c r="B42" s="204"/>
-      <c r="C42" s="196"/>
+      <c r="A42" s="190"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="193"/>
       <c r="D42" s="59" t="s">
         <v>28</v>
       </c>
@@ -4806,9 +4857,9 @@
       <c r="S42" s="5"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="203"/>
-      <c r="B43" s="204"/>
-      <c r="C43" s="196"/>
+      <c r="A43" s="190"/>
+      <c r="B43" s="191"/>
+      <c r="C43" s="193"/>
       <c r="D43" s="67" t="s">
         <v>29</v>
       </c>
@@ -4834,9 +4885,9 @@
       <c r="S43" s="5"/>
     </row>
     <row r="44" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="203"/>
-      <c r="B44" s="204"/>
-      <c r="C44" s="197" t="s">
+      <c r="A44" s="190"/>
+      <c r="B44" s="191"/>
+      <c r="C44" s="194" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="18" t="s">
@@ -4869,9 +4920,9 @@
       <c r="S44" s="5"/>
     </row>
     <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="203"/>
-      <c r="B45" s="204"/>
-      <c r="C45" s="197"/>
+      <c r="A45" s="190"/>
+      <c r="B45" s="191"/>
+      <c r="C45" s="194"/>
       <c r="D45" s="80" t="s">
         <v>26</v>
       </c>
@@ -4880,14 +4931,16 @@
       </c>
       <c r="F45" s="29">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G45" s="80">
         <v>1</v>
       </c>
-      <c r="H45" s="80"/>
+      <c r="H45" s="80">
+        <v>1</v>
+      </c>
       <c r="I45" s="80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J45" s="80">
         <v>1</v>
@@ -4901,9 +4954,9 @@
       <c r="S45" s="5"/>
     </row>
     <row r="46" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="203"/>
-      <c r="B46" s="204"/>
-      <c r="C46" s="197"/>
+      <c r="A46" s="190"/>
+      <c r="B46" s="191"/>
+      <c r="C46" s="194"/>
       <c r="D46" s="83" t="s">
         <v>27</v>
       </c>
@@ -4933,9 +4986,9 @@
       <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="203"/>
-      <c r="B47" s="204"/>
-      <c r="C47" s="197"/>
+      <c r="A47" s="190"/>
+      <c r="B47" s="191"/>
+      <c r="C47" s="194"/>
       <c r="D47" s="80" t="s">
         <v>28</v>
       </c>
@@ -4944,12 +4997,12 @@
       </c>
       <c r="F47" s="29">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" s="80"/>
       <c r="H47" s="80"/>
       <c r="I47" s="80">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J47" s="80">
         <v>1</v>
@@ -4963,9 +5016,9 @@
       <c r="S47" s="5"/>
     </row>
     <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="203"/>
-      <c r="B48" s="204"/>
-      <c r="C48" s="197"/>
+      <c r="A48" s="190"/>
+      <c r="B48" s="191"/>
+      <c r="C48" s="194"/>
       <c r="D48" s="83" t="s">
         <v>29</v>
       </c>
@@ -4995,11 +5048,11 @@
       <c r="S48" s="5"/>
     </row>
     <row r="49" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="203"/>
-      <c r="B49" s="198" t="s">
+      <c r="A49" s="190"/>
+      <c r="B49" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="199" t="s">
+      <c r="C49" s="196" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="95" t="s">
@@ -5032,9 +5085,9 @@
       <c r="S49" s="5"/>
     </row>
     <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="203"/>
-      <c r="B50" s="198"/>
-      <c r="C50" s="199"/>
+      <c r="A50" s="190"/>
+      <c r="B50" s="195"/>
+      <c r="C50" s="196"/>
       <c r="D50" s="103" t="s">
         <v>34</v>
       </c>
@@ -5043,10 +5096,12 @@
       </c>
       <c r="F50" s="105">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G50" s="103"/>
-      <c r="H50" s="103"/>
+      <c r="H50" s="103">
+        <v>1</v>
+      </c>
       <c r="I50" s="103"/>
       <c r="J50" s="103">
         <v>1</v>
@@ -5060,9 +5115,9 @@
       <c r="S50" s="5"/>
     </row>
     <row r="51" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="203"/>
-      <c r="B51" s="198"/>
-      <c r="C51" s="199"/>
+      <c r="A51" s="190"/>
+      <c r="B51" s="195"/>
+      <c r="C51" s="196"/>
       <c r="D51" s="111" t="s">
         <v>26</v>
       </c>
@@ -5086,9 +5141,9 @@
       <c r="S51" s="5"/>
     </row>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="203"/>
-      <c r="B52" s="198"/>
-      <c r="C52" s="199"/>
+      <c r="A52" s="190"/>
+      <c r="B52" s="195"/>
+      <c r="C52" s="196"/>
       <c r="D52" s="103" t="s">
         <v>27</v>
       </c>
@@ -5112,9 +5167,9 @@
       <c r="S52" s="5"/>
     </row>
     <row r="53" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="203"/>
-      <c r="B53" s="198"/>
-      <c r="C53" s="199"/>
+      <c r="A53" s="190"/>
+      <c r="B53" s="195"/>
+      <c r="C53" s="196"/>
       <c r="D53" s="119" t="s">
         <v>28</v>
       </c>
@@ -5138,9 +5193,9 @@
       <c r="S53" s="5"/>
     </row>
     <row r="54" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="203"/>
-      <c r="B54" s="198"/>
-      <c r="C54" s="206" t="s">
+      <c r="A54" s="190"/>
+      <c r="B54" s="195"/>
+      <c r="C54" s="197" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="95" t="s">
@@ -5171,9 +5226,9 @@
       <c r="S54" s="5"/>
     </row>
     <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="203"/>
-      <c r="B55" s="198"/>
-      <c r="C55" s="206"/>
+      <c r="A55" s="190"/>
+      <c r="B55" s="195"/>
+      <c r="C55" s="197"/>
       <c r="D55" s="103" t="s">
         <v>34</v>
       </c>
@@ -5199,9 +5254,9 @@
       <c r="S55" s="5"/>
     </row>
     <row r="56" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="203"/>
-      <c r="B56" s="198"/>
-      <c r="C56" s="206"/>
+      <c r="A56" s="190"/>
+      <c r="B56" s="195"/>
+      <c r="C56" s="197"/>
       <c r="D56" s="111" t="s">
         <v>26</v>
       </c>
@@ -5225,9 +5280,9 @@
       <c r="S56" s="5"/>
     </row>
     <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="203"/>
-      <c r="B57" s="198"/>
-      <c r="C57" s="206"/>
+      <c r="A57" s="190"/>
+      <c r="B57" s="195"/>
+      <c r="C57" s="197"/>
       <c r="D57" s="103" t="s">
         <v>27</v>
       </c>
@@ -5251,9 +5306,9 @@
       <c r="S57" s="5"/>
     </row>
     <row r="58" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="203"/>
-      <c r="B58" s="198"/>
-      <c r="C58" s="207"/>
+      <c r="A58" s="190"/>
+      <c r="B58" s="195"/>
+      <c r="C58" s="198"/>
       <c r="D58" s="135" t="s">
         <v>28</v>
       </c>
@@ -5278,7 +5333,7 @@
     </row>
     <row r="59" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="C59" s="202" t="s">
+      <c r="C59" s="189" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="168" t="s">
@@ -5313,7 +5368,7 @@
     </row>
     <row r="60" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
-      <c r="C60" s="202"/>
+      <c r="C60" s="189"/>
       <c r="D60" s="176" t="s">
         <v>38</v>
       </c>
@@ -5384,15 +5439,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A36:A58"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:P7"/>
@@ -5405,6 +5451,15 @@
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C35"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A36:A58"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Aktualisierung Inventar nach Verkauf auf Reisen (CdA, Ligurien) und Bestellung im Shop (Berthold Theobald)
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,6 +30,54 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="M9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- 1x Lukas Kamber (110 €) (evtl. falsch in RE)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Gewinnspiel: Christoph Birnbaum</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M10" authorId="0" shapeId="0">
       <text>
         <r>
@@ -50,8 +98,84 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Volker Laabs #1565
-Gewinnspiel: Christoph Birnbaum</t>
+- 1x Volker Laabs #1565
+- 1x Michael Kusch Reisen 2017 (110 €)
+- 1x Tobias Zimmermann (110 €)
+- 2x Berthold Theobald (Bestellnummer #2140)
+- 2x Matthias Dorn (110 €, 1x geschenkt)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- 1x Martin Slonina Reisen 2017 (110 €)
+- 1x Tobias Zimmermann (110 €)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1x Thomas als Guidelohen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- 1x Lukas Kamber (50 €)</t>
         </r>
       </text>
     </comment>
@@ -75,7 +199,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Volker Laabs #1565</t>
+- 1x Volker Laabs #1565
+- 1x Edgar Reisen 2017 (110 €)</t>
         </r>
       </text>
     </comment>
@@ -99,7 +224,62 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Volker Laabs #1565</t>
+- 1x Volker Laabs #1565
+- 1x Michael Kusch Reisen 2017 (110 €)
+- 1x Christopher Kielbassa (110 €)
+- 1x Tobias Zimmermann (110 €)
+- 2x Berthold Theobald (Bestellnummer #2140)
+- 1x Lukas Kamber (110 €)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- 1x Lukas Kamber (110 €)
+- 1x Tobias Zimmermann (110 €)
+- 2x Matthias Dorn (220 €)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1x Thomas als Guidelohen</t>
         </r>
       </text>
     </comment>
@@ -138,6 +318,30 @@
           </rPr>
           <t xml:space="preserve">
 FÜR ALEX</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1xKarmen (50€ EK-Preis)</t>
         </r>
       </text>
     </comment>
@@ -218,6 +422,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G37" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Volker Laabs</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I37" authorId="0" shapeId="0">
       <text>
         <r>
@@ -269,6 +497,56 @@
         </r>
       </text>
     </comment>
+    <comment ref="I40" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1xLukas
+1xFrederik (50 €)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H41" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- 1x Lutz
+- 1x Manuel (50 €)</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G45" authorId="1" shapeId="0">
       <text>
         <r>
@@ -279,7 +557,8 @@
             <charset val="1"/>
           </rPr>
           <t>Ruth:
-Guide Südtirol, muss noch übergeben werden</t>
+Guide Südtirol, 
+Richard Palma + Volker Laabs</t>
         </r>
       </text>
     </comment>
@@ -402,6 +681,32 @@
           </rPr>
           <t xml:space="preserve">
 Manuel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- 1x Ruth
+- 1x Susanne Schwandner (50 €)
+</t>
         </r>
       </text>
     </comment>
@@ -2770,6 +3075,58 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2786,63 +3143,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="84" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3437,8 +3742,8 @@
   <dimension ref="A1:IX69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S43" sqref="S43"/>
+      <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3447,8 +3752,8 @@
     <col min="2" max="2" width="10.42578125" style="3"/>
     <col min="3" max="3" width="13.140625" style="3"/>
     <col min="4" max="4" width="7.42578125" style="185"/>
-    <col min="5" max="5" width="11" style="186"/>
-    <col min="6" max="11" width="6.5703125" style="3"/>
+    <col min="5" max="5" width="9.140625" style="186" customWidth="1"/>
+    <col min="6" max="11" width="9.140625" style="3" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" style="3"/>
     <col min="13" max="13" width="9.140625" style="3"/>
     <col min="14" max="14" width="10.42578125" style="3"/>
@@ -3514,7 +3819,7 @@
       </c>
       <c r="B4" s="8">
         <f ca="1">TODAY()</f>
-        <v>42807</v>
+        <v>42843</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -3574,30 +3879,30 @@
       <c r="S6" s="5"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="199" t="s">
+      <c r="A7" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="200"/>
-      <c r="C7" s="200"/>
-      <c r="D7" s="200"/>
-      <c r="E7" s="200"/>
-      <c r="F7" s="201" t="s">
+      <c r="B7" s="190"/>
+      <c r="C7" s="190"/>
+      <c r="D7" s="190"/>
+      <c r="E7" s="190"/>
+      <c r="F7" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="201"/>
-      <c r="H7" s="201"/>
-      <c r="I7" s="201"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="201"/>
-      <c r="L7" s="201" t="s">
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
+      <c r="L7" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="201"/>
-      <c r="N7" s="201" t="s">
+      <c r="M7" s="191"/>
+      <c r="N7" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="201"/>
-      <c r="P7" s="202"/>
+      <c r="O7" s="191"/>
+      <c r="P7" s="192"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
@@ -3654,13 +3959,13 @@
       <c r="S8" s="5"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="203" t="s">
+      <c r="A9" s="193" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="205" t="s">
+      <c r="C9" s="195" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -3686,10 +3991,12 @@
         <f>F9</f>
         <v>11</v>
       </c>
-      <c r="M9" s="23"/>
+      <c r="M9" s="23">
+        <v>1</v>
+      </c>
       <c r="N9" s="18">
         <f>L9-M9</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O9" s="24">
         <f>49.18-(49.18*10/100)</f>
@@ -3702,9 +4009,9 @@
       <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
-      <c r="C10" s="205"/>
+      <c r="A10" s="193"/>
+      <c r="B10" s="194"/>
+      <c r="C10" s="195"/>
       <c r="D10" s="27" t="s">
         <v>27</v>
       </c>
@@ -3713,25 +4020,26 @@
       </c>
       <c r="F10" s="29">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27">
-        <v>3</v>
+        <f>3+1</f>
+        <v>4</v>
       </c>
       <c r="K10" s="30"/>
       <c r="L10" s="31">
         <f t="shared" ref="L10:L35" si="1">F10</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M10" s="32">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N10" s="27">
         <f t="shared" ref="N10:N35" si="2">L10-M10</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="O10" s="33"/>
       <c r="P10" s="34"/>
@@ -3739,9 +4047,9 @@
       <c r="S10" s="5"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="203"/>
-      <c r="B11" s="204"/>
-      <c r="C11" s="205"/>
+      <c r="A11" s="193"/>
+      <c r="B11" s="194"/>
+      <c r="C11" s="195"/>
       <c r="D11" s="18" t="s">
         <v>28</v>
       </c>
@@ -3763,10 +4071,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="M11" s="23"/>
+      <c r="M11" s="23">
+        <v>2</v>
+      </c>
       <c r="N11" s="18">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O11" s="24"/>
       <c r="P11" s="25"/>
@@ -3774,9 +4084,9 @@
       <c r="S11" s="5"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="203"/>
-      <c r="B12" s="204"/>
-      <c r="C12" s="205"/>
+      <c r="A12" s="193"/>
+      <c r="B12" s="194"/>
+      <c r="C12" s="195"/>
       <c r="D12" s="35" t="s">
         <v>29</v>
       </c>
@@ -3798,20 +4108,26 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M12" s="40"/>
+      <c r="M12" s="40">
+        <v>1</v>
+      </c>
       <c r="N12" s="35">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O12" s="41"/>
       <c r="P12" s="42"/>
+      <c r="Q12" s="3">
+        <f>SUM(N9:N12)</f>
+        <v>37</v>
+      </c>
       <c r="R12" s="26"/>
       <c r="S12" s="5"/>
     </row>
     <row r="13" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="203"/>
-      <c r="B13" s="204"/>
-      <c r="C13" s="193" t="s">
+      <c r="A13" s="193"/>
+      <c r="B13" s="194"/>
+      <c r="C13" s="196" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="43" t="s">
@@ -3835,10 +4151,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M13" s="48"/>
+      <c r="M13" s="48">
+        <v>1</v>
+      </c>
       <c r="N13" s="43">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O13" s="49">
         <f>56.01-(56.01*10/100)</f>
@@ -3851,9 +4169,9 @@
       <c r="S13" s="5"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="203"/>
-      <c r="B14" s="204"/>
-      <c r="C14" s="193"/>
+      <c r="A14" s="193"/>
+      <c r="B14" s="194"/>
+      <c r="C14" s="196"/>
       <c r="D14" s="51" t="s">
         <v>27</v>
       </c>
@@ -3878,20 +4196,21 @@
         <v>2</v>
       </c>
       <c r="M14" s="56">
-        <v>1</v>
+        <f>1+1</f>
+        <v>2</v>
       </c>
       <c r="N14" s="51">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="57"/>
       <c r="P14" s="58"/>
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="203"/>
-      <c r="B15" s="204"/>
-      <c r="C15" s="193"/>
+      <c r="A15" s="193"/>
+      <c r="B15" s="194"/>
+      <c r="C15" s="196"/>
       <c r="D15" s="59" t="s">
         <v>28</v>
       </c>
@@ -3921,9 +4240,9 @@
       <c r="S15" s="5"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="203"/>
-      <c r="B16" s="204"/>
-      <c r="C16" s="193"/>
+      <c r="A16" s="193"/>
+      <c r="B16" s="194"/>
+      <c r="C16" s="196"/>
       <c r="D16" s="67" t="s">
         <v>29</v>
       </c>
@@ -3952,12 +4271,16 @@
       </c>
       <c r="O16" s="73"/>
       <c r="P16" s="74"/>
+      <c r="Q16" s="3">
+        <f>SUM(N13:N16)</f>
+        <v>3</v>
+      </c>
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="203"/>
-      <c r="B17" s="204"/>
-      <c r="C17" s="194" t="s">
+      <c r="A17" s="193"/>
+      <c r="B17" s="194"/>
+      <c r="C17" s="197" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -3996,9 +4319,9 @@
       <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="203"/>
-      <c r="B18" s="204"/>
-      <c r="C18" s="194"/>
+      <c r="A18" s="193"/>
+      <c r="B18" s="194"/>
+      <c r="C18" s="197"/>
       <c r="D18" s="80" t="s">
         <v>27</v>
       </c>
@@ -4021,20 +4344,20 @@
         <v>11</v>
       </c>
       <c r="M18" s="27">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N18" s="27">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="O18" s="27"/>
       <c r="P18" s="82"/>
       <c r="S18" s="5"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="203"/>
-      <c r="B19" s="204"/>
-      <c r="C19" s="194"/>
+      <c r="A19" s="193"/>
+      <c r="B19" s="194"/>
+      <c r="C19" s="197"/>
       <c r="D19" s="83" t="s">
         <v>28</v>
       </c>
@@ -4056,19 +4379,21 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="M19" s="86"/>
+      <c r="M19" s="86">
+        <v>4</v>
+      </c>
       <c r="N19" s="83">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O19" s="87"/>
       <c r="P19" s="88"/>
       <c r="S19" s="5"/>
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="203"/>
-      <c r="B20" s="204"/>
-      <c r="C20" s="194"/>
+      <c r="A20" s="193"/>
+      <c r="B20" s="194"/>
+      <c r="C20" s="197"/>
       <c r="D20" s="89" t="s">
         <v>29</v>
       </c>
@@ -4092,21 +4417,27 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M20" s="27"/>
+      <c r="M20" s="27">
+        <v>1</v>
+      </c>
       <c r="N20" s="27">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O20" s="27"/>
       <c r="P20" s="94"/>
+      <c r="Q20" s="3">
+        <f>SUM(N17:N20)</f>
+        <v>17</v>
+      </c>
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="203"/>
-      <c r="B21" s="195" t="s">
+      <c r="A21" s="193"/>
+      <c r="B21" s="198" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="196" t="s">
+      <c r="C21" s="199" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="95" t="s">
@@ -4145,9 +4476,9 @@
       <c r="S21" s="5"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="203"/>
-      <c r="B22" s="195"/>
-      <c r="C22" s="196"/>
+      <c r="A22" s="193"/>
+      <c r="B22" s="198"/>
+      <c r="C22" s="199"/>
       <c r="D22" s="103" t="s">
         <v>34</v>
       </c>
@@ -4179,9 +4510,9 @@
       <c r="S22" s="5"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="203"/>
-      <c r="B23" s="195"/>
-      <c r="C23" s="196"/>
+      <c r="A23" s="193"/>
+      <c r="B23" s="198"/>
+      <c r="C23" s="199"/>
       <c r="D23" s="111" t="s">
         <v>26</v>
       </c>
@@ -4217,9 +4548,9 @@
       <c r="S23" s="5"/>
     </row>
     <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="203"/>
-      <c r="B24" s="195"/>
-      <c r="C24" s="196"/>
+      <c r="A24" s="193"/>
+      <c r="B24" s="198"/>
+      <c r="C24" s="199"/>
       <c r="D24" s="103" t="s">
         <v>27</v>
       </c>
@@ -4251,9 +4582,9 @@
       <c r="S24" s="5"/>
     </row>
     <row r="25" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="203"/>
-      <c r="B25" s="195"/>
-      <c r="C25" s="196"/>
+      <c r="A25" s="193"/>
+      <c r="B25" s="198"/>
+      <c r="C25" s="199"/>
       <c r="D25" s="119" t="s">
         <v>28</v>
       </c>
@@ -4282,12 +4613,16 @@
       </c>
       <c r="O25" s="125"/>
       <c r="P25" s="126"/>
+      <c r="Q25" s="3">
+        <f>SUM(N21:N25)</f>
+        <v>12</v>
+      </c>
       <c r="S25" s="5"/>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="203"/>
-      <c r="B26" s="195"/>
-      <c r="C26" s="206" t="s">
+      <c r="A26" s="193"/>
+      <c r="B26" s="198"/>
+      <c r="C26" s="200" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="95" t="s">
@@ -4326,9 +4661,9 @@
       <c r="S26" s="5"/>
     </row>
     <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="203"/>
-      <c r="B27" s="195"/>
-      <c r="C27" s="206"/>
+      <c r="A27" s="193"/>
+      <c r="B27" s="198"/>
+      <c r="C27" s="200"/>
       <c r="D27" s="103" t="s">
         <v>34</v>
       </c>
@@ -4359,10 +4694,10 @@
       <c r="P27" s="110"/>
       <c r="S27" s="5"/>
     </row>
-    <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="203"/>
-      <c r="B28" s="195"/>
-      <c r="C28" s="206"/>
+    <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="193"/>
+      <c r="B28" s="198"/>
+      <c r="C28" s="200"/>
       <c r="D28" s="111" t="s">
         <v>26</v>
       </c>
@@ -4384,19 +4719,21 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M28" s="116"/>
+      <c r="M28" s="108">
+        <v>1</v>
+      </c>
       <c r="N28" s="111">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O28" s="117"/>
       <c r="P28" s="118"/>
       <c r="S28" s="5"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="203"/>
-      <c r="B29" s="195"/>
-      <c r="C29" s="206"/>
+      <c r="A29" s="193"/>
+      <c r="B29" s="198"/>
+      <c r="C29" s="200"/>
       <c r="D29" s="103" t="s">
         <v>27</v>
       </c>
@@ -4426,9 +4763,9 @@
       <c r="S29" s="5"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="203"/>
-      <c r="B30" s="195"/>
-      <c r="C30" s="206"/>
+      <c r="A30" s="193"/>
+      <c r="B30" s="198"/>
+      <c r="C30" s="200"/>
       <c r="D30" s="127" t="s">
         <v>28</v>
       </c>
@@ -4455,12 +4792,16 @@
       </c>
       <c r="O30" s="133"/>
       <c r="P30" s="134"/>
+      <c r="Q30" s="3">
+        <f>SUM(N26:N30)</f>
+        <v>6</v>
+      </c>
       <c r="S30" s="5"/>
     </row>
     <row r="31" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="203"/>
-      <c r="B31" s="195"/>
-      <c r="C31" s="207" t="s">
+      <c r="A31" s="193"/>
+      <c r="B31" s="198"/>
+      <c r="C31" s="201" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="95" t="s">
@@ -4481,13 +4822,12 @@
       <c r="J31" s="111"/>
       <c r="K31" s="114"/>
       <c r="L31" s="115">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M31" s="116"/>
       <c r="N31" s="111">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O31" s="117">
         <f>38.88-(38.88*10/100)</f>
@@ -4499,9 +4839,9 @@
       <c r="S31" s="5"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="203"/>
-      <c r="B32" s="195"/>
-      <c r="C32" s="207"/>
+      <c r="A32" s="193"/>
+      <c r="B32" s="198"/>
+      <c r="C32" s="201"/>
       <c r="D32" s="103" t="s">
         <v>26</v>
       </c>
@@ -4537,9 +4877,9 @@
       <c r="S32" s="5"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="203"/>
-      <c r="B33" s="195"/>
-      <c r="C33" s="207"/>
+      <c r="A33" s="193"/>
+      <c r="B33" s="198"/>
+      <c r="C33" s="201"/>
       <c r="D33" s="111" t="s">
         <v>27</v>
       </c>
@@ -4558,22 +4898,21 @@
       </c>
       <c r="K33" s="114"/>
       <c r="L33" s="115">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M33" s="116"/>
       <c r="N33" s="111">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O33" s="117"/>
       <c r="P33" s="118"/>
       <c r="S33" s="5"/>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="203"/>
-      <c r="B34" s="195"/>
-      <c r="C34" s="207"/>
+      <c r="A34" s="193"/>
+      <c r="B34" s="198"/>
+      <c r="C34" s="201"/>
       <c r="D34" s="103" t="s">
         <v>28</v>
       </c>
@@ -4605,9 +4944,9 @@
       <c r="S34" s="5"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="203"/>
-      <c r="B35" s="195"/>
-      <c r="C35" s="207"/>
+      <c r="A35" s="193"/>
+      <c r="B35" s="198"/>
+      <c r="C35" s="201"/>
       <c r="D35" s="135" t="s">
         <v>29</v>
       </c>
@@ -4634,16 +4973,20 @@
       </c>
       <c r="O35" s="141"/>
       <c r="P35" s="142"/>
+      <c r="Q35" s="3">
+        <f>SUM(N31:N35)</f>
+        <v>10</v>
+      </c>
       <c r="S35" s="5"/>
     </row>
     <row r="36" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="190" t="s">
+      <c r="A36" s="203" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="191" t="s">
+      <c r="B36" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="192" t="s">
+      <c r="C36" s="205" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="143" t="s">
@@ -4680,9 +5023,9 @@
       <c r="S36" s="5"/>
     </row>
     <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="190"/>
-      <c r="B37" s="191"/>
-      <c r="C37" s="192"/>
+      <c r="A37" s="203"/>
+      <c r="B37" s="204"/>
+      <c r="C37" s="205"/>
       <c r="D37" s="27" t="s">
         <v>27</v>
       </c>
@@ -4691,9 +5034,11 @@
       </c>
       <c r="F37" s="20">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G37" s="27"/>
+        <v>3</v>
+      </c>
+      <c r="G37" s="27">
+        <v>1</v>
+      </c>
       <c r="H37" s="27">
         <v>1</v>
       </c>
@@ -4712,9 +5057,9 @@
       <c r="S37" s="5"/>
     </row>
     <row r="38" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="190"/>
-      <c r="B38" s="191"/>
-      <c r="C38" s="192"/>
+      <c r="A38" s="203"/>
+      <c r="B38" s="204"/>
+      <c r="C38" s="205"/>
       <c r="D38" s="18" t="s">
         <v>28</v>
       </c>
@@ -4740,9 +5085,9 @@
       <c r="S38" s="5"/>
     </row>
     <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="190"/>
-      <c r="B39" s="191"/>
-      <c r="C39" s="192"/>
+      <c r="A39" s="203"/>
+      <c r="B39" s="204"/>
+      <c r="C39" s="205"/>
       <c r="D39" s="35" t="s">
         <v>29</v>
       </c>
@@ -4768,9 +5113,9 @@
       <c r="S39" s="5"/>
     </row>
     <row r="40" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="190"/>
-      <c r="B40" s="191"/>
-      <c r="C40" s="193" t="s">
+      <c r="A40" s="203"/>
+      <c r="B40" s="204"/>
+      <c r="C40" s="196" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="43" t="s">
@@ -4781,12 +5126,12 @@
       </c>
       <c r="F40" s="45">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J40" s="43"/>
       <c r="K40" s="46"/>
@@ -4801,9 +5146,9 @@
       <c r="S40" s="5"/>
     </row>
     <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="190"/>
-      <c r="B41" s="191"/>
-      <c r="C41" s="193"/>
+      <c r="A41" s="203"/>
+      <c r="B41" s="204"/>
+      <c r="C41" s="196"/>
       <c r="D41" s="51" t="s">
         <v>27</v>
       </c>
@@ -4812,11 +5157,11 @@
       </c>
       <c r="F41" s="53">
         <f t="shared" ref="F41:F60" si="3">E41-G41-H41-I41-J41-K41</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="51"/>
       <c r="H41" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41" s="51"/>
       <c r="J41" s="51">
@@ -4831,9 +5176,9 @@
       <c r="S41" s="5"/>
     </row>
     <row r="42" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="190"/>
-      <c r="B42" s="191"/>
-      <c r="C42" s="193"/>
+      <c r="A42" s="203"/>
+      <c r="B42" s="204"/>
+      <c r="C42" s="196"/>
       <c r="D42" s="59" t="s">
         <v>28</v>
       </c>
@@ -4857,9 +5202,9 @@
       <c r="S42" s="5"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="190"/>
-      <c r="B43" s="191"/>
-      <c r="C43" s="193"/>
+      <c r="A43" s="203"/>
+      <c r="B43" s="204"/>
+      <c r="C43" s="196"/>
       <c r="D43" s="67" t="s">
         <v>29</v>
       </c>
@@ -4885,9 +5230,9 @@
       <c r="S43" s="5"/>
     </row>
     <row r="44" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="190"/>
-      <c r="B44" s="191"/>
-      <c r="C44" s="194" t="s">
+      <c r="A44" s="203"/>
+      <c r="B44" s="204"/>
+      <c r="C44" s="197" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="18" t="s">
@@ -4920,9 +5265,9 @@
       <c r="S44" s="5"/>
     </row>
     <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="190"/>
-      <c r="B45" s="191"/>
-      <c r="C45" s="194"/>
+      <c r="A45" s="203"/>
+      <c r="B45" s="204"/>
+      <c r="C45" s="197"/>
       <c r="D45" s="80" t="s">
         <v>26</v>
       </c>
@@ -4931,10 +5276,10 @@
       </c>
       <c r="F45" s="29">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G45" s="80">
         <v>2</v>
-      </c>
-      <c r="G45" s="80">
-        <v>1</v>
       </c>
       <c r="H45" s="80">
         <v>1</v>
@@ -4954,9 +5299,9 @@
       <c r="S45" s="5"/>
     </row>
     <row r="46" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="190"/>
-      <c r="B46" s="191"/>
-      <c r="C46" s="194"/>
+      <c r="A46" s="203"/>
+      <c r="B46" s="204"/>
+      <c r="C46" s="197"/>
       <c r="D46" s="83" t="s">
         <v>27</v>
       </c>
@@ -4986,9 +5331,9 @@
       <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="190"/>
-      <c r="B47" s="191"/>
-      <c r="C47" s="194"/>
+      <c r="A47" s="203"/>
+      <c r="B47" s="204"/>
+      <c r="C47" s="197"/>
       <c r="D47" s="80" t="s">
         <v>28</v>
       </c>
@@ -5016,9 +5361,9 @@
       <c r="S47" s="5"/>
     </row>
     <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="190"/>
-      <c r="B48" s="191"/>
-      <c r="C48" s="194"/>
+      <c r="A48" s="203"/>
+      <c r="B48" s="204"/>
+      <c r="C48" s="197"/>
       <c r="D48" s="83" t="s">
         <v>29</v>
       </c>
@@ -5048,11 +5393,11 @@
       <c r="S48" s="5"/>
     </row>
     <row r="49" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="190"/>
-      <c r="B49" s="195" t="s">
+      <c r="A49" s="203"/>
+      <c r="B49" s="198" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="196" t="s">
+      <c r="C49" s="199" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="95" t="s">
@@ -5085,9 +5430,9 @@
       <c r="S49" s="5"/>
     </row>
     <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="190"/>
-      <c r="B50" s="195"/>
-      <c r="C50" s="196"/>
+      <c r="A50" s="203"/>
+      <c r="B50" s="198"/>
+      <c r="C50" s="199"/>
       <c r="D50" s="103" t="s">
         <v>34</v>
       </c>
@@ -5115,9 +5460,9 @@
       <c r="S50" s="5"/>
     </row>
     <row r="51" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="190"/>
-      <c r="B51" s="195"/>
-      <c r="C51" s="196"/>
+      <c r="A51" s="203"/>
+      <c r="B51" s="198"/>
+      <c r="C51" s="199"/>
       <c r="D51" s="111" t="s">
         <v>26</v>
       </c>
@@ -5141,9 +5486,9 @@
       <c r="S51" s="5"/>
     </row>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="190"/>
-      <c r="B52" s="195"/>
-      <c r="C52" s="196"/>
+      <c r="A52" s="203"/>
+      <c r="B52" s="198"/>
+      <c r="C52" s="199"/>
       <c r="D52" s="103" t="s">
         <v>27</v>
       </c>
@@ -5167,9 +5512,9 @@
       <c r="S52" s="5"/>
     </row>
     <row r="53" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="190"/>
-      <c r="B53" s="195"/>
-      <c r="C53" s="196"/>
+      <c r="A53" s="203"/>
+      <c r="B53" s="198"/>
+      <c r="C53" s="199"/>
       <c r="D53" s="119" t="s">
         <v>28</v>
       </c>
@@ -5193,9 +5538,9 @@
       <c r="S53" s="5"/>
     </row>
     <row r="54" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="190"/>
-      <c r="B54" s="195"/>
-      <c r="C54" s="197" t="s">
+      <c r="A54" s="203"/>
+      <c r="B54" s="198"/>
+      <c r="C54" s="206" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="95" t="s">
@@ -5226,9 +5571,9 @@
       <c r="S54" s="5"/>
     </row>
     <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="190"/>
-      <c r="B55" s="195"/>
-      <c r="C55" s="197"/>
+      <c r="A55" s="203"/>
+      <c r="B55" s="198"/>
+      <c r="C55" s="206"/>
       <c r="D55" s="103" t="s">
         <v>34</v>
       </c>
@@ -5254,9 +5599,9 @@
       <c r="S55" s="5"/>
     </row>
     <row r="56" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="190"/>
-      <c r="B56" s="195"/>
-      <c r="C56" s="197"/>
+      <c r="A56" s="203"/>
+      <c r="B56" s="198"/>
+      <c r="C56" s="206"/>
       <c r="D56" s="111" t="s">
         <v>26</v>
       </c>
@@ -5280,9 +5625,9 @@
       <c r="S56" s="5"/>
     </row>
     <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="190"/>
-      <c r="B57" s="195"/>
-      <c r="C57" s="197"/>
+      <c r="A57" s="203"/>
+      <c r="B57" s="198"/>
+      <c r="C57" s="206"/>
       <c r="D57" s="103" t="s">
         <v>27</v>
       </c>
@@ -5306,9 +5651,9 @@
       <c r="S57" s="5"/>
     </row>
     <row r="58" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="190"/>
-      <c r="B58" s="195"/>
-      <c r="C58" s="198"/>
+      <c r="A58" s="203"/>
+      <c r="B58" s="198"/>
+      <c r="C58" s="207"/>
       <c r="D58" s="135" t="s">
         <v>28</v>
       </c>
@@ -5333,7 +5678,7 @@
     </row>
     <row r="59" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="C59" s="189" t="s">
+      <c r="C59" s="202" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="168" t="s">
@@ -5368,7 +5713,7 @@
     </row>
     <row r="60" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
-      <c r="C60" s="189"/>
+      <c r="C60" s="202"/>
       <c r="D60" s="176" t="s">
         <v>38</v>
       </c>
@@ -5439,6 +5784,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A36:A58"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C58"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:P7"/>
@@ -5451,19 +5805,13 @@
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C35"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A36:A58"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="92" firstPageNumber="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="84" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F9:L9 F12:L12 F10:I10 N10:P10 K10:L10 F16:P17 F14:L14 N14:P14 F11:L11 N11:P11 F29:P30 F27:L27 N27:P27 F21:P26 F19:L19 N19:P19 F15:L15 N15:P15 F18:L18 N18:P18 F13:L13 N13:P13 N9:P9 N12:P12 F20:L20 N20:P20 F28:L28 N28:P28 F32:P32 F31:K31 M31:P31 F34:P35 F33:K33 N33:P33" unlockedFormula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aktualisierung Inventar: HaPe 2x Guiding Team Kollektion (1x gekauft)
</commit_message>
<xml_diff>
--- a/2017 Reisen/inventar.xlsx
+++ b/2017 Reisen/inventar.xlsx
@@ -472,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I38" authorId="0" shapeId="0">
+    <comment ref="G38" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -492,6 +492,30 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+2x HaPe (50€)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 Adrian
 Manuel</t>
         </r>
@@ -608,6 +632,30 @@
           </rPr>
           <t xml:space="preserve">
 für simon, muss noch übergeben werden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+2x HaPe (50€)</t>
         </r>
       </text>
     </comment>
@@ -3075,6 +3123,46 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -3103,51 +3191,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="86" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3742,8 +3790,8 @@
   <dimension ref="A1:IX69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
+      <pane ySplit="8" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3819,7 +3867,7 @@
       </c>
       <c r="B4" s="8">
         <f ca="1">TODAY()</f>
-        <v>42843</v>
+        <v>42852</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -3879,30 +3927,30 @@
       <c r="S6" s="5"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="189" t="s">
+      <c r="A7" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="190"/>
-      <c r="C7" s="190"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="190"/>
-      <c r="F7" s="191" t="s">
+      <c r="B7" s="200"/>
+      <c r="C7" s="200"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="191"/>
-      <c r="H7" s="191"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="191"/>
-      <c r="K7" s="191"/>
-      <c r="L7" s="191" t="s">
+      <c r="G7" s="201"/>
+      <c r="H7" s="201"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="201"/>
+      <c r="L7" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="191"/>
-      <c r="N7" s="191" t="s">
+      <c r="M7" s="201"/>
+      <c r="N7" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="191"/>
-      <c r="P7" s="192"/>
+      <c r="O7" s="201"/>
+      <c r="P7" s="202"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
@@ -3959,13 +4007,13 @@
       <c r="S8" s="5"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="203" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="194" t="s">
+      <c r="B9" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="195" t="s">
+      <c r="C9" s="205" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -4009,9 +4057,9 @@
       <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="193"/>
-      <c r="B10" s="194"/>
-      <c r="C10" s="195"/>
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
+      <c r="C10" s="205"/>
       <c r="D10" s="27" t="s">
         <v>27</v>
       </c>
@@ -4047,9 +4095,9 @@
       <c r="S10" s="5"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="193"/>
-      <c r="B11" s="194"/>
-      <c r="C11" s="195"/>
+      <c r="A11" s="203"/>
+      <c r="B11" s="204"/>
+      <c r="C11" s="205"/>
       <c r="D11" s="18" t="s">
         <v>28</v>
       </c>
@@ -4084,9 +4132,9 @@
       <c r="S11" s="5"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="193"/>
-      <c r="B12" s="194"/>
-      <c r="C12" s="195"/>
+      <c r="A12" s="203"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="205"/>
       <c r="D12" s="35" t="s">
         <v>29</v>
       </c>
@@ -4125,9 +4173,9 @@
       <c r="S12" s="5"/>
     </row>
     <row r="13" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="193"/>
-      <c r="B13" s="194"/>
-      <c r="C13" s="196" t="s">
+      <c r="A13" s="203"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="193" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="43" t="s">
@@ -4169,9 +4217,9 @@
       <c r="S13" s="5"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="193"/>
-      <c r="B14" s="194"/>
-      <c r="C14" s="196"/>
+      <c r="A14" s="203"/>
+      <c r="B14" s="204"/>
+      <c r="C14" s="193"/>
       <c r="D14" s="51" t="s">
         <v>27</v>
       </c>
@@ -4208,9 +4256,9 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="193"/>
-      <c r="B15" s="194"/>
-      <c r="C15" s="196"/>
+      <c r="A15" s="203"/>
+      <c r="B15" s="204"/>
+      <c r="C15" s="193"/>
       <c r="D15" s="59" t="s">
         <v>28</v>
       </c>
@@ -4240,9 +4288,9 @@
       <c r="S15" s="5"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="193"/>
-      <c r="B16" s="194"/>
-      <c r="C16" s="196"/>
+      <c r="A16" s="203"/>
+      <c r="B16" s="204"/>
+      <c r="C16" s="193"/>
       <c r="D16" s="67" t="s">
         <v>29</v>
       </c>
@@ -4278,9 +4326,9 @@
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
-      <c r="B17" s="194"/>
-      <c r="C17" s="197" t="s">
+      <c r="A17" s="203"/>
+      <c r="B17" s="204"/>
+      <c r="C17" s="194" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -4319,9 +4367,9 @@
       <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="193"/>
-      <c r="B18" s="194"/>
-      <c r="C18" s="197"/>
+      <c r="A18" s="203"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="194"/>
       <c r="D18" s="80" t="s">
         <v>27</v>
       </c>
@@ -4355,9 +4403,9 @@
       <c r="S18" s="5"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="193"/>
-      <c r="B19" s="194"/>
-      <c r="C19" s="197"/>
+      <c r="A19" s="203"/>
+      <c r="B19" s="204"/>
+      <c r="C19" s="194"/>
       <c r="D19" s="83" t="s">
         <v>28</v>
       </c>
@@ -4391,9 +4439,9 @@
       <c r="S19" s="5"/>
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="193"/>
-      <c r="B20" s="194"/>
-      <c r="C20" s="197"/>
+      <c r="A20" s="203"/>
+      <c r="B20" s="204"/>
+      <c r="C20" s="194"/>
       <c r="D20" s="89" t="s">
         <v>29</v>
       </c>
@@ -4433,11 +4481,11 @@
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="193"/>
-      <c r="B21" s="198" t="s">
+      <c r="A21" s="203"/>
+      <c r="B21" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="199" t="s">
+      <c r="C21" s="196" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="95" t="s">
@@ -4476,9 +4524,9 @@
       <c r="S21" s="5"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="193"/>
-      <c r="B22" s="198"/>
-      <c r="C22" s="199"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="195"/>
+      <c r="C22" s="196"/>
       <c r="D22" s="103" t="s">
         <v>34</v>
       </c>
@@ -4510,9 +4558,9 @@
       <c r="S22" s="5"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="193"/>
-      <c r="B23" s="198"/>
-      <c r="C23" s="199"/>
+      <c r="A23" s="203"/>
+      <c r="B23" s="195"/>
+      <c r="C23" s="196"/>
       <c r="D23" s="111" t="s">
         <v>26</v>
       </c>
@@ -4548,9 +4596,9 @@
       <c r="S23" s="5"/>
     </row>
     <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="193"/>
-      <c r="B24" s="198"/>
-      <c r="C24" s="199"/>
+      <c r="A24" s="203"/>
+      <c r="B24" s="195"/>
+      <c r="C24" s="196"/>
       <c r="D24" s="103" t="s">
         <v>27</v>
       </c>
@@ -4582,9 +4630,9 @@
       <c r="S24" s="5"/>
     </row>
     <row r="25" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="193"/>
-      <c r="B25" s="198"/>
-      <c r="C25" s="199"/>
+      <c r="A25" s="203"/>
+      <c r="B25" s="195"/>
+      <c r="C25" s="196"/>
       <c r="D25" s="119" t="s">
         <v>28</v>
       </c>
@@ -4620,9 +4668,9 @@
       <c r="S25" s="5"/>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="193"/>
-      <c r="B26" s="198"/>
-      <c r="C26" s="200" t="s">
+      <c r="A26" s="203"/>
+      <c r="B26" s="195"/>
+      <c r="C26" s="206" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="95" t="s">
@@ -4661,9 +4709,9 @@
       <c r="S26" s="5"/>
     </row>
     <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="193"/>
-      <c r="B27" s="198"/>
-      <c r="C27" s="200"/>
+      <c r="A27" s="203"/>
+      <c r="B27" s="195"/>
+      <c r="C27" s="206"/>
       <c r="D27" s="103" t="s">
         <v>34</v>
       </c>
@@ -4695,9 +4743,9 @@
       <c r="S27" s="5"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="193"/>
-      <c r="B28" s="198"/>
-      <c r="C28" s="200"/>
+      <c r="A28" s="203"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="206"/>
       <c r="D28" s="111" t="s">
         <v>26</v>
       </c>
@@ -4731,9 +4779,9 @@
       <c r="S28" s="5"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="193"/>
-      <c r="B29" s="198"/>
-      <c r="C29" s="200"/>
+      <c r="A29" s="203"/>
+      <c r="B29" s="195"/>
+      <c r="C29" s="206"/>
       <c r="D29" s="103" t="s">
         <v>27</v>
       </c>
@@ -4763,9 +4811,9 @@
       <c r="S29" s="5"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="193"/>
-      <c r="B30" s="198"/>
-      <c r="C30" s="200"/>
+      <c r="A30" s="203"/>
+      <c r="B30" s="195"/>
+      <c r="C30" s="206"/>
       <c r="D30" s="127" t="s">
         <v>28</v>
       </c>
@@ -4799,9 +4847,9 @@
       <c r="S30" s="5"/>
     </row>
     <row r="31" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="193"/>
-      <c r="B31" s="198"/>
-      <c r="C31" s="201" t="s">
+      <c r="A31" s="203"/>
+      <c r="B31" s="195"/>
+      <c r="C31" s="207" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="95" t="s">
@@ -4839,9 +4887,9 @@
       <c r="S31" s="5"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="193"/>
-      <c r="B32" s="198"/>
-      <c r="C32" s="201"/>
+      <c r="A32" s="203"/>
+      <c r="B32" s="195"/>
+      <c r="C32" s="207"/>
       <c r="D32" s="103" t="s">
         <v>26</v>
       </c>
@@ -4877,9 +4925,9 @@
       <c r="S32" s="5"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="193"/>
-      <c r="B33" s="198"/>
-      <c r="C33" s="201"/>
+      <c r="A33" s="203"/>
+      <c r="B33" s="195"/>
+      <c r="C33" s="207"/>
       <c r="D33" s="111" t="s">
         <v>27</v>
       </c>
@@ -4898,21 +4946,21 @@
       </c>
       <c r="K33" s="114"/>
       <c r="L33" s="115">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M33" s="116"/>
       <c r="N33" s="111">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O33" s="117"/>
       <c r="P33" s="118"/>
       <c r="S33" s="5"/>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="193"/>
-      <c r="B34" s="198"/>
-      <c r="C34" s="201"/>
+      <c r="A34" s="203"/>
+      <c r="B34" s="195"/>
+      <c r="C34" s="207"/>
       <c r="D34" s="103" t="s">
         <v>28</v>
       </c>
@@ -4944,9 +4992,9 @@
       <c r="S34" s="5"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="193"/>
-      <c r="B35" s="198"/>
-      <c r="C35" s="201"/>
+      <c r="A35" s="203"/>
+      <c r="B35" s="195"/>
+      <c r="C35" s="207"/>
       <c r="D35" s="135" t="s">
         <v>29</v>
       </c>
@@ -4975,18 +5023,18 @@
       <c r="P35" s="142"/>
       <c r="Q35" s="3">
         <f>SUM(N31:N35)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S35" s="5"/>
     </row>
     <row r="36" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="203" t="s">
+      <c r="A36" s="190" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="204" t="s">
+      <c r="B36" s="191" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="205" t="s">
+      <c r="C36" s="192" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="143" t="s">
@@ -5023,9 +5071,9 @@
       <c r="S36" s="5"/>
     </row>
     <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="203"/>
-      <c r="B37" s="204"/>
-      <c r="C37" s="205"/>
+      <c r="A37" s="190"/>
+      <c r="B37" s="191"/>
+      <c r="C37" s="192"/>
       <c r="D37" s="27" t="s">
         <v>27</v>
       </c>
@@ -5057,9 +5105,9 @@
       <c r="S37" s="5"/>
     </row>
     <row r="38" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="203"/>
-      <c r="B38" s="204"/>
-      <c r="C38" s="205"/>
+      <c r="A38" s="190"/>
+      <c r="B38" s="191"/>
+      <c r="C38" s="192"/>
       <c r="D38" s="18" t="s">
         <v>28</v>
       </c>
@@ -5068,9 +5116,11 @@
       </c>
       <c r="F38" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G38" s="18"/>
+        <v>2</v>
+      </c>
+      <c r="G38" s="18">
+        <v>2</v>
+      </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18">
         <v>2</v>
@@ -5085,9 +5135,9 @@
       <c r="S38" s="5"/>
     </row>
     <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="203"/>
-      <c r="B39" s="204"/>
-      <c r="C39" s="205"/>
+      <c r="A39" s="190"/>
+      <c r="B39" s="191"/>
+      <c r="C39" s="192"/>
       <c r="D39" s="35" t="s">
         <v>29</v>
       </c>
@@ -5113,9 +5163,9 @@
       <c r="S39" s="5"/>
     </row>
     <row r="40" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="203"/>
-      <c r="B40" s="204"/>
-      <c r="C40" s="196" t="s">
+      <c r="A40" s="190"/>
+      <c r="B40" s="191"/>
+      <c r="C40" s="193" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="43" t="s">
@@ -5146,9 +5196,9 @@
       <c r="S40" s="5"/>
     </row>
     <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="203"/>
-      <c r="B41" s="204"/>
-      <c r="C41" s="196"/>
+      <c r="A41" s="190"/>
+      <c r="B41" s="191"/>
+      <c r="C41" s="193"/>
       <c r="D41" s="51" t="s">
         <v>27</v>
       </c>
@@ -5176,9 +5226,9 @@
       <c r="S41" s="5"/>
     </row>
     <row r="42" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="203"/>
-      <c r="B42" s="204"/>
-      <c r="C42" s="196"/>
+      <c r="A42" s="190"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="193"/>
       <c r="D42" s="59" t="s">
         <v>28</v>
       </c>
@@ -5202,9 +5252,9 @@
       <c r="S42" s="5"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="203"/>
-      <c r="B43" s="204"/>
-      <c r="C43" s="196"/>
+      <c r="A43" s="190"/>
+      <c r="B43" s="191"/>
+      <c r="C43" s="193"/>
       <c r="D43" s="67" t="s">
         <v>29</v>
       </c>
@@ -5230,9 +5280,9 @@
       <c r="S43" s="5"/>
     </row>
     <row r="44" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="203"/>
-      <c r="B44" s="204"/>
-      <c r="C44" s="197" t="s">
+      <c r="A44" s="190"/>
+      <c r="B44" s="191"/>
+      <c r="C44" s="194" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="18" t="s">
@@ -5265,9 +5315,9 @@
       <c r="S44" s="5"/>
     </row>
     <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="203"/>
-      <c r="B45" s="204"/>
-      <c r="C45" s="197"/>
+      <c r="A45" s="190"/>
+      <c r="B45" s="191"/>
+      <c r="C45" s="194"/>
       <c r="D45" s="80" t="s">
         <v>26</v>
       </c>
@@ -5299,9 +5349,9 @@
       <c r="S45" s="5"/>
     </row>
     <row r="46" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="203"/>
-      <c r="B46" s="204"/>
-      <c r="C46" s="197"/>
+      <c r="A46" s="190"/>
+      <c r="B46" s="191"/>
+      <c r="C46" s="194"/>
       <c r="D46" s="83" t="s">
         <v>27</v>
       </c>
@@ -5310,9 +5360,11 @@
       </c>
       <c r="F46" s="29">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="G46" s="83"/>
+        <v>5</v>
+      </c>
+      <c r="G46" s="83">
+        <v>2</v>
+      </c>
       <c r="H46" s="83">
         <v>3</v>
       </c>
@@ -5331,9 +5383,9 @@
       <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="203"/>
-      <c r="B47" s="204"/>
-      <c r="C47" s="197"/>
+      <c r="A47" s="190"/>
+      <c r="B47" s="191"/>
+      <c r="C47" s="194"/>
       <c r="D47" s="80" t="s">
         <v>28</v>
       </c>
@@ -5361,9 +5413,9 @@
       <c r="S47" s="5"/>
     </row>
     <row r="48" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="203"/>
-      <c r="B48" s="204"/>
-      <c r="C48" s="197"/>
+      <c r="A48" s="190"/>
+      <c r="B48" s="191"/>
+      <c r="C48" s="194"/>
       <c r="D48" s="83" t="s">
         <v>29</v>
       </c>
@@ -5393,11 +5445,11 @@
       <c r="S48" s="5"/>
     </row>
     <row r="49" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="203"/>
-      <c r="B49" s="198" t="s">
+      <c r="A49" s="190"/>
+      <c r="B49" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="199" t="s">
+      <c r="C49" s="196" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="95" t="s">
@@ -5430,9 +5482,9 @@
       <c r="S49" s="5"/>
     </row>
     <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="203"/>
-      <c r="B50" s="198"/>
-      <c r="C50" s="199"/>
+      <c r="A50" s="190"/>
+      <c r="B50" s="195"/>
+      <c r="C50" s="196"/>
       <c r="D50" s="103" t="s">
         <v>34</v>
       </c>
@@ -5460,9 +5512,9 @@
       <c r="S50" s="5"/>
     </row>
     <row r="51" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="203"/>
-      <c r="B51" s="198"/>
-      <c r="C51" s="199"/>
+      <c r="A51" s="190"/>
+      <c r="B51" s="195"/>
+      <c r="C51" s="196"/>
       <c r="D51" s="111" t="s">
         <v>26</v>
       </c>
@@ -5486,9 +5538,9 @@
       <c r="S51" s="5"/>
     </row>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="203"/>
-      <c r="B52" s="198"/>
-      <c r="C52" s="199"/>
+      <c r="A52" s="190"/>
+      <c r="B52" s="195"/>
+      <c r="C52" s="196"/>
       <c r="D52" s="103" t="s">
         <v>27</v>
       </c>
@@ -5512,9 +5564,9 @@
       <c r="S52" s="5"/>
     </row>
     <row r="53" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="203"/>
-      <c r="B53" s="198"/>
-      <c r="C53" s="199"/>
+      <c r="A53" s="190"/>
+      <c r="B53" s="195"/>
+      <c r="C53" s="196"/>
       <c r="D53" s="119" t="s">
         <v>28</v>
       </c>
@@ -5538,9 +5590,9 @@
       <c r="S53" s="5"/>
     </row>
     <row r="54" spans="1:19" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="203"/>
-      <c r="B54" s="198"/>
-      <c r="C54" s="206" t="s">
+      <c r="A54" s="190"/>
+      <c r="B54" s="195"/>
+      <c r="C54" s="197" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="95" t="s">
@@ -5571,9 +5623,9 @@
       <c r="S54" s="5"/>
     </row>
     <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="203"/>
-      <c r="B55" s="198"/>
-      <c r="C55" s="206"/>
+      <c r="A55" s="190"/>
+      <c r="B55" s="195"/>
+      <c r="C55" s="197"/>
       <c r="D55" s="103" t="s">
         <v>34</v>
       </c>
@@ -5599,9 +5651,9 @@
       <c r="S55" s="5"/>
     </row>
     <row r="56" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="203"/>
-      <c r="B56" s="198"/>
-      <c r="C56" s="206"/>
+      <c r="A56" s="190"/>
+      <c r="B56" s="195"/>
+      <c r="C56" s="197"/>
       <c r="D56" s="111" t="s">
         <v>26</v>
       </c>
@@ -5625,9 +5677,9 @@
       <c r="S56" s="5"/>
     </row>
     <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="203"/>
-      <c r="B57" s="198"/>
-      <c r="C57" s="206"/>
+      <c r="A57" s="190"/>
+      <c r="B57" s="195"/>
+      <c r="C57" s="197"/>
       <c r="D57" s="103" t="s">
         <v>27</v>
       </c>
@@ -5651,9 +5703,9 @@
       <c r="S57" s="5"/>
     </row>
     <row r="58" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="203"/>
-      <c r="B58" s="198"/>
-      <c r="C58" s="207"/>
+      <c r="A58" s="190"/>
+      <c r="B58" s="195"/>
+      <c r="C58" s="198"/>
       <c r="D58" s="135" t="s">
         <v>28</v>
       </c>
@@ -5678,7 +5730,7 @@
     </row>
     <row r="59" spans="1:19" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="C59" s="202" t="s">
+      <c r="C59" s="189" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="168" t="s">
@@ -5689,10 +5741,10 @@
       </c>
       <c r="F59" s="170">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G59" s="171">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H59" s="171"/>
       <c r="I59" s="171">
@@ -5713,7 +5765,7 @@
     </row>
     <row r="60" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
-      <c r="C60" s="202"/>
+      <c r="C60" s="189"/>
       <c r="D60" s="176" t="s">
         <v>38</v>
       </c>
@@ -5784,15 +5836,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A36:A58"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:P7"/>
@@ -5805,6 +5848,15 @@
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C35"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A36:A58"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>